<commit_message>
2022 Day 3 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D923CC-0064-460F-BE26-C8326D128777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D9E9A5-6DC7-4595-8B69-4C8C73E2A394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4992" yWindow="1542" windowWidth="17280" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2021" sheetId="7" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
+    <sheet name="2022" sheetId="9" r:id="rId1"/>
+    <sheet name="2021" sheetId="7" r:id="rId2"/>
     <sheet name="2020" sheetId="6" r:id="rId3"/>
     <sheet name="2019" sheetId="5" r:id="rId4"/>
     <sheet name="2018" sheetId="4" r:id="rId5"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="12">
   <si>
     <t>Day</t>
   </si>
@@ -81,19 +81,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Source Code Pro"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,16 +110,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -136,7 +127,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -427,11 +423,876 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A3E9AF-60E4-42C2-9582-F318C9A6FCBA}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>36348</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4848</v>
+      </c>
+      <c r="D2">
+        <f>IF(ISBLANK(B2),"",B2+C2)</f>
+        <v>41196</v>
+      </c>
+      <c r="E2" s="2">
+        <v>21900</v>
+      </c>
+      <c r="F2" s="2">
+        <v>21562</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
+        <v>0.5316050101951646</v>
+      </c>
+      <c r="H2" s="1">
+        <f>IF(ISBLANK(C2),"",F2/B2)</f>
+        <v>0.59321008033454381</v>
+      </c>
+      <c r="I2" s="1">
+        <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
+        <v>0.5316050101951646</v>
+      </c>
+      <c r="J2" s="1">
+        <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
+        <v>0.59321008033454381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>128659</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5355</v>
+      </c>
+      <c r="D3">
+        <f>IF(ISBLANK(B3),"",B3+C3)</f>
+        <v>134014</v>
+      </c>
+      <c r="E3" s="2">
+        <v>33440</v>
+      </c>
+      <c r="F3" s="2">
+        <v>31447</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24952616890772605</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
+        <v>0.24442129971474985</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
+        <v>0.81172929410622385</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
+        <v>0.86516452074391992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <f t="shared" ref="A4:A26" si="4">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" t="str">
+        <f>IF(ISBLANK(B4),"",B4+C4)</f>
+        <v/>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" t="str">
+        <f>IF(ISBLANK(B5),"",B5+C5)</f>
+        <v/>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J5" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" t="str">
+        <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
+        <v/>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J6" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J7" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J8" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J9" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J10" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" t="str">
+        <f>IF(ISBLANK(B12),"",B12+C12)</f>
+        <v/>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1" t="str">
+        <f>IF(D12="","",E12/D12)</f>
+        <v/>
+      </c>
+      <c r="H12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" t="str">
+        <f>IF(ISBLANK(B13),"",B13+C13)</f>
+        <v/>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1" t="str">
+        <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
+        <v/>
+      </c>
+      <c r="H13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J13" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" t="str">
+        <f>IF(ISBLANK(B14),"",B14+C14)</f>
+        <v/>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J14" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" t="str">
+        <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
+        <v/>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="J26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <conditionalFormatting sqref="G1:H26">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:J26">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:J26">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:F26">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -441,34 +1302,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -539,7 +1400,7 @@
         <v>0.17584751167002524</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:J26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
+        <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
         <v>0.13973190348525469</v>
       </c>
       <c r="J3" s="1">
@@ -1336,7 +2197,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -1390,146 +2251,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390756BD-4C07-44C6-B772-96FA9EC8100A}">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="4">
-        <v>17395</v>
-      </c>
-      <c r="B1">
-        <v>15534</v>
-      </c>
-      <c r="C1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4">
-        <v>48347</v>
-      </c>
-      <c r="B2">
-        <v>45135</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4">
-        <v>24434</v>
-      </c>
-      <c r="B3">
-        <v>20525</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="4">
-        <v>23902</v>
-      </c>
-      <c r="B4">
-        <v>22799</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="4">
-        <v>20541</v>
-      </c>
-      <c r="B5">
-        <v>19427</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="4">
-        <v>21281</v>
-      </c>
-      <c r="B6">
-        <v>16288</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="4">
-        <v>16986</v>
-      </c>
-      <c r="B7">
-        <v>17614</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="4">
-        <v>17127</v>
-      </c>
-      <c r="B8">
-        <v>17381</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="4">
-        <v>10658</v>
-      </c>
-      <c r="B9">
-        <v>11795</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="4">
-        <v>12736</v>
-      </c>
-      <c r="B10">
-        <v>11592</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="4">
-        <v>13506</v>
-      </c>
-      <c r="B11">
-        <v>19654</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C11">
-    <sortCondition descending="1" ref="C1:C11"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J26"/>
@@ -2531,7 +3252,7 @@
     <sortCondition descending="1" ref="L2"/>
   </sortState>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -3541,7 +4262,7 @@
     <sortCondition descending="1" ref="N2:N26"/>
   </sortState>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
Day 4 done.  Fixed stupid bug with display of times in batch mode.
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D9E9A5-6DC7-4595-8B69-4C8C73E2A394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38022562-8FC8-4B92-974C-2E3CEE6585CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3222" yWindow="1470" windowWidth="14202" windowHeight="9846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="9" r:id="rId1"/>
@@ -427,7 +427,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -469,14 +469,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>36348</v>
+        <v>177174</v>
       </c>
       <c r="C2" s="2">
-        <v>4848</v>
+        <v>6752</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>41196</v>
+        <v>183926</v>
       </c>
       <c r="E2" s="2">
         <v>21900</v>
@@ -486,19 +486,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>0.5316050101951646</v>
+        <v>0.11906962582777857</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>0.59321008033454381</v>
+        <v>0.12169957217198912</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>0.5316050101951646</v>
+        <v>0.11906962582777857</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>0.59321008033454381</v>
+        <v>0.12169957217198912</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -507,14 +507,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>128659</v>
+        <v>143328</v>
       </c>
       <c r="C3" s="2">
-        <v>5355</v>
+        <v>6395</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>134014</v>
+        <v>149723</v>
       </c>
       <c r="E3" s="2">
         <v>33440</v>
@@ -524,19 +524,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.24952616890772605</v>
+        <v>0.22334577853769963</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.24442129971474985</v>
+        <v>0.21940583835677607</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.81172929410622385</v>
+        <v>0.18181225057903722</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.86516452074391992</v>
+        <v>0.17749218282592255</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -544,29 +544,37 @@
         <f t="shared" ref="A4:A26" si="4">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" t="str">
+      <c r="B4" s="2">
+        <v>111150</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5645</v>
+      </c>
+      <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v/>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1" t="str">
+        <v>116795</v>
+      </c>
+      <c r="E4" s="2">
+        <v>35205</v>
+      </c>
+      <c r="F4" s="2">
+        <v>31491</v>
+      </c>
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J4" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.30142557472494541</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.28331983805668015</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.19140850124506595</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.1777405262623184</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -574,29 +582,37 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" t="str">
+      <c r="B5" s="2">
+        <v>92883</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1862</v>
+      </c>
+      <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v/>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1" t="str">
+        <v>94745</v>
+      </c>
+      <c r="E5" s="2">
+        <v>20073</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20122</v>
+      </c>
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H5" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J5" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.21186342287191937</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.21663813614977984</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10913628307036526</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11357196879903372</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1232,7 +1248,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -2197,7 +2213,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -3252,7 +3268,7 @@
     <sortCondition descending="1" ref="L2"/>
   </sortState>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -4262,7 +4278,7 @@
     <sortCondition descending="1" ref="N2:N26"/>
   </sortState>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
Fixed some historic ones that weren't working
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B2A51F-25BB-4E0D-9EC2-0565CDF8D465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E554CFC9-1508-4055-8208-D61C79DA7A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="9120" windowWidth="19770" windowHeight="13035" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23985" yWindow="7635" windowWidth="19770" windowHeight="13035" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -216,20 +216,40 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -247,11 +267,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF49C050"/>
+        <color rgb="FF24B850"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF49C050"/>
+          <bgColor rgb="FF24B850"/>
         </patternFill>
       </fill>
     </dxf>
@@ -294,221 +314,6 @@
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF24B850"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF24B850"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF49C050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1605,7 +1410,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="28" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -2727,7 +2532,7 @@
   <dimension ref="A1:CX20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="AP11" sqref="AP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2738,358 +2543,358 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="B1" s="5">
+      <c r="B1" s="11">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11">
         <v>2</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11">
         <v>3</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11">
         <v>4</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5">
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11">
         <v>5</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5">
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11">
         <v>6</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5">
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11">
         <v>7</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5">
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11">
         <v>8</v>
       </c>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5">
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11">
         <v>9</v>
       </c>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5">
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11">
         <v>10</v>
       </c>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5">
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11">
         <v>11</v>
       </c>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="5"/>
-      <c r="AT1" s="5">
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11">
         <v>12</v>
       </c>
-      <c r="AU1" s="5"/>
-      <c r="AV1" s="5"/>
-      <c r="AW1" s="5"/>
-      <c r="AX1" s="5">
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11">
         <v>13</v>
       </c>
-      <c r="AY1" s="5"/>
-      <c r="AZ1" s="5"/>
-      <c r="BA1" s="5"/>
-      <c r="BB1" s="5">
-        <v>14</v>
-      </c>
-      <c r="BC1" s="5"/>
-      <c r="BD1" s="5"/>
-      <c r="BE1" s="5"/>
-      <c r="BF1" s="5">
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11">
+        <v>14</v>
+      </c>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11">
         <v>15</v>
       </c>
-      <c r="BG1" s="5"/>
-      <c r="BH1" s="5"/>
-      <c r="BI1" s="5"/>
-      <c r="BJ1" s="5">
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11">
         <v>16</v>
       </c>
-      <c r="BK1" s="5"/>
-      <c r="BL1" s="5"/>
-      <c r="BM1" s="5"/>
-      <c r="BN1" s="5">
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11">
         <v>17</v>
       </c>
-      <c r="BO1" s="5"/>
-      <c r="BP1" s="5"/>
-      <c r="BQ1" s="5"/>
-      <c r="BR1" s="5">
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11">
         <v>18</v>
       </c>
-      <c r="BS1" s="5"/>
-      <c r="BT1" s="5"/>
-      <c r="BU1" s="5"/>
-      <c r="BV1" s="5">
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11">
         <v>19</v>
       </c>
-      <c r="BW1" s="5"/>
-      <c r="BX1" s="5"/>
-      <c r="BY1" s="5"/>
-      <c r="BZ1" s="5">
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11">
         <v>20</v>
       </c>
-      <c r="CA1" s="5"/>
-      <c r="CB1" s="5"/>
-      <c r="CC1" s="5"/>
-      <c r="CD1" s="5">
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11">
         <v>21</v>
       </c>
-      <c r="CE1" s="5"/>
-      <c r="CF1" s="5"/>
-      <c r="CG1" s="5"/>
-      <c r="CH1" s="5">
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11">
         <v>22</v>
       </c>
-      <c r="CI1" s="5"/>
-      <c r="CJ1" s="5"/>
-      <c r="CK1" s="5"/>
-      <c r="CL1" s="5">
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11">
         <v>23</v>
       </c>
-      <c r="CM1" s="5"/>
-      <c r="CN1" s="5"/>
-      <c r="CO1" s="5"/>
-      <c r="CP1" s="5">
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11">
         <v>24</v>
       </c>
-      <c r="CQ1" s="5"/>
-      <c r="CR1" s="5"/>
-      <c r="CS1" s="5"/>
-      <c r="CT1" s="5">
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11">
         <v>25</v>
       </c>
-      <c r="CU1" s="5"/>
-      <c r="CV1" s="5"/>
-      <c r="CW1" s="5"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
     </row>
     <row r="2" spans="1:102" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="11"/>
+      <c r="L2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="11"/>
+      <c r="N2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5" t="s">
+      <c r="O2" s="11"/>
+      <c r="P2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5" t="s">
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5" t="s">
+      <c r="S2" s="11"/>
+      <c r="T2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5" t="s">
+      <c r="U2" s="11"/>
+      <c r="V2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5" t="s">
+      <c r="W2" s="11"/>
+      <c r="X2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5" t="s">
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5" t="s">
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5" t="s">
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5" t="s">
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5" t="s">
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5" t="s">
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5" t="s">
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5" t="s">
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="5" t="s">
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5" t="s">
+      <c r="AQ2" s="11"/>
+      <c r="AR2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AS2" s="5"/>
-      <c r="AT2" s="5" t="s">
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AU2" s="5"/>
-      <c r="AV2" s="5" t="s">
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AW2" s="5"/>
-      <c r="AX2" s="5" t="s">
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AY2" s="5"/>
-      <c r="AZ2" s="5" t="s">
+      <c r="AY2" s="11"/>
+      <c r="AZ2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BA2" s="5"/>
-      <c r="BB2" s="5" t="s">
+      <c r="BA2" s="11"/>
+      <c r="BB2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5" t="s">
+      <c r="BC2" s="11"/>
+      <c r="BD2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BE2" s="5"/>
-      <c r="BF2" s="5" t="s">
+      <c r="BE2" s="11"/>
+      <c r="BF2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BG2" s="5"/>
-      <c r="BH2" s="5" t="s">
+      <c r="BG2" s="11"/>
+      <c r="BH2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BI2" s="5"/>
-      <c r="BJ2" s="5" t="s">
+      <c r="BI2" s="11"/>
+      <c r="BJ2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BK2" s="5"/>
-      <c r="BL2" s="5" t="s">
+      <c r="BK2" s="11"/>
+      <c r="BL2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BM2" s="5"/>
-      <c r="BN2" s="5" t="s">
+      <c r="BM2" s="11"/>
+      <c r="BN2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BO2" s="5"/>
-      <c r="BP2" s="5" t="s">
+      <c r="BO2" s="11"/>
+      <c r="BP2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BQ2" s="5"/>
-      <c r="BR2" s="5" t="s">
+      <c r="BQ2" s="11"/>
+      <c r="BR2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BS2" s="5"/>
-      <c r="BT2" s="5" t="s">
+      <c r="BS2" s="11"/>
+      <c r="BT2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BU2" s="5"/>
-      <c r="BV2" s="5" t="s">
+      <c r="BU2" s="11"/>
+      <c r="BV2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BW2" s="5"/>
-      <c r="BX2" s="5" t="s">
+      <c r="BW2" s="11"/>
+      <c r="BX2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BY2" s="5"/>
-      <c r="BZ2" s="5" t="s">
+      <c r="BY2" s="11"/>
+      <c r="BZ2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CA2" s="5"/>
-      <c r="CB2" s="5" t="s">
+      <c r="CA2" s="11"/>
+      <c r="CB2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CC2" s="5"/>
-      <c r="CD2" s="5" t="s">
+      <c r="CC2" s="11"/>
+      <c r="CD2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CE2" s="5"/>
-      <c r="CF2" s="5" t="s">
+      <c r="CE2" s="11"/>
+      <c r="CF2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CG2" s="5"/>
-      <c r="CH2" s="5" t="s">
+      <c r="CG2" s="11"/>
+      <c r="CH2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CI2" s="5"/>
-      <c r="CJ2" s="5" t="s">
+      <c r="CI2" s="11"/>
+      <c r="CJ2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CK2" s="5"/>
-      <c r="CL2" s="5" t="s">
+      <c r="CK2" s="11"/>
+      <c r="CL2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CM2" s="5"/>
-      <c r="CN2" s="5" t="s">
+      <c r="CM2" s="11"/>
+      <c r="CN2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CO2" s="5"/>
-      <c r="CP2" s="5" t="s">
+      <c r="CO2" s="11"/>
+      <c r="CP2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CQ2" s="5"/>
-      <c r="CR2" s="5" t="s">
+      <c r="CQ2" s="11"/>
+      <c r="CR2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CS2" s="5"/>
-      <c r="CT2" s="5" t="s">
+      <c r="CS2" s="11"/>
+      <c r="CT2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CU2" s="5"/>
-      <c r="CV2" s="5" t="s">
+      <c r="CU2" s="11"/>
+      <c r="CV2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CW2" s="5"/>
+      <c r="CW2" s="11"/>
     </row>
     <row r="3" spans="1:102" x14ac:dyDescent="0.25">
       <c r="B3">
@@ -4989,7 +4794,7 @@
         <v>14</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T9" s="2" t="s">
         <v>14</v>
@@ -5094,16 +4899,16 @@
         <v>14</v>
       </c>
       <c r="BB9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="BC9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="BD9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="BE9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="BF9" s="2" t="s">
         <v>14</v>
@@ -5393,13 +5198,13 @@
         <v>14</v>
       </c>
       <c r="AY10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AZ10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="BA10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="BB10" s="2" t="s">
         <v>14</v>
@@ -5441,13 +5246,13 @@
         <v>14</v>
       </c>
       <c r="BO10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="BP10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="BQ10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="BR10" s="2" t="s">
         <v>14</v>
@@ -5489,13 +5294,13 @@
         <v>14</v>
       </c>
       <c r="CE10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="CF10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="CG10" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="CH10" s="2" t="s">
         <v>19</v>
@@ -5665,13 +5470,13 @@
         <v>14</v>
       </c>
       <c r="AM11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AN11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AO11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AP11" s="2" t="s">
         <v>14</v>
@@ -6169,7 +5974,7 @@
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -6177,7 +5982,7 @@
       <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6185,7 +5990,7 @@
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6193,7 +5998,7 @@
       <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -6201,7 +6006,7 @@
       <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -6209,7 +6014,7 @@
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -6223,47 +6028,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6280,45 +6062,68 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
-    <cfRule type="cellIs" dxfId="13" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>"s"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="equal">
       <formula>"f"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"t"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7212,7 +7017,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="32" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -8177,7 +7982,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="31" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -9232,7 +9037,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -10242,7 +10047,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
2023 day 5 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32EA1B2-C131-4D6B-A741-89C6FDF59A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8923453-2E29-4B47-A0CF-C6F6AB50ACB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="252" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2538" yWindow="570" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId2"/>
-    <sheet name="Overall" sheetId="11" r:id="rId3"/>
-    <sheet name="2022" sheetId="9" r:id="rId4"/>
-    <sheet name="2021" sheetId="7" r:id="rId5"/>
-    <sheet name="2020" sheetId="6" r:id="rId6"/>
-    <sheet name="2019" sheetId="5" r:id="rId7"/>
-    <sheet name="2018" sheetId="4" r:id="rId8"/>
-    <sheet name="2017" sheetId="3" r:id="rId9"/>
-    <sheet name="2016" sheetId="1" r:id="rId10"/>
-    <sheet name="2015" sheetId="2" r:id="rId11"/>
+    <sheet name="Overall" sheetId="11" r:id="rId2"/>
+    <sheet name="2022" sheetId="9" r:id="rId3"/>
+    <sheet name="2021" sheetId="7" r:id="rId4"/>
+    <sheet name="2020" sheetId="6" r:id="rId5"/>
+    <sheet name="2019" sheetId="5" r:id="rId6"/>
+    <sheet name="2018" sheetId="4" r:id="rId7"/>
+    <sheet name="2017" sheetId="3" r:id="rId8"/>
+    <sheet name="2016" sheetId="1" r:id="rId9"/>
+    <sheet name="2015" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="28">
   <si>
     <t>Day</t>
   </si>
@@ -120,87 +119,12 @@
   <si>
     <t>not done yet</t>
   </si>
-  <si>
-    <t xml:space="preserve">25       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">24       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">23       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">22       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">21       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">20       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">19       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">18       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">17       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">16       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">15       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">14       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">13       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">12       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">11       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 6       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3       0      0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2   41895   3730  ************</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1  113625  42560  *****************************************</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,20 +134,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color rgb="FF666666"/>
-      <name val="Source Code Pro"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -282,11 +192,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -304,18 +213,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -694,7 +596,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -740,14 +642,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>113625</v>
+        <v>169144</v>
       </c>
       <c r="C2" s="2">
-        <v>42560</v>
+        <v>54862</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>156185</v>
+        <v>224006</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -757,19 +659,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>0.16322310080993693</v>
+        <v>0.11380498736640983</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>0.18092849284928492</v>
+        <v>0.1215414085039966</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>0.16322310080993693</v>
+        <v>0.11380498736640983</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>0.18092849284928492</v>
+        <v>0.1215414085039966</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -778,14 +680,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>41895</v>
+        <v>136839</v>
       </c>
       <c r="C3" s="2">
-        <v>3730</v>
+        <v>6109</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>45625</v>
+        <v>142948</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -795,19 +697,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.64563287671232872</v>
+        <v>0.20606794078965779</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.70667144050602693</v>
+        <v>0.21635644808862969</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.18860325895572558</v>
+        <v>0.1315009419390552</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.26055885588558858</v>
+        <v>0.17503429030884926</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -815,29 +717,37 @@
         <f t="shared" ref="A4:A26" si="4">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" t="str">
+      <c r="B4" s="2">
+        <v>86401</v>
+      </c>
+      <c r="C4" s="2">
+        <v>13082</v>
+      </c>
+      <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v/>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1" t="str">
+        <v>99483</v>
+      </c>
+      <c r="E4" s="2">
+        <v>65258</v>
+      </c>
+      <c r="F4" s="2">
+        <v>57008</v>
+      </c>
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H4" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J4" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.65597137199320488</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.65980717815766021</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.29132255386016448</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.33703826325497799</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -845,29 +755,37 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" t="str">
+      <c r="B5" s="2">
+        <v>80102</v>
+      </c>
+      <c r="C5" s="2">
+        <v>11758</v>
+      </c>
+      <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v/>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="1" t="str">
+        <v>91860</v>
+      </c>
+      <c r="E5" s="2">
+        <v>34119</v>
+      </c>
+      <c r="F5" s="2">
+        <v>26287</v>
+      </c>
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H5" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J5" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.37142390594382757</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.32816908441736786</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.15231288447630867</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.15541195667596841</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -875,29 +793,37 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" t="str">
+      <c r="B6" s="2">
+        <v>16583</v>
+      </c>
+      <c r="C6" s="2">
+        <v>19182</v>
+      </c>
+      <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v/>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1" t="str">
+        <v>35765</v>
+      </c>
+      <c r="E6" s="2">
+        <v>22224</v>
+      </c>
+      <c r="F6" s="2">
+        <v>15100</v>
+      </c>
+      <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I6" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J6" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.62138962673004339</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.91057106675511068</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="2"/>
+        <v>9.9211628259957316E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="3"/>
+        <v>8.9273045452395589E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1558,1057 +1484,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:J28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="7" max="8" width="9.15625" style="1"/>
-    <col min="10" max="10" width="11.15625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>5505</v>
-      </c>
-      <c r="C2">
-        <v>17517</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2:D11" si="0">IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>23022</v>
-      </c>
-      <c r="E2">
-        <v>6133</v>
-      </c>
-      <c r="F2">
-        <v>4554</v>
-      </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G11" si="1">IF(D2="","",E2/D2)</f>
-        <v>0.26639735904786727</v>
-      </c>
-      <c r="H2" s="1">
-        <f>IF(ISBLANK(C2),"",F2/C2)</f>
-        <v>0.25997602329165953</v>
-      </c>
-      <c r="I2" s="1">
-        <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>0.26639735904786727</v>
-      </c>
-      <c r="J2" s="1">
-        <f>IF(ISBLANK(F2),"",F2/$D$2)</f>
-        <v>0.19781078967943705</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2121</v>
-      </c>
-      <c r="C3">
-        <v>15620</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>17741</v>
-      </c>
-      <c r="E3">
-        <v>2402</v>
-      </c>
-      <c r="F3">
-        <v>2060</v>
-      </c>
-      <c r="G3" s="1">
-        <f t="shared" si="1"/>
-        <v>0.13539259342765345</v>
-      </c>
-      <c r="H3" s="1">
-        <f t="shared" ref="H3:H10" si="2">IF(ISBLANK(C3),"",F3/C3)</f>
-        <v>0.13188220230473752</v>
-      </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I28" si="3">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.10433498392841629</v>
-      </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J26" si="4">IF(ISBLANK(F3),"",F3/$D$2)</f>
-        <v>8.9479628181739213E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4">
-        <f t="shared" ref="A4:A26" si="5">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1944</v>
-      </c>
-      <c r="C4">
-        <v>14421</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>16365</v>
-      </c>
-      <c r="E4">
-        <v>2496</v>
-      </c>
-      <c r="F4">
-        <v>2129</v>
-      </c>
-      <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>0.15252062328139321</v>
-      </c>
-      <c r="H4" s="1">
-        <f t="shared" si="2"/>
-        <v>0.14763192566396227</v>
-      </c>
-      <c r="I4" s="1">
-        <f t="shared" si="3"/>
-        <v>0.10841803492311702</v>
-      </c>
-      <c r="J4" s="1">
-        <f t="shared" si="4"/>
-        <v>9.247676135870038E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>780</v>
-      </c>
-      <c r="C5">
-        <v>12194</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>12974</v>
-      </c>
-      <c r="E5">
-        <v>5011</v>
-      </c>
-      <c r="F5">
-        <v>4781</v>
-      </c>
-      <c r="G5" s="1">
-        <f t="shared" si="1"/>
-        <v>0.38623400647448741</v>
-      </c>
-      <c r="H5" s="1">
-        <f t="shared" si="2"/>
-        <v>0.39207807118254878</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="3"/>
-        <v>0.2176613673877161</v>
-      </c>
-      <c r="J5" s="1">
-        <f t="shared" si="4"/>
-        <v>0.20767092346451221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>623</v>
-      </c>
-      <c r="C6">
-        <v>11398</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>12021</v>
-      </c>
-      <c r="E6">
-        <v>4863</v>
-      </c>
-      <c r="F6">
-        <v>4600</v>
-      </c>
-      <c r="G6" s="1">
-        <f t="shared" si="1"/>
-        <v>0.40454205141003247</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" si="2"/>
-        <v>0.40357957536409894</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" si="3"/>
-        <v>0.21123273390669794</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" si="4"/>
-        <v>0.19980887846407783</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>411</v>
-      </c>
-      <c r="C7">
-        <v>11773</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>12184</v>
-      </c>
-      <c r="E7">
-        <v>4796</v>
-      </c>
-      <c r="F7">
-        <v>4681</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.39363099146421537</v>
-      </c>
-      <c r="H7" s="1">
-        <f t="shared" si="2"/>
-        <v>0.39760468869447041</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="3"/>
-        <v>0.20832247415515595</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="4"/>
-        <v>0.20332725219355399</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1190</v>
-      </c>
-      <c r="C8">
-        <v>9357</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>10547</v>
-      </c>
-      <c r="E8">
-        <v>2340</v>
-      </c>
-      <c r="F8">
-        <v>1931</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="1"/>
-        <v>0.2218640371669669</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" si="2"/>
-        <v>0.20636956289408998</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="3"/>
-        <v>0.1016419077404222</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="4"/>
-        <v>8.387629224220311E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>187</v>
-      </c>
-      <c r="C9">
-        <v>8903</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>9090</v>
-      </c>
-      <c r="E9">
-        <v>2267</v>
-      </c>
-      <c r="F9">
-        <v>2234</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.24939493949394939</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="2"/>
-        <v>0.25092665393687519</v>
-      </c>
-      <c r="I9" s="1">
-        <f t="shared" si="3"/>
-        <v>9.8471027712622713E-2</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="4"/>
-        <v>9.70376161932065E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1387</v>
-      </c>
-      <c r="C10">
-        <v>6978</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>8365</v>
-      </c>
-      <c r="E10">
-        <v>2015</v>
-      </c>
-      <c r="F10">
-        <v>1645</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>0.24088463837417812</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" si="2"/>
-        <v>0.23574089997133849</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" si="3"/>
-        <v>8.7524976109808014E-2</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" si="4"/>
-        <v>7.1453392407262617E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>134</v>
-      </c>
-      <c r="C11">
-        <v>6455</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>6589</v>
-      </c>
-      <c r="E11">
-        <v>1347</v>
-      </c>
-      <c r="F11">
-        <v>1317</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>0.20443162847169524</v>
-      </c>
-      <c r="H11" s="1">
-        <f>IF(ISBLANK(C11),"",F11/C11)</f>
-        <v>0.2040278853601859</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" si="3"/>
-        <v>5.850925201980714E-2</v>
-      </c>
-      <c r="J11" s="1">
-        <f t="shared" si="4"/>
-        <v>5.7206150638519679E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>271</v>
-      </c>
-      <c r="C12">
-        <v>3686</v>
-      </c>
-      <c r="D12">
-        <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>3957</v>
-      </c>
-      <c r="E12">
-        <v>1226</v>
-      </c>
-      <c r="F12">
-        <v>1089</v>
-      </c>
-      <c r="G12" s="1">
-        <f>IF(D12="","",E12/D12)</f>
-        <v>0.30983067980793533</v>
-      </c>
-      <c r="H12" s="1">
-        <f>IF(ISBLANK(C12),"",F12/C12)</f>
-        <v>0.29544221378187735</v>
-      </c>
-      <c r="I12" s="1">
-        <f t="shared" si="3"/>
-        <v>5.3253409781947703E-2</v>
-      </c>
-      <c r="J12" s="1">
-        <f t="shared" si="4"/>
-        <v>4.7302580140734948E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
-        <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>84</v>
-      </c>
-      <c r="C13">
-        <v>5634</v>
-      </c>
-      <c r="D13">
-        <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>5718</v>
-      </c>
-      <c r="E13">
-        <v>1885</v>
-      </c>
-      <c r="F13">
-        <v>1857</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.32966072053165441</v>
-      </c>
-      <c r="H13" s="1">
-        <f t="shared" ref="H13:H26" si="7">IF(ISBLANK(C13),"",F13/C13)</f>
-        <v>0.32960596379126733</v>
-      </c>
-      <c r="I13" s="1">
-        <f t="shared" si="3"/>
-        <v>8.1878203457562332E-2</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" si="4"/>
-        <v>8.066197550169403E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
-        <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>242</v>
-      </c>
-      <c r="C14">
-        <v>4553</v>
-      </c>
-      <c r="D14">
-        <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>4795</v>
-      </c>
-      <c r="E14">
-        <v>1081</v>
-      </c>
-      <c r="F14">
-        <v>984</v>
-      </c>
-      <c r="G14" s="1">
-        <f t="shared" si="6"/>
-        <v>0.22544316996871741</v>
-      </c>
-      <c r="H14" s="1">
-        <f t="shared" si="7"/>
-        <v>0.2161212387436855</v>
-      </c>
-      <c r="I14" s="1">
-        <f t="shared" si="3"/>
-        <v>4.695508643905829E-2</v>
-      </c>
-      <c r="J14" s="1">
-        <f t="shared" si="4"/>
-        <v>4.2741725306228821E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>212</v>
-      </c>
-      <c r="C15">
-        <v>4499</v>
-      </c>
-      <c r="D15">
-        <f t="shared" ref="D15:D26" si="8">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>4711</v>
-      </c>
-      <c r="E15">
-        <v>1662</v>
-      </c>
-      <c r="F15">
-        <v>1534</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="6"/>
-        <v>0.35279133941838253</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="7"/>
-        <v>0.34096465881306959</v>
-      </c>
-      <c r="I15" s="1">
-        <f t="shared" si="3"/>
-        <v>7.2191816523325514E-2</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" si="4"/>
-        <v>6.6631917296499005E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>37</v>
-      </c>
-      <c r="C16">
-        <v>4525</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="8"/>
-        <v>4562</v>
-      </c>
-      <c r="E16">
-        <v>1130</v>
-      </c>
-      <c r="F16">
-        <v>1109</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" si="6"/>
-        <v>0.24769837790442789</v>
-      </c>
-      <c r="H16" s="1">
-        <f t="shared" si="7"/>
-        <v>0.24508287292817679</v>
-      </c>
-      <c r="I16" s="1">
-        <f t="shared" si="3"/>
-        <v>4.9083485361827814E-2</v>
-      </c>
-      <c r="J16" s="1">
-        <f t="shared" si="4"/>
-        <v>4.8171314394926591E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>147</v>
-      </c>
-      <c r="C17">
-        <v>4520</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="8"/>
-        <v>4667</v>
-      </c>
-      <c r="E17">
-        <v>1226</v>
-      </c>
-      <c r="F17">
-        <v>1545</v>
-      </c>
-      <c r="G17" s="1">
-        <f t="shared" si="6"/>
-        <v>0.26269552174844651</v>
-      </c>
-      <c r="H17" s="1">
-        <f t="shared" si="7"/>
-        <v>0.3418141592920354</v>
-      </c>
-      <c r="I17" s="1">
-        <f t="shared" si="3"/>
-        <v>5.3253409781947703E-2</v>
-      </c>
-      <c r="J17" s="1">
-        <f t="shared" si="4"/>
-        <v>6.7109721136304409E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>103</v>
-      </c>
-      <c r="C18">
-        <v>3827</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="8"/>
-        <v>3930</v>
-      </c>
-      <c r="E18">
-        <v>923</v>
-      </c>
-      <c r="F18">
-        <v>1196</v>
-      </c>
-      <c r="G18" s="1">
-        <f t="shared" si="6"/>
-        <v>0.23486005089058523</v>
-      </c>
-      <c r="H18" s="1">
-        <f t="shared" si="7"/>
-        <v>0.31251633133002354</v>
-      </c>
-      <c r="I18" s="1">
-        <f t="shared" si="3"/>
-        <v>4.0092085830944313E-2</v>
-      </c>
-      <c r="J18" s="1">
-        <f t="shared" si="4"/>
-        <v>5.1950308400660235E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
-        <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>40</v>
-      </c>
-      <c r="C19">
-        <v>4251</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="8"/>
-        <v>4291</v>
-      </c>
-      <c r="E19">
-        <v>1880</v>
-      </c>
-      <c r="F19">
-        <v>1857</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" si="6"/>
-        <v>0.438126310883244</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" si="7"/>
-        <v>0.43683839096683136</v>
-      </c>
-      <c r="I19" s="1">
-        <f t="shared" si="3"/>
-        <v>8.1661019894014419E-2</v>
-      </c>
-      <c r="J19" s="1">
-        <f t="shared" si="4"/>
-        <v>8.066197550169403E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
-        <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>791</v>
-      </c>
-      <c r="C20">
-        <v>3614</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="8"/>
-        <v>4405</v>
-      </c>
-      <c r="E20">
-        <v>2049</v>
-      </c>
-      <c r="F20">
-        <v>1511</v>
-      </c>
-      <c r="G20" s="1">
-        <f t="shared" si="6"/>
-        <v>0.46515323496027244</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" si="7"/>
-        <v>0.41809629219701161</v>
-      </c>
-      <c r="I20" s="1">
-        <f t="shared" si="3"/>
-        <v>8.9001824341933808E-2</v>
-      </c>
-      <c r="J20" s="1">
-        <f t="shared" si="4"/>
-        <v>6.5632872904178616E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
-        <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>201</v>
-      </c>
-      <c r="C21">
-        <v>3986</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="8"/>
-        <v>4187</v>
-      </c>
-      <c r="E21">
-        <v>1579</v>
-      </c>
-      <c r="F21">
-        <v>1412</v>
-      </c>
-      <c r="G21" s="1">
-        <f t="shared" si="6"/>
-        <v>0.37711965607833769</v>
-      </c>
-      <c r="H21" s="1">
-        <f t="shared" si="7"/>
-        <v>0.35423983943803311</v>
-      </c>
-      <c r="I21" s="1">
-        <f t="shared" si="3"/>
-        <v>6.8586569368430203E-2</v>
-      </c>
-      <c r="J21" s="1">
-        <f t="shared" si="4"/>
-        <v>6.1332638345929981E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
-        <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>250</v>
-      </c>
-      <c r="C22">
-        <v>3512</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="8"/>
-        <v>3762</v>
-      </c>
-      <c r="E22">
-        <v>1226</v>
-      </c>
-      <c r="F22">
-        <v>1499</v>
-      </c>
-      <c r="G22" s="1">
-        <f t="shared" si="6"/>
-        <v>0.32589048378522062</v>
-      </c>
-      <c r="H22" s="1">
-        <f t="shared" si="7"/>
-        <v>0.42682232346241455</v>
-      </c>
-      <c r="I22" s="1">
-        <f t="shared" si="3"/>
-        <v>5.3253409781947703E-2</v>
-      </c>
-      <c r="J22" s="1">
-        <f t="shared" si="4"/>
-        <v>6.5111632351663631E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23">
-        <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>952</v>
-      </c>
-      <c r="C23">
-        <v>2659</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="8"/>
-        <v>3611</v>
-      </c>
-      <c r="E23">
-        <v>1220</v>
-      </c>
-      <c r="F23">
-        <v>613</v>
-      </c>
-      <c r="G23" s="1">
-        <f t="shared" si="6"/>
-        <v>0.33785654943229021</v>
-      </c>
-      <c r="H23" s="1">
-        <f t="shared" si="7"/>
-        <v>0.23053779616397141</v>
-      </c>
-      <c r="I23" s="1">
-        <f t="shared" si="3"/>
-        <v>5.299278950569021E-2</v>
-      </c>
-      <c r="J23" s="1">
-        <f t="shared" si="4"/>
-        <v>2.6626704890973851E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>182</v>
-      </c>
-      <c r="C24">
-        <v>2885</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="8"/>
-        <v>3067</v>
-      </c>
-      <c r="E24">
-        <v>1773</v>
-      </c>
-      <c r="F24">
-        <v>1645</v>
-      </c>
-      <c r="G24" s="1">
-        <f t="shared" si="6"/>
-        <v>0.57808933811542229</v>
-      </c>
-      <c r="H24" s="1">
-        <f t="shared" si="7"/>
-        <v>0.57019064124783359</v>
-      </c>
-      <c r="I24" s="1">
-        <f t="shared" si="3"/>
-        <v>7.7013291634089126E-2</v>
-      </c>
-      <c r="J24" s="1">
-        <f t="shared" si="4"/>
-        <v>7.1453392407262617E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25">
-        <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>18</v>
-      </c>
-      <c r="C25">
-        <v>2591</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="8"/>
-        <v>2609</v>
-      </c>
-      <c r="E25">
-        <v>1391</v>
-      </c>
-      <c r="F25">
-        <v>1382</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" si="6"/>
-        <v>0.5331544653123802</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" si="7"/>
-        <v>0.53338479351601698</v>
-      </c>
-      <c r="I25" s="1">
-        <f t="shared" si="3"/>
-        <v>6.0420467379028758E-2</v>
-      </c>
-      <c r="J25" s="1">
-        <f t="shared" si="4"/>
-        <v>6.0029536964642513E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>406</v>
-      </c>
-      <c r="C26">
-        <v>2221</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="8"/>
-        <v>2627</v>
-      </c>
-      <c r="E26">
-        <v>1481</v>
-      </c>
-      <c r="F26">
-        <v>1211</v>
-      </c>
-      <c r="G26" s="1">
-        <f t="shared" si="6"/>
-        <v>0.56376094404263422</v>
-      </c>
-      <c r="H26" s="1">
-        <f t="shared" si="7"/>
-        <v>0.545249887438091</v>
-      </c>
-      <c r="I26" s="1">
-        <f t="shared" si="3"/>
-        <v>6.4329771522891141E-2</v>
-      </c>
-      <c r="J26" s="1">
-        <f t="shared" si="4"/>
-        <v>5.2601859091303972E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="I27" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="I28" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:N26">
-    <sortCondition ref="L2:L26"/>
-  </sortState>
-  <conditionalFormatting sqref="E1:F1048576">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I1:J1048576">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J28"/>
@@ -3684,272 +2559,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BC8E35-EAE3-45F9-9A2E-8D885D01E5AC}">
-  <dimension ref="A1:D25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="1" max="2" width="16.41796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="12">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>113625</v>
-      </c>
-      <c r="D1">
-        <v>42560</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="12">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>41895</v>
-      </c>
-      <c r="D2">
-        <v>3730</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="11"/>
-      <c r="C6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="11"/>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D25">
-    <sortCondition ref="B1:B25"/>
-  </sortState>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://adventofcode.com/2023/day/2" xr:uid="{7315C9F7-0CF4-4B4E-8775-5A9EC0FF39A5}"/>
-    <hyperlink ref="A1" r:id="rId2" display="https://adventofcode.com/2023/day/1" xr:uid="{A9D74035-9C91-474B-B69D-81192737DCAA}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3960,358 +2574,358 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="13">
+      <c r="B1" s="11">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11">
         <v>2</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11">
         <v>3</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11">
         <v>4</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13">
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11">
         <v>5</v>
       </c>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13">
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11">
         <v>6</v>
       </c>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13">
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11">
         <v>7</v>
       </c>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13">
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11">
         <v>8</v>
       </c>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13">
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11">
         <v>9</v>
       </c>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13">
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11">
         <v>10</v>
       </c>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13">
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11">
         <v>11</v>
       </c>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13">
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11">
         <v>12</v>
       </c>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13">
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11">
         <v>13</v>
       </c>
-      <c r="AY1" s="13"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13">
-        <v>14</v>
-      </c>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13">
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11">
+        <v>14</v>
+      </c>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11">
         <v>15</v>
       </c>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13">
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11">
         <v>16</v>
       </c>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13"/>
-      <c r="BN1" s="13">
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11">
         <v>17</v>
       </c>
-      <c r="BO1" s="13"/>
-      <c r="BP1" s="13"/>
-      <c r="BQ1" s="13"/>
-      <c r="BR1" s="13">
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11">
         <v>18</v>
       </c>
-      <c r="BS1" s="13"/>
-      <c r="BT1" s="13"/>
-      <c r="BU1" s="13"/>
-      <c r="BV1" s="13">
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11">
         <v>19</v>
       </c>
-      <c r="BW1" s="13"/>
-      <c r="BX1" s="13"/>
-      <c r="BY1" s="13"/>
-      <c r="BZ1" s="13">
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11">
         <v>20</v>
       </c>
-      <c r="CA1" s="13"/>
-      <c r="CB1" s="13"/>
-      <c r="CC1" s="13"/>
-      <c r="CD1" s="13">
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11">
         <v>21</v>
       </c>
-      <c r="CE1" s="13"/>
-      <c r="CF1" s="13"/>
-      <c r="CG1" s="13"/>
-      <c r="CH1" s="13">
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11">
         <v>22</v>
       </c>
-      <c r="CI1" s="13"/>
-      <c r="CJ1" s="13"/>
-      <c r="CK1" s="13"/>
-      <c r="CL1" s="13">
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11">
         <v>23</v>
       </c>
-      <c r="CM1" s="13"/>
-      <c r="CN1" s="13"/>
-      <c r="CO1" s="13"/>
-      <c r="CP1" s="13">
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11">
         <v>24</v>
       </c>
-      <c r="CQ1" s="13"/>
-      <c r="CR1" s="13"/>
-      <c r="CS1" s="13"/>
-      <c r="CT1" s="13">
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11">
         <v>25</v>
       </c>
-      <c r="CU1" s="13"/>
-      <c r="CV1" s="13"/>
-      <c r="CW1" s="13"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
     </row>
     <row r="2" spans="1:102" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13" t="s">
+      <c r="I2" s="11"/>
+      <c r="J2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13" t="s">
+      <c r="K2" s="11"/>
+      <c r="L2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13" t="s">
+      <c r="M2" s="11"/>
+      <c r="N2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13" t="s">
+      <c r="O2" s="11"/>
+      <c r="P2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13" t="s">
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13" t="s">
+      <c r="S2" s="11"/>
+      <c r="T2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13" t="s">
+      <c r="U2" s="11"/>
+      <c r="V2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13" t="s">
+      <c r="W2" s="11"/>
+      <c r="X2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13" t="s">
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13" t="s">
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13" t="s">
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13" t="s">
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AG2" s="13"/>
-      <c r="AH2" s="13" t="s">
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13" t="s">
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AK2" s="13"/>
-      <c r="AL2" s="13" t="s">
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AM2" s="13"/>
-      <c r="AN2" s="13" t="s">
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AO2" s="13"/>
-      <c r="AP2" s="13" t="s">
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AQ2" s="13"/>
-      <c r="AR2" s="13" t="s">
+      <c r="AQ2" s="11"/>
+      <c r="AR2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AS2" s="13"/>
-      <c r="AT2" s="13" t="s">
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AU2" s="13"/>
-      <c r="AV2" s="13" t="s">
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AW2" s="13"/>
-      <c r="AX2" s="13" t="s">
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AY2" s="13"/>
-      <c r="AZ2" s="13" t="s">
+      <c r="AY2" s="11"/>
+      <c r="AZ2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BA2" s="13"/>
-      <c r="BB2" s="13" t="s">
+      <c r="BA2" s="11"/>
+      <c r="BB2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BC2" s="13"/>
-      <c r="BD2" s="13" t="s">
+      <c r="BC2" s="11"/>
+      <c r="BD2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BE2" s="13"/>
-      <c r="BF2" s="13" t="s">
+      <c r="BE2" s="11"/>
+      <c r="BF2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BG2" s="13"/>
-      <c r="BH2" s="13" t="s">
+      <c r="BG2" s="11"/>
+      <c r="BH2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BI2" s="13"/>
-      <c r="BJ2" s="13" t="s">
+      <c r="BI2" s="11"/>
+      <c r="BJ2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BK2" s="13"/>
-      <c r="BL2" s="13" t="s">
+      <c r="BK2" s="11"/>
+      <c r="BL2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BM2" s="13"/>
-      <c r="BN2" s="13" t="s">
+      <c r="BM2" s="11"/>
+      <c r="BN2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BO2" s="13"/>
-      <c r="BP2" s="13" t="s">
+      <c r="BO2" s="11"/>
+      <c r="BP2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BQ2" s="13"/>
-      <c r="BR2" s="13" t="s">
+      <c r="BQ2" s="11"/>
+      <c r="BR2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BS2" s="13"/>
-      <c r="BT2" s="13" t="s">
+      <c r="BS2" s="11"/>
+      <c r="BT2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BU2" s="13"/>
-      <c r="BV2" s="13" t="s">
+      <c r="BU2" s="11"/>
+      <c r="BV2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="BW2" s="13"/>
-      <c r="BX2" s="13" t="s">
+      <c r="BW2" s="11"/>
+      <c r="BX2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BY2" s="13"/>
-      <c r="BZ2" s="13" t="s">
+      <c r="BY2" s="11"/>
+      <c r="BZ2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CA2" s="13"/>
-      <c r="CB2" s="13" t="s">
+      <c r="CA2" s="11"/>
+      <c r="CB2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CC2" s="13"/>
-      <c r="CD2" s="13" t="s">
+      <c r="CC2" s="11"/>
+      <c r="CD2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CE2" s="13"/>
-      <c r="CF2" s="13" t="s">
+      <c r="CE2" s="11"/>
+      <c r="CF2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CG2" s="13"/>
-      <c r="CH2" s="13" t="s">
+      <c r="CG2" s="11"/>
+      <c r="CH2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CI2" s="13"/>
-      <c r="CJ2" s="13" t="s">
+      <c r="CI2" s="11"/>
+      <c r="CJ2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CK2" s="13"/>
-      <c r="CL2" s="13" t="s">
+      <c r="CK2" s="11"/>
+      <c r="CL2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CM2" s="13"/>
-      <c r="CN2" s="13" t="s">
+      <c r="CM2" s="11"/>
+      <c r="CN2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CO2" s="13"/>
-      <c r="CP2" s="13" t="s">
+      <c r="CO2" s="11"/>
+      <c r="CP2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CQ2" s="13"/>
-      <c r="CR2" s="13" t="s">
+      <c r="CQ2" s="11"/>
+      <c r="CR2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CS2" s="13"/>
-      <c r="CT2" s="13" t="s">
+      <c r="CS2" s="11"/>
+      <c r="CT2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="CU2" s="13"/>
-      <c r="CV2" s="13" t="s">
+      <c r="CU2" s="11"/>
+      <c r="CV2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="CW2" s="13"/>
+      <c r="CW2" s="11"/>
     </row>
     <row r="3" spans="1:102" x14ac:dyDescent="0.55000000000000004">
       <c r="B3">
@@ -7108,16 +5722,16 @@
         <v>14</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="K12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="L12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="M12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="N12" t="s">
         <v>20</v>
@@ -7445,47 +6059,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -7502,24 +6093,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
@@ -7548,7 +6162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A3E9AF-60E4-42C2-9582-F318C9A6FCBA}">
   <dimension ref="A1:J26"/>
   <sheetViews>
@@ -8477,7 +7091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
@@ -9441,7 +8055,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
@@ -10497,7 +9111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
@@ -11507,7 +10121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J26"/>
@@ -12557,7 +11171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J26"/>
@@ -13605,4 +12219,1055 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="7" max="8" width="9.15625" style="1"/>
+    <col min="10" max="10" width="11.15625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>5505</v>
+      </c>
+      <c r="C2">
+        <v>17517</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D11" si="0">IF(ISBLANK(B2),"",B2+C2)</f>
+        <v>23022</v>
+      </c>
+      <c r="E2">
+        <v>6133</v>
+      </c>
+      <c r="F2">
+        <v>4554</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" ref="G2:G11" si="1">IF(D2="","",E2/D2)</f>
+        <v>0.26639735904786727</v>
+      </c>
+      <c r="H2" s="1">
+        <f>IF(ISBLANK(C2),"",F2/C2)</f>
+        <v>0.25997602329165953</v>
+      </c>
+      <c r="I2" s="1">
+        <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
+        <v>0.26639735904786727</v>
+      </c>
+      <c r="J2" s="1">
+        <f>IF(ISBLANK(F2),"",F2/$D$2)</f>
+        <v>0.19781078967943705</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2121</v>
+      </c>
+      <c r="C3">
+        <v>15620</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>17741</v>
+      </c>
+      <c r="E3">
+        <v>2402</v>
+      </c>
+      <c r="F3">
+        <v>2060</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="1"/>
+        <v>0.13539259342765345</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H10" si="2">IF(ISBLANK(C3),"",F3/C3)</f>
+        <v>0.13188220230473752</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I28" si="3">IF(ISBLANK(E3),"",E3/$D$2)</f>
+        <v>0.10433498392841629</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J26" si="4">IF(ISBLANK(F3),"",F3/$D$2)</f>
+        <v>8.9479628181739213E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <f t="shared" ref="A4:A26" si="5">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1944</v>
+      </c>
+      <c r="C4">
+        <v>14421</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>16365</v>
+      </c>
+      <c r="E4">
+        <v>2496</v>
+      </c>
+      <c r="F4">
+        <v>2129</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.15252062328139321</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="2"/>
+        <v>0.14763192566396227</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.10841803492311702</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="4"/>
+        <v>9.247676135870038E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>780</v>
+      </c>
+      <c r="C5">
+        <v>12194</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>12974</v>
+      </c>
+      <c r="E5">
+        <v>5011</v>
+      </c>
+      <c r="F5">
+        <v>4781</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.38623400647448741</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="2"/>
+        <v>0.39207807118254878</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.2176613673877161</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="4"/>
+        <v>0.20767092346451221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>623</v>
+      </c>
+      <c r="C6">
+        <v>11398</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>12021</v>
+      </c>
+      <c r="E6">
+        <v>4863</v>
+      </c>
+      <c r="F6">
+        <v>4600</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.40454205141003247</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.40357957536409894</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.21123273390669794</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="4"/>
+        <v>0.19980887846407783</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>411</v>
+      </c>
+      <c r="C7">
+        <v>11773</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>12184</v>
+      </c>
+      <c r="E7">
+        <v>4796</v>
+      </c>
+      <c r="F7">
+        <v>4681</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.39363099146421537</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.39760468869447041</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="3"/>
+        <v>0.20832247415515595</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="4"/>
+        <v>0.20332725219355399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1190</v>
+      </c>
+      <c r="C8">
+        <v>9357</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>10547</v>
+      </c>
+      <c r="E8">
+        <v>2340</v>
+      </c>
+      <c r="F8">
+        <v>1931</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.2218640371669669</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>0.20636956289408998</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.1016419077404222</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="4"/>
+        <v>8.387629224220311E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>187</v>
+      </c>
+      <c r="C9">
+        <v>8903</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>9090</v>
+      </c>
+      <c r="E9">
+        <v>2267</v>
+      </c>
+      <c r="F9">
+        <v>2234</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24939493949394939</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.25092665393687519</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="3"/>
+        <v>9.8471027712622713E-2</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="4"/>
+        <v>9.70376161932065E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1387</v>
+      </c>
+      <c r="C10">
+        <v>6978</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>8365</v>
+      </c>
+      <c r="E10">
+        <v>2015</v>
+      </c>
+      <c r="F10">
+        <v>1645</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.24088463837417812</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>0.23574089997133849</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="3"/>
+        <v>8.7524976109808014E-2</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="4"/>
+        <v>7.1453392407262617E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>134</v>
+      </c>
+      <c r="C11">
+        <v>6455</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>6589</v>
+      </c>
+      <c r="E11">
+        <v>1347</v>
+      </c>
+      <c r="F11">
+        <v>1317</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.20443162847169524</v>
+      </c>
+      <c r="H11" s="1">
+        <f>IF(ISBLANK(C11),"",F11/C11)</f>
+        <v>0.2040278853601859</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="3"/>
+        <v>5.850925201980714E-2</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="4"/>
+        <v>5.7206150638519679E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>271</v>
+      </c>
+      <c r="C12">
+        <v>3686</v>
+      </c>
+      <c r="D12">
+        <f>IF(ISBLANK(B12),"",B12+C12)</f>
+        <v>3957</v>
+      </c>
+      <c r="E12">
+        <v>1226</v>
+      </c>
+      <c r="F12">
+        <v>1089</v>
+      </c>
+      <c r="G12" s="1">
+        <f>IF(D12="","",E12/D12)</f>
+        <v>0.30983067980793533</v>
+      </c>
+      <c r="H12" s="1">
+        <f>IF(ISBLANK(C12),"",F12/C12)</f>
+        <v>0.29544221378187735</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3253409781947703E-2</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="4"/>
+        <v>4.7302580140734948E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>84</v>
+      </c>
+      <c r="C13">
+        <v>5634</v>
+      </c>
+      <c r="D13">
+        <f>IF(ISBLANK(B13),"",B13+C13)</f>
+        <v>5718</v>
+      </c>
+      <c r="E13">
+        <v>1885</v>
+      </c>
+      <c r="F13">
+        <v>1857</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
+        <v>0.32966072053165441</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" ref="H13:H26" si="7">IF(ISBLANK(C13),"",F13/C13)</f>
+        <v>0.32960596379126733</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="3"/>
+        <v>8.1878203457562332E-2</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="4"/>
+        <v>8.066197550169403E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>242</v>
+      </c>
+      <c r="C14">
+        <v>4553</v>
+      </c>
+      <c r="D14">
+        <f>IF(ISBLANK(B14),"",B14+C14)</f>
+        <v>4795</v>
+      </c>
+      <c r="E14">
+        <v>1081</v>
+      </c>
+      <c r="F14">
+        <v>984</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="6"/>
+        <v>0.22544316996871741</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="7"/>
+        <v>0.2161212387436855</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="3"/>
+        <v>4.695508643905829E-2</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="4"/>
+        <v>4.2741725306228821E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>212</v>
+      </c>
+      <c r="C15">
+        <v>4499</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:D26" si="8">IF(ISBLANK(B15),"",B15+C15)</f>
+        <v>4711</v>
+      </c>
+      <c r="E15">
+        <v>1662</v>
+      </c>
+      <c r="F15">
+        <v>1534</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="6"/>
+        <v>0.35279133941838253</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="7"/>
+        <v>0.34096465881306959</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="3"/>
+        <v>7.2191816523325514E-2</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="4"/>
+        <v>6.6631917296499005E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <v>4525</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="8"/>
+        <v>4562</v>
+      </c>
+      <c r="E16">
+        <v>1130</v>
+      </c>
+      <c r="F16">
+        <v>1109</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="6"/>
+        <v>0.24769837790442789</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="7"/>
+        <v>0.24508287292817679</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="3"/>
+        <v>4.9083485361827814E-2</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="4"/>
+        <v>4.8171314394926591E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>147</v>
+      </c>
+      <c r="C17">
+        <v>4520</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="8"/>
+        <v>4667</v>
+      </c>
+      <c r="E17">
+        <v>1226</v>
+      </c>
+      <c r="F17">
+        <v>1545</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="6"/>
+        <v>0.26269552174844651</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="7"/>
+        <v>0.3418141592920354</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3253409781947703E-2</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="4"/>
+        <v>6.7109721136304409E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>103</v>
+      </c>
+      <c r="C18">
+        <v>3827</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="8"/>
+        <v>3930</v>
+      </c>
+      <c r="E18">
+        <v>923</v>
+      </c>
+      <c r="F18">
+        <v>1196</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="6"/>
+        <v>0.23486005089058523</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="7"/>
+        <v>0.31251633133002354</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="3"/>
+        <v>4.0092085830944313E-2</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="4"/>
+        <v>5.1950308400660235E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>4251</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="8"/>
+        <v>4291</v>
+      </c>
+      <c r="E19">
+        <v>1880</v>
+      </c>
+      <c r="F19">
+        <v>1857</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="6"/>
+        <v>0.438126310883244</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="7"/>
+        <v>0.43683839096683136</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="3"/>
+        <v>8.1661019894014419E-2</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="4"/>
+        <v>8.066197550169403E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>791</v>
+      </c>
+      <c r="C20">
+        <v>3614</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="8"/>
+        <v>4405</v>
+      </c>
+      <c r="E20">
+        <v>2049</v>
+      </c>
+      <c r="F20">
+        <v>1511</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="6"/>
+        <v>0.46515323496027244</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="7"/>
+        <v>0.41809629219701161</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="3"/>
+        <v>8.9001824341933808E-2</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="4"/>
+        <v>6.5632872904178616E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>201</v>
+      </c>
+      <c r="C21">
+        <v>3986</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="8"/>
+        <v>4187</v>
+      </c>
+      <c r="E21">
+        <v>1579</v>
+      </c>
+      <c r="F21">
+        <v>1412</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="6"/>
+        <v>0.37711965607833769</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="7"/>
+        <v>0.35423983943803311</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="3"/>
+        <v>6.8586569368430203E-2</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="4"/>
+        <v>6.1332638345929981E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>250</v>
+      </c>
+      <c r="C22">
+        <v>3512</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="8"/>
+        <v>3762</v>
+      </c>
+      <c r="E22">
+        <v>1226</v>
+      </c>
+      <c r="F22">
+        <v>1499</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="6"/>
+        <v>0.32589048378522062</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="7"/>
+        <v>0.42682232346241455</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="3"/>
+        <v>5.3253409781947703E-2</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="4"/>
+        <v>6.5111632351663631E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>952</v>
+      </c>
+      <c r="C23">
+        <v>2659</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="8"/>
+        <v>3611</v>
+      </c>
+      <c r="E23">
+        <v>1220</v>
+      </c>
+      <c r="F23">
+        <v>613</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="6"/>
+        <v>0.33785654943229021</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="7"/>
+        <v>0.23053779616397141</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="3"/>
+        <v>5.299278950569021E-2</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="4"/>
+        <v>2.6626704890973851E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>182</v>
+      </c>
+      <c r="C24">
+        <v>2885</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="8"/>
+        <v>3067</v>
+      </c>
+      <c r="E24">
+        <v>1773</v>
+      </c>
+      <c r="F24">
+        <v>1645</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="6"/>
+        <v>0.57808933811542229</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="7"/>
+        <v>0.57019064124783359</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="3"/>
+        <v>7.7013291634089126E-2</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="4"/>
+        <v>7.1453392407262617E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>2591</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="8"/>
+        <v>2609</v>
+      </c>
+      <c r="E25">
+        <v>1391</v>
+      </c>
+      <c r="F25">
+        <v>1382</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="6"/>
+        <v>0.5331544653123802</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="7"/>
+        <v>0.53338479351601698</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="3"/>
+        <v>6.0420467379028758E-2</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="4"/>
+        <v>6.0029536964642513E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>406</v>
+      </c>
+      <c r="C26">
+        <v>2221</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="8"/>
+        <v>2627</v>
+      </c>
+      <c r="E26">
+        <v>1481</v>
+      </c>
+      <c r="F26">
+        <v>1211</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="6"/>
+        <v>0.56376094404263422</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="7"/>
+        <v>0.545249887438091</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="3"/>
+        <v>6.4329771522891141E-2</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="4"/>
+        <v>5.2601859091303972E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:N26">
+    <sortCondition ref="L2:L26"/>
+  </sortState>
+  <conditionalFormatting sqref="E1:F1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:H1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:J1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
2023 day 6 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8923453-2E29-4B47-A0CF-C6F6AB50ACB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8F5E05-840E-4B47-917F-2E3AAB502187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2538" yWindow="570" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4182" yWindow="426" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -596,7 +596,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -642,14 +642,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>169144</v>
+        <v>177167</v>
       </c>
       <c r="C2" s="2">
-        <v>54862</v>
+        <v>57076</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>224006</v>
+        <v>234243</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -659,19 +659,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>0.11380498736640983</v>
+        <v>0.10883142719312851</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>0.1215414085039966</v>
+        <v>0.11603741103027088</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>0.11380498736640983</v>
+        <v>0.10883142719312851</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>0.1215414085039966</v>
+        <v>0.11603741103027088</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -680,14 +680,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>136839</v>
+        <v>144771</v>
       </c>
       <c r="C3" s="2">
-        <v>6109</v>
+        <v>6498</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>142948</v>
+        <v>151269</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -697,19 +697,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.20606794078965779</v>
+        <v>0.19473256252107174</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.21635644808862969</v>
+        <v>0.20450228291577732</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.1315009419390552</v>
+        <v>0.12575402466669228</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.17503429030884926</v>
+        <v>0.16710786997578556</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -718,14 +718,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>86401</v>
+        <v>92609</v>
       </c>
       <c r="C4" s="2">
-        <v>13082</v>
+        <v>13981</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>99483</v>
+        <v>106590</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -735,19 +735,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.65597137199320488</v>
+        <v>0.61223379303874659</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.65980717815766021</v>
+        <v>0.61557731969894935</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.29132255386016448</v>
+        <v>0.27859103580469852</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.33703826325497799</v>
+        <v>0.32177549995202265</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -756,14 +756,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>80102</v>
+        <v>88627</v>
       </c>
       <c r="C5" s="2">
-        <v>11758</v>
+        <v>12189</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>91860</v>
+        <v>100816</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -773,19 +773,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.37142390594382757</v>
+        <v>0.33842842405967305</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.32816908441736786</v>
+        <v>0.29660261545578659</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.15231288447630867</v>
+        <v>0.14565643370346179</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.15541195667596841</v>
+        <v>0.14837413288027679</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -794,14 +794,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>16583</v>
+        <v>43521</v>
       </c>
       <c r="C6" s="2">
-        <v>19182</v>
+        <v>24745</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>35765</v>
+        <v>68266</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -811,19 +811,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.62138962673004339</v>
+        <v>0.32555005419974803</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.91057106675511068</v>
+        <v>0.34695893936260658</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>9.9211628259957316E-2</v>
+        <v>9.4875834069748088E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>8.9273045452395589E-2</v>
+        <v>8.523031941614409E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -831,29 +831,37 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" t="str">
+      <c r="B7" s="2">
+        <v>24833</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1559</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="1" t="str">
+        <v>26392</v>
+      </c>
+      <c r="E7" s="2">
+        <v>23988</v>
+      </c>
+      <c r="F7" s="2">
+        <v>23393</v>
+      </c>
+      <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I7" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J7" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.90891179145195511</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.94201264446502642</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.10240647532690411</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="3"/>
+        <v>0.13203926239085156</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2563,7 +2571,7 @@
   <dimension ref="A1:CX20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5734,16 +5742,16 @@
         <v>14</v>
       </c>
       <c r="N12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="O12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="P12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="Q12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="R12" t="s">
         <v>20</v>
@@ -6059,24 +6067,47 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6093,47 +6124,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 day 7 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8F5E05-840E-4B47-917F-2E3AAB502187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE31480-8B4E-45AB-BCA0-12466D4CE0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4182" yWindow="426" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11730" yWindow="1044" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -596,7 +596,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -642,14 +642,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>177167</v>
+        <v>184667</v>
       </c>
       <c r="C2" s="2">
-        <v>57076</v>
+        <v>59242</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>234243</v>
+        <v>243909</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -659,19 +659,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>0.10883142719312851</v>
+        <v>0.10451848845266062</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>0.11603741103027088</v>
+        <v>0.11132470880016462</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>0.10883142719312851</v>
+        <v>0.10451848845266062</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>0.11603741103027088</v>
+        <v>0.11132470880016462</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -680,14 +680,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>144771</v>
+        <v>152385</v>
       </c>
       <c r="C3" s="2">
-        <v>6498</v>
+        <v>6778</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>151269</v>
+        <v>159163</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -697,19 +697,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.19473256252107174</v>
+        <v>0.18507442056256793</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.20450228291577732</v>
+        <v>0.19428421432555698</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.12575402466669228</v>
+        <v>0.1207704512748607</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.16710786997578556</v>
+        <v>0.16032101025088402</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -718,14 +718,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>92609</v>
+        <v>98542</v>
       </c>
       <c r="C4" s="2">
-        <v>13981</v>
+        <v>14719</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>106590</v>
+        <v>113261</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -735,19 +735,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.61223379303874659</v>
+        <v>0.57617361669065259</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.61557731969894935</v>
+        <v>0.57851474498183519</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.27859103580469852</v>
+        <v>0.2675506028887823</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.32177549995202265</v>
+        <v>0.30870702399454153</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -756,14 +756,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>88627</v>
+        <v>95535</v>
       </c>
       <c r="C5" s="2">
-        <v>12189</v>
+        <v>12904</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>100816</v>
+        <v>108439</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -773,19 +773,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.33842842405967305</v>
+        <v>0.31463772259058087</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.29660261545578659</v>
+        <v>0.27515570209870727</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.14565643370346179</v>
+        <v>0.13988413711671155</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.14837413288027679</v>
+        <v>0.14234811850520127</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -794,14 +794,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>43521</v>
+        <v>54001</v>
       </c>
       <c r="C6" s="2">
-        <v>24745</v>
+        <v>23849</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>68266</v>
+        <v>77850</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -811,19 +811,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.32555005419974803</v>
+        <v>0.28547206165703276</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.34695893936260658</v>
+        <v>0.27962445139904818</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>9.4875834069748088E-2</v>
+        <v>9.1115948980972417E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>8.523031941614409E-2</v>
+        <v>8.1768805471470266E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -832,14 +832,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>24833</v>
+        <v>66391</v>
       </c>
       <c r="C7" s="2">
-        <v>1559</v>
+        <v>1225</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>26392</v>
+        <v>67616</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -849,19 +849,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.90891179145195511</v>
+        <v>0.35476810222432559</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.94201264446502642</v>
+        <v>0.35235197541835489</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>0.10240647532690411</v>
+        <v>9.8348154434645702E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.13203926239085156</v>
+        <v>0.12667666664861615</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -869,29 +869,37 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" t="str">
+      <c r="B8" s="2">
+        <v>18092</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5528</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="1" t="str">
+        <v>23620</v>
+      </c>
+      <c r="E8" s="2">
+        <v>21528</v>
+      </c>
+      <c r="F8" s="2">
+        <v>17984</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J8" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.91143099068585942</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.99403051072297144</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="2"/>
+        <v>8.826242574074758E-2</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="3"/>
+        <v>9.7386105801253064E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2571,7 +2579,7 @@
   <dimension ref="A1:CX20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5754,40 +5762,40 @@
         <v>14</v>
       </c>
       <c r="R12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="S12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="T12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="U12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="V12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="W12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="X12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="Y12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="Z12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AA12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AB12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AC12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AD12" t="s">
         <v>20</v>
@@ -6067,47 +6075,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6124,24 +6109,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 day 8 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE31480-8B4E-45AB-BCA0-12466D4CE0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765BF4B2-ECBE-4D83-A5BE-519C25155D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11730" yWindow="1044" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6252" yWindow="1002" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="30">
   <si>
     <t>Day</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>not done yet</t>
+  </si>
+  <si>
+    <t>Excuse</t>
+  </si>
+  <si>
+    <t>Hillwalking</t>
   </si>
 </sst>
 </file>
@@ -593,19 +599,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="10.26171875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -636,20 +643,23 @@
       <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>184667</v>
+        <v>189859</v>
       </c>
       <c r="C2" s="2">
-        <v>59242</v>
+        <v>60848</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>243909</v>
+        <v>250707</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -659,35 +669,35 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>0.10451848845266062</v>
+        <v>0.10168443641382172</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>0.11132470880016462</v>
+        <v>0.10828035542165501</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>0.10451848845266062</v>
+        <v>0.10168443641382172</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>0.11132470880016462</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.10828035542165501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>152385</v>
+        <v>157457</v>
       </c>
       <c r="C3" s="2">
-        <v>6778</v>
+        <v>7133</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>159163</v>
+        <v>164590</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -697,35 +707,35 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.18507442056256793</v>
+        <v>0.17897199100795916</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.19428421432555698</v>
+        <v>0.18802593724000838</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.1207704512748607</v>
+        <v>0.11749572209790712</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.16032101025088402</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.15593677413238244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f t="shared" ref="A4:A26" si="4">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>98542</v>
+        <v>102369</v>
       </c>
       <c r="C4" s="2">
-        <v>14719</v>
+        <v>15263</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>113261</v>
+        <v>117632</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -735,35 +745,38 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.57617361669065259</v>
+        <v>0.55476400979325358</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.57851474498183519</v>
+        <v>0.55688733894049958</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.2675506028887823</v>
+        <v>0.26029588324219111</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.30870702399454153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.30026493345061334</v>
+      </c>
+      <c r="K4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>95535</v>
+        <v>99971</v>
       </c>
       <c r="C5" s="2">
-        <v>12904</v>
+        <v>13504</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>108439</v>
+        <v>113475</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -773,35 +786,35 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.31463772259058087</v>
+        <v>0.30067415730337077</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.27515570209870727</v>
+        <v>0.26294625441378</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.13988413711671155</v>
+        <v>0.13609113427227801</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.14234811850520127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.13845538004519142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>54001</v>
+        <v>58165</v>
       </c>
       <c r="C6" s="2">
-        <v>23849</v>
+        <v>24323</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>77850</v>
+        <v>82488</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -811,35 +824,35 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.28547206165703276</v>
+        <v>0.26942100669188246</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.27962445139904818</v>
+        <v>0.25960629244390959</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>9.1115948980972417E-2</v>
+        <v>8.8645311060321405E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>8.1768805471470266E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>7.9532705850130891E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>66391</v>
+        <v>73263</v>
       </c>
       <c r="C7" s="2">
-        <v>1225</v>
+        <v>1228</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>67616</v>
+        <v>74491</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -849,35 +862,35 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.35476810222432559</v>
+        <v>0.32202547958813815</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.35235197541835489</v>
+        <v>0.31930169389732882</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>9.8348154434645702E-2</v>
+        <v>9.5681412964137416E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.12667666664861615</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.12321248926835178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>18092</v>
+        <v>51003</v>
       </c>
       <c r="C8" s="2">
-        <v>5528</v>
+        <v>5885</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>23620</v>
+        <v>56888</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -887,52 +900,60 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.91143099068585942</v>
+        <v>0.37842778793418647</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.99403051072297144</v>
+        <v>0.35260670940925043</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>8.826242574074758E-2</v>
+        <v>8.5869162009836186E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>9.7386105801253064E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>9.4722925960844626E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" t="str">
+      <c r="B9" s="2">
+        <v>15175</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10763</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1" t="str">
+        <v>25938</v>
+      </c>
+      <c r="E9" s="2">
+        <v>19776</v>
+      </c>
+      <c r="F9" s="2">
+        <v>14140</v>
+      </c>
+      <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J9" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>0.7624334952579227</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.93179571663920924</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="2"/>
+        <v>7.888092474482164E-2</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="3"/>
+        <v>7.4476321902043091E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -962,7 +983,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -992,7 +1013,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -1022,7 +1043,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -1052,7 +1073,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -1082,7 +1103,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -1112,7 +1133,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -1443,7 +1464,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <conditionalFormatting sqref="E2:F26">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -2579,7 +2600,7 @@
   <dimension ref="A1:CX20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+      <selection activeCell="AH12" sqref="AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5798,16 +5819,16 @@
         <v>14</v>
       </c>
       <c r="AD12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AE12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AF12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AG12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AH12" t="s">
         <v>20</v>
@@ -6075,24 +6096,47 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6109,47 +6153,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 day 9 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765BF4B2-ECBE-4D83-A5BE-519C25155D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6965DB9-D443-4039-8FEC-C4A8E23BD643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6252" yWindow="1002" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6252" yWindow="1002" windowWidth="16788" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -652,14 +652,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>189859</v>
+        <v>194425</v>
       </c>
       <c r="C2" s="2">
-        <v>60848</v>
+        <v>62098</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>250707</v>
+        <v>256523</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -669,19 +669,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>0.10168443641382172</v>
+        <v>9.9379003052357875E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>0.10828035542165501</v>
+        <v>0.10573743088594574</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>0.10168443641382172</v>
+        <v>9.9379003052357875E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>0.10828035542165501</v>
+        <v>0.10573743088594574</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -690,14 +690,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>157457</v>
+        <v>161961</v>
       </c>
       <c r="C3" s="2">
-        <v>7133</v>
+        <v>7295</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>164590</v>
+        <v>169256</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -707,19 +707,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.17897199100795916</v>
+        <v>0.17403814340407431</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.18802593724000838</v>
+        <v>0.18279709312735781</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.11749572209790712</v>
+        <v>0.11483180845382285</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.15593677413238244</v>
+        <v>0.15227465603703227</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -728,14 +728,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>102369</v>
+        <v>105706</v>
       </c>
       <c r="C4" s="2">
-        <v>15263</v>
+        <v>15797</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>117632</v>
+        <v>121503</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -745,19 +745,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.55476400979325358</v>
+        <v>0.53708961918635756</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.55688733894049958</v>
+        <v>0.53930713488354498</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.26029588324219111</v>
+        <v>0.25439434280746753</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.30026493345061334</v>
+        <v>0.29321332133213324</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -769,14 +769,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>99971</v>
+        <v>103579</v>
       </c>
       <c r="C5" s="2">
-        <v>13504</v>
+        <v>13996</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>113475</v>
+        <v>117575</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -786,19 +786,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.30067415730337077</v>
+        <v>0.29018924091005743</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.26294625441378</v>
+        <v>0.25378696453914401</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.13609113427227801</v>
+        <v>0.13300561743001602</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.13845538004519142</v>
+        <v>0.13520380609489521</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -807,14 +807,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>58165</v>
+        <v>61307</v>
       </c>
       <c r="C6" s="2">
-        <v>24323</v>
+        <v>24885</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>82488</v>
+        <v>86192</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -824,19 +824,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.26942100669188246</v>
+        <v>0.25784295526266937</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.25960629244390959</v>
+        <v>0.24630140114505686</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>8.8645311060321405E-2</v>
+        <v>8.6635506367850057E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>7.9532705850130891E-2</v>
+        <v>7.7664909348077668E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -845,14 +845,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>73263</v>
+        <v>77568</v>
       </c>
       <c r="C7" s="2">
-        <v>1228</v>
+        <v>1273</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>74491</v>
+        <v>78841</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -862,19 +862,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.32202547958813815</v>
+        <v>0.30425793686026303</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.31930169389732882</v>
+        <v>0.301580548679868</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>9.5681412964137416E-2</v>
+        <v>9.3512082737220448E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.12321248926835178</v>
+        <v>0.12031888903176031</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -883,14 +883,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>51003</v>
+        <v>57934</v>
       </c>
       <c r="C8" s="2">
-        <v>5885</v>
+        <v>5647</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>56888</v>
+        <v>63581</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -900,19 +900,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.37842778793418647</v>
+        <v>0.33859171765149965</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.35260670940925043</v>
+        <v>0.31042220457762282</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>8.5869162009836186E-2</v>
+        <v>8.3922299364969227E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>9.4722925960844626E-2</v>
+        <v>9.2498392696412496E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -921,14 +921,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>15175</v>
+        <v>46429</v>
       </c>
       <c r="C9" s="2">
-        <v>10763</v>
+        <v>11811</v>
       </c>
       <c r="D9">
-        <f t="shared" si="5"/>
-        <v>25938</v>
+        <f>IF(ISBLANK(B9),"",B9+C9)</f>
+        <v>58240</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -938,19 +938,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.7624334952579227</v>
+        <v>0.33956043956043958</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="1"/>
-        <v>0.93179571663920924</v>
+        <f>IF(ISBLANK(C9),"",F9/B9)</f>
+        <v>0.30455103491352387</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>7.888092474482164E-2</v>
+        <v>7.7092502426682988E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>7.4476321902043091E-2</v>
+        <v>7.2727272727272724E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -958,29 +958,37 @@
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="1" t="str">
+      <c r="B10" s="2">
+        <v>19558</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1121</v>
+      </c>
+      <c r="D10">
+        <f>IF(ISBLANK(B10),"",B10+C10)</f>
+        <v>20679</v>
+      </c>
+      <c r="E10" s="2">
+        <v>19396</v>
+      </c>
+      <c r="F10" s="2">
+        <v>19037</v>
+      </c>
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J10" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.93795638086948108</v>
+      </c>
+      <c r="H10" s="1">
+        <f>IF(ISBLANK(C10),"",F10/B10)</f>
+        <v>0.97336128438490643</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>7.5611153775684836E-2</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="3"/>
+        <v>9.7914362864857912E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2599,8 +2607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH12" sqref="AH12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5831,16 +5839,16 @@
         <v>14</v>
       </c>
       <c r="AH12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AI12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AJ12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AK12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AL12" t="s">
         <v>20</v>
@@ -6096,47 +6104,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6153,24 +6138,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 day 10 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6965DB9-D443-4039-8FEC-C4A8E23BD643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA121DF-3A01-467A-8BEF-EFECC8794BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6252" yWindow="1002" windowWidth="16788" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3102" yWindow="270" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -652,14 +652,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>194425</v>
+        <v>198526</v>
       </c>
       <c r="C2" s="2">
-        <v>62098</v>
+        <v>62899</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>256523</v>
+        <v>261425</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -669,19 +669,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>9.9379003052357875E-2</v>
+        <v>9.7515539829779091E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>0.10573743088594574</v>
+        <v>0.10355318698810231</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>9.9379003052357875E-2</v>
+        <v>9.7515539829779091E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>0.10573743088594574</v>
+        <v>0.10355318698810231</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -690,14 +690,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>161961</v>
+        <v>166170</v>
       </c>
       <c r="C3" s="2">
-        <v>7295</v>
+        <v>7497</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>169256</v>
+        <v>173667</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -707,19 +707,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.17403814340407431</v>
+        <v>0.16961771666465131</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.18279709312735781</v>
+        <v>0.17816693747367154</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.11483180845382285</v>
+        <v>0.11267858850530744</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.15227465603703227</v>
+        <v>0.14912908132939767</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -728,14 +728,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>105706</v>
+        <v>109040</v>
       </c>
       <c r="C4" s="2">
-        <v>15797</v>
+        <v>16248</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>121503</v>
+        <v>125288</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -745,19 +745,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.53708961918635756</v>
+        <v>0.52086392950641724</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.53930713488354498</v>
+        <v>0.52281731474688187</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.25439434280746753</v>
+        <v>0.24962417519365018</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.29321332133213324</v>
+        <v>0.28715634224232595</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -769,14 +769,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>103579</v>
+        <v>107445</v>
       </c>
       <c r="C5" s="2">
-        <v>13996</v>
+        <v>14295</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>117575</v>
+        <v>121740</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -786,19 +786,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.29018924091005743</v>
+        <v>0.28026121241991131</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.25378696453914401</v>
+        <v>0.24465540509097677</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.13300561743001602</v>
+        <v>0.13051161901118868</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.13520380609489521</v>
+        <v>0.13241086809788138</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -807,14 +807,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>61307</v>
+        <v>64612</v>
       </c>
       <c r="C6" s="2">
-        <v>24885</v>
+        <v>25462</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>86192</v>
+        <v>90074</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -824,19 +824,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.25784295526266937</v>
+        <v>0.24673046606123852</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.24630140114505686</v>
+        <v>0.23370271776140655</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>8.6635506367850057E-2</v>
+        <v>8.5010997417997516E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>7.7664909348077668E-2</v>
+        <v>7.6060566374177685E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -845,14 +845,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>77568</v>
+        <v>81794</v>
       </c>
       <c r="C7" s="2">
-        <v>1273</v>
+        <v>1346</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>78841</v>
+        <v>83140</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -862,19 +862,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.30425793686026303</v>
+        <v>0.28852537887899926</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.301580548679868</v>
+        <v>0.28599897302980659</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>9.3512082737220448E-2</v>
+        <v>9.1758630582385009E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.12031888903176031</v>
+        <v>0.11783343239676415</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -883,14 +883,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>57934</v>
+        <v>62799</v>
       </c>
       <c r="C8" s="2">
-        <v>5647</v>
+        <v>5664</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>63581</v>
+        <v>68463</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -900,19 +900,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.33859171765149965</v>
+        <v>0.31444721966609701</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.31042220457762282</v>
+        <v>0.28637398684692433</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>8.3922299364969227E-2</v>
+        <v>8.234866596538204E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>9.2498392696412496E-2</v>
+        <v>9.0587630839285532E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -921,14 +921,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>46429</v>
+        <v>54013</v>
       </c>
       <c r="C9" s="2">
-        <v>11811</v>
+        <v>11460</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>58240</v>
+        <v>65473</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -938,19 +938,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.33956043956043958</v>
+        <v>0.30204817252913413</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.30455103491352387</v>
+        <v>0.26178882861533337</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>7.7092502426682988E-2</v>
+        <v>7.5646935067418958E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>7.2727272727272724E-2</v>
+        <v>7.1224927717276329E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -959,14 +959,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>19558</v>
+        <v>50297</v>
       </c>
       <c r="C10" s="2">
-        <v>1121</v>
+        <v>780</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>20679</v>
+        <v>51077</v>
       </c>
       <c r="E10" s="2">
         <v>19396</v>
@@ -976,19 +976,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.93795638086948108</v>
+        <v>0.37974039195724102</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.97336128438490643</v>
+        <v>0.37849175895182613</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>7.5611153775684836E-2</v>
+        <v>7.4193363297312812E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>9.7914362864857912E-2</v>
+        <v>9.5891721991074222E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -996,29 +996,37 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" t="str">
+      <c r="B11" s="2">
+        <v>12121</v>
+      </c>
+      <c r="C11" s="2">
+        <v>12946</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="1" t="str">
+        <v>25067</v>
+      </c>
+      <c r="E11" s="2">
+        <v>15272</v>
+      </c>
+      <c r="F11" s="2">
+        <v>11642</v>
+      </c>
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J11" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.60924721745721466</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.96048180843164754</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8418284402792391E-2</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="3"/>
+        <v>5.8642192962130905E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2607,8 +2615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL12" sqref="AL12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AP12" sqref="AP12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5851,16 +5859,16 @@
         <v>14</v>
       </c>
       <c r="AL12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AM12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AN12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AO12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AP12" t="s">
         <v>20</v>
@@ -6104,24 +6112,47 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6138,47 +6169,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 day 11 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA121DF-3A01-467A-8BEF-EFECC8794BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5382B783-B786-4B0C-A20D-9AD2729A10EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3102" yWindow="270" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -602,7 +602,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -652,14 +652,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>198526</v>
+        <v>200872</v>
       </c>
       <c r="C2" s="2">
-        <v>62899</v>
+        <v>63434</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>261425</v>
+        <v>264306</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -669,19 +669,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>9.7515539829779091E-2</v>
+        <v>9.6452596611503336E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>0.10355318698810231</v>
+        <v>0.10234378111434148</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>9.7515539829779091E-2</v>
+        <v>9.6452596611503336E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>0.10355318698810231</v>
+        <v>0.10234378111434148</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -690,14 +690,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>166170</v>
+        <v>168562</v>
       </c>
       <c r="C3" s="2">
-        <v>7497</v>
+        <v>7606</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>173667</v>
+        <v>176168</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -707,19 +707,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.16961771666465131</v>
+        <v>0.16720970891421824</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.17816693747367154</v>
+        <v>0.17563863741531305</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.11267858850530744</v>
+        <v>0.11145036435041203</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.14912908132939767</v>
+        <v>0.14738739097534748</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -728,14 +728,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>109040</v>
+        <v>110983</v>
       </c>
       <c r="C4" s="2">
-        <v>16248</v>
+        <v>16491</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>125288</v>
+        <v>127474</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -745,19 +745,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.52086392950641724</v>
+        <v>0.51193184492523969</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.52281731474688187</v>
+        <v>0.51366425488588341</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.24962417519365018</v>
+        <v>0.24690321067247811</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.28715634224232595</v>
+        <v>0.28380262057429606</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -769,14 +769,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>107445</v>
+        <v>109681</v>
       </c>
       <c r="C5" s="2">
-        <v>14295</v>
+        <v>14455</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>121740</v>
+        <v>124136</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -786,19 +786,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.28026121241991131</v>
+        <v>0.27485177547206291</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.24465540509097677</v>
+        <v>0.23966776378771162</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.13051161901118868</v>
+        <v>0.12908901046514268</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.13241086809788138</v>
+        <v>0.13086443108048906</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -807,14 +807,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>64612</v>
+        <v>66368</v>
       </c>
       <c r="C6" s="2">
-        <v>25462</v>
+        <v>25819</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>90074</v>
+        <v>92187</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -824,19 +824,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.24673046606123852</v>
+        <v>0.24107520583162484</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.23370271776140655</v>
+        <v>0.22751928640308583</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>8.5010997417997516E-2</v>
+        <v>8.4084356768291305E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>7.6060566374177685E-2</v>
+        <v>7.5172248994384488E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -845,14 +845,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>81794</v>
+        <v>84067</v>
       </c>
       <c r="C7" s="2">
-        <v>1346</v>
+        <v>1354</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>83140</v>
+        <v>85421</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -862,19 +862,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.28852537887899926</v>
+        <v>0.28082087542875872</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.28599897302980659</v>
+        <v>0.27826614486064688</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>9.1758630582385009E-2</v>
+        <v>9.0758439081973161E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.11783343239676415</v>
+        <v>0.11645724640567127</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -883,14 +883,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>62799</v>
+        <v>65148</v>
       </c>
       <c r="C8" s="2">
-        <v>5664</v>
+        <v>5769</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>68463</v>
+        <v>70917</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -900,19 +900,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.31444721966609701</v>
+        <v>0.30356614069969118</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.28637398684692433</v>
+        <v>0.27604838214526922</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>8.234866596538204E-2</v>
+        <v>8.1451045379219544E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>9.0587630839285532E-2</v>
+        <v>8.9529650722848381E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -921,14 +921,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>54013</v>
+        <v>56966</v>
       </c>
       <c r="C9" s="2">
-        <v>11460</v>
+        <v>11567</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>65473</v>
+        <v>68533</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -938,19 +938,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.30204817252913413</v>
+        <v>0.28856171479433268</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.26178882861533337</v>
+        <v>0.24821823543868271</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>7.5646935067418958E-2</v>
+        <v>7.4822364986038906E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>7.1224927717276329E-2</v>
+        <v>7.0393086144410366E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -959,14 +959,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>50297</v>
+        <v>55206</v>
       </c>
       <c r="C10" s="2">
-        <v>780</v>
+        <v>746</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>51077</v>
+        <v>55952</v>
       </c>
       <c r="E10" s="2">
         <v>19396</v>
@@ -976,19 +976,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.37974039195724102</v>
+        <v>0.34665427509293678</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.37849175895182613</v>
+        <v>0.34483570626381188</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>7.4193363297312812E-2</v>
+        <v>7.3384637503499731E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>9.5891721991074222E-2</v>
+        <v>9.4771794973913734E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -997,14 +997,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>12121</v>
+        <v>28621</v>
       </c>
       <c r="C11" s="2">
-        <v>12946</v>
+        <v>14324</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>25067</v>
+        <v>42945</v>
       </c>
       <c r="E11" s="2">
         <v>15272</v>
@@ -1014,19 +1014,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.60924721745721466</v>
+        <v>0.35561765048317617</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.96048180843164754</v>
+        <v>0.40676426400195659</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>5.8418284402792391E-2</v>
+        <v>5.7781510824574549E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>5.8642192962130905E-2</v>
+        <v>5.7957306145206895E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1034,29 +1034,37 @@
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" t="str">
+      <c r="B12" s="2">
+        <v>12059</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1978</v>
+      </c>
+      <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v/>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1" t="str">
+        <v>14037</v>
+      </c>
+      <c r="E12" s="2">
+        <v>12710</v>
+      </c>
+      <c r="F12" s="2">
+        <v>11612</v>
+      </c>
+      <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v/>
-      </c>
-      <c r="H12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J12" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.90546413051221775</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.96293224977195457</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="2"/>
+        <v>4.8088200797560404E-2</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="3"/>
+        <v>5.7807957306145206E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2616,7 +2624,7 @@
   <dimension ref="A1:CX20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AP12" sqref="AP12"/>
+      <selection activeCell="AT12" sqref="AT12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5871,16 +5879,16 @@
         <v>16</v>
       </c>
       <c r="AP12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AQ12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AR12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AS12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AT12" t="s">
         <v>20</v>
@@ -6112,47 +6120,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6169,24 +6154,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 day 13 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5382B783-B786-4B0C-A20D-9AD2729A10EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581D009A-37FC-4E0E-AF9F-72D15F1C5D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3102" yWindow="270" windowWidth="16788" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1938" yWindow="402" windowWidth="11418" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="31">
   <si>
     <t>Day</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Hillwalking</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2623,8 +2626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AT12" sqref="AT12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="BB12" sqref="BB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5891,28 +5894,28 @@
         <v>14</v>
       </c>
       <c r="AT12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AU12" t="s">
         <v>20</v>
       </c>
       <c r="AV12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AW12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="AX12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AY12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="AZ12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BA12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BB12" t="s">
         <v>20</v>
@@ -6120,24 +6123,47 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6154,47 +6180,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 day 16 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581D009A-37FC-4E0E-AF9F-72D15F1C5D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DD70DF-7947-460B-B509-CE19EFEC2E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1938" yWindow="402" windowWidth="11418" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8820" yWindow="756" windowWidth="11418" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -605,7 +605,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -655,14 +655,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>200872</v>
+        <v>212682</v>
       </c>
       <c r="C2" s="2">
-        <v>63434</v>
+        <v>67750</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>264306</v>
+        <v>280432</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -672,19 +672,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>9.6452596611503336E-2</v>
+        <v>9.0906173332572601E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>0.10234378111434148</v>
+        <v>9.6660742328922994E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>9.6452596611503336E-2</v>
+        <v>9.0906173332572601E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>0.10234378111434148</v>
+        <v>9.6660742328922994E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -693,14 +693,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>168562</v>
+        <v>179446</v>
       </c>
       <c r="C3" s="2">
-        <v>7606</v>
+        <v>9284</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>176168</v>
+        <v>188730</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -710,19 +710,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.16720970891421824</v>
+        <v>0.15608011444921316</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.17563863741531305</v>
+        <v>0.16498556668858599</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.11145036435041203</v>
+        <v>0.10504150738860045</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.14738739097534748</v>
+        <v>0.13920312955492237</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -731,14 +731,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>110983</v>
+        <v>118633</v>
       </c>
       <c r="C4" s="2">
-        <v>16491</v>
+        <v>17787</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>127474</v>
+        <v>136420</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -748,19 +748,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.51193184492523969</v>
+        <v>0.4783609441430875</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.51366425488588341</v>
+        <v>0.48054082759434558</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.24690321067247811</v>
+        <v>0.23270525474981457</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.28380262057429606</v>
+        <v>0.26804336991376798</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -772,14 +772,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>109681</v>
+        <v>117910</v>
       </c>
       <c r="C5" s="2">
-        <v>14455</v>
+        <v>15825</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>124136</v>
+        <v>133735</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -789,19 +789,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.27485177547206291</v>
+        <v>0.25512393913336073</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.23966776378771162</v>
+        <v>0.22294122635908745</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.12908901046514268</v>
+        <v>0.1216658583899127</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.13086443108048906</v>
+        <v>0.12359767164122963</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -810,14 +810,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>66368</v>
+        <v>72000</v>
       </c>
       <c r="C6" s="2">
-        <v>25819</v>
+        <v>27881</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>92187</v>
+        <v>99881</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -827,19 +827,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.24107520583162484</v>
+        <v>0.22250478068901994</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.22751928640308583</v>
+        <v>0.20972222222222223</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>8.4084356768291305E-2</v>
+        <v>7.9249158441262055E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>7.5172248994384488E-2</v>
+        <v>7.0998015817041404E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -848,14 +848,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>84067</v>
+        <v>92201</v>
       </c>
       <c r="C7" s="2">
-        <v>1354</v>
+        <v>1508</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>85421</v>
+        <v>93709</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -865,19 +865,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.28082087542875872</v>
+        <v>0.25598395031427079</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.27826614486064688</v>
+        <v>0.25371742171993794</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>9.0758439081973161E-2</v>
+        <v>8.5539453414731556E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.11645724640567127</v>
+        <v>0.10999050225218872</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -886,14 +886,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>65148</v>
+        <v>72397</v>
       </c>
       <c r="C8" s="2">
-        <v>5769</v>
+        <v>6385</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>70917</v>
+        <v>78782</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -903,19 +903,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.30356614069969118</v>
+        <v>0.27326038942905739</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.27604838214526922</v>
+        <v>0.24840808320786772</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>8.1451045379219544E-2</v>
+        <v>7.6767273349689052E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>8.9529650722848381E-2</v>
+        <v>8.4558166652561106E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -924,14 +924,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>56966</v>
+        <v>64928</v>
       </c>
       <c r="C9" s="2">
-        <v>11567</v>
+        <v>12779</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>68533</v>
+        <v>77707</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -941,19 +941,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.28856171479433268</v>
+        <v>0.25449444708970875</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.24821823543868271</v>
+        <v>0.21777969443075407</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>7.4822364986038906E-2</v>
+        <v>7.0519769498488052E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>7.0393086144410366E-2</v>
+        <v>6.6484234679004342E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -962,14 +962,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>55206</v>
+        <v>66048</v>
       </c>
       <c r="C10" s="2">
-        <v>746</v>
+        <v>952</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>55952</v>
+        <v>67000</v>
       </c>
       <c r="E10" s="2">
         <v>19396</v>
@@ -979,19 +979,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.34665427509293678</v>
+        <v>0.28949253731343283</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.34483570626381188</v>
+        <v>0.28822977228682173</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>7.3384637503499731E-2</v>
+        <v>6.9164717293318884E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>9.4771794973913734E-2</v>
+        <v>8.9509220338345505E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1000,14 +1000,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>28621</v>
+        <v>40681</v>
       </c>
       <c r="C11" s="2">
-        <v>14324</v>
+        <v>14915</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>42945</v>
+        <v>55596</v>
       </c>
       <c r="E11" s="2">
         <v>15272</v>
@@ -1017,19 +1017,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.35561765048317617</v>
+        <v>0.27469602129649617</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.40676426400195659</v>
+        <v>0.28617782257073326</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>5.7781510824574549E-2</v>
+        <v>5.4458834940377704E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>5.7957306145206895E-2</v>
+        <v>5.473900000940371E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1038,14 +1038,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>12059</v>
+        <v>47987</v>
       </c>
       <c r="C12" s="2">
-        <v>1978</v>
+        <v>1972</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>14037</v>
+        <v>49959</v>
       </c>
       <c r="E12" s="2">
         <v>12710</v>
@@ -1055,19 +1055,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.90546413051221775</v>
+        <v>0.25440861506435275</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.96293224977195457</v>
+        <v>0.24198220351345157</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>4.8088200797560404E-2</v>
+        <v>4.5322930336052947E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>5.7807957306145206E-2</v>
+        <v>5.459794434884005E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1075,29 +1075,38 @@
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" t="str">
+      <c r="B13" s="2">
+        <v>23952</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12930</v>
+      </c>
+      <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v/>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="1" t="str">
+        <v>36882</v>
+      </c>
+      <c r="E13" s="2">
+        <v>15031</v>
+      </c>
+      <c r="F13" s="2">
+        <f>D2</f>
+        <v>280432</v>
+      </c>
+      <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v/>
-      </c>
-      <c r="H13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J13" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.4075429748929017</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>11.70808283233133</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
+        <v>5.3599446568151993E-2</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="3"/>
+        <v>1.318550700106262</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1105,29 +1114,37 @@
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" t="str">
+      <c r="B14" s="2">
+        <v>29616</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4334</v>
+      </c>
+      <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v/>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1" t="str">
+        <v>33950</v>
+      </c>
+      <c r="E14" s="2">
+        <v>17633</v>
+      </c>
+      <c r="F14" s="2">
+        <v>18289</v>
+      </c>
+      <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J14" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.51938144329896907</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.61753781739600211</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="2"/>
+        <v>6.2877988246705083E-2</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="3"/>
+        <v>8.5992232534958288E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1135,29 +1152,38 @@
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" t="str">
+      <c r="B15" s="2">
+        <v>27084</v>
+      </c>
+      <c r="C15" s="2">
+        <v>6053</v>
+      </c>
+      <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v/>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1" t="str">
+        <v>33137</v>
+      </c>
+      <c r="E15" s="2">
+        <v>10753</v>
+      </c>
+      <c r="F15" s="2">
+        <f>D2</f>
+        <v>280432</v>
+      </c>
+      <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J15" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.32450131273199145</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>10.35415743612465</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="2"/>
+        <v>3.8344411479431732E-2</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="3"/>
+        <v>1.318550700106262</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1165,29 +1191,37 @@
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" t="str">
+      <c r="B16" s="2">
+        <v>28691</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3659</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1" t="str">
+        <v>32350</v>
+      </c>
+      <c r="E16" s="2">
+        <v>13047</v>
+      </c>
+      <c r="F16" s="2">
+        <v>24040</v>
+      </c>
+      <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J16" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.40330757341576506</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.83789341605381473</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="2"/>
+        <v>4.6524647686426654E-2</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11303260266501161</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1195,29 +1229,37 @@
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" t="str">
+      <c r="B17" s="2">
+        <v>9200</v>
+      </c>
+      <c r="C17" s="2">
+        <v>971</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1" t="str">
+        <v>10171</v>
+      </c>
+      <c r="E17" s="2">
+        <v>9676</v>
+      </c>
+      <c r="F17" s="2">
+        <v>9129</v>
+      </c>
+      <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J17" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.95133221905417364</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.99228260869565221</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4503908255833854E-2</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="3"/>
+        <v>4.2923237509521255E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2626,8 +2668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="BB12" sqref="BB12"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="BN12" sqref="BN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5918,40 +5960,40 @@
         <v>14</v>
       </c>
       <c r="BB12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BC12" t="s">
         <v>20</v>
       </c>
       <c r="BD12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BE12" t="s">
         <v>20</v>
       </c>
       <c r="BF12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BG12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BH12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BI12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BJ12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BK12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BL12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BM12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BN12" t="s">
         <v>20</v>
@@ -6123,47 +6165,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6180,24 +6199,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 day 17 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DD70DF-7947-460B-B509-CE19EFEC2E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A72992B-FEE6-405B-936E-12AA102A4987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8820" yWindow="756" windowWidth="11418" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,7 +605,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -655,14 +655,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>212682</v>
+        <v>214467</v>
       </c>
       <c r="C2" s="2">
-        <v>67750</v>
+        <v>68264</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>280432</v>
+        <v>282731</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -672,19 +672,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>9.0906173332572601E-2</v>
+        <v>9.0166978506071138E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>9.6660742328922994E-2</v>
+        <v>9.5856238955177253E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>9.0906173332572601E-2</v>
+        <v>9.0166978506071138E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>9.6660742328922994E-2</v>
+        <v>9.5856238955177253E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -693,14 +693,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>179446</v>
+        <v>181154</v>
       </c>
       <c r="C3" s="2">
-        <v>9284</v>
+        <v>8390</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>188730</v>
+        <v>189544</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -710,19 +710,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.15608011444921316</v>
+        <v>0.15540982568691175</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.16498556668858599</v>
+        <v>0.16343000982589398</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.10504150738860045</v>
+        <v>0.10418737244943073</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.13920312955492237</v>
+        <v>0.13804454764602481</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -731,14 +731,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>118633</v>
+        <v>119803</v>
       </c>
       <c r="C4" s="2">
-        <v>17787</v>
+        <v>17983</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>136420</v>
+        <v>137786</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -748,19 +748,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.4783609441430875</v>
+        <v>0.4736185098631211</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.48054082759434558</v>
+        <v>0.47584785022077913</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.23270525474981457</v>
+        <v>0.2308130342976186</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.26804336991376798</v>
+        <v>0.26581245599556108</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -772,14 +772,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>117910</v>
+        <v>119182</v>
       </c>
       <c r="C5" s="2">
-        <v>15825</v>
+        <v>16002</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>133735</v>
+        <v>135184</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -789,19 +789,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.25512393913336073</v>
+        <v>0.25238933601609659</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.22294122635908745</v>
+        <v>0.2205618298065144</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.1216658583899127</v>
+        <v>0.12067654413559178</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.12359767164122963</v>
+        <v>0.12256897331524197</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -810,14 +810,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>72000</v>
+        <v>72911</v>
       </c>
       <c r="C6" s="2">
-        <v>27881</v>
+        <v>28205</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>99881</v>
+        <v>101116</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -827,19 +827,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.22250478068901994</v>
+        <v>0.21978717512559831</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.20972222222222223</v>
+        <v>0.20710180905487513</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>7.9249158441262055E-2</v>
+        <v>7.8604751512922177E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>7.0998015817041404E-2</v>
+        <v>7.0407102258156273E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -848,14 +848,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>92201</v>
+        <v>93439</v>
       </c>
       <c r="C7" s="2">
-        <v>1508</v>
+        <v>1550</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>93709</v>
+        <v>94989</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -865,19 +865,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.25598395031427079</v>
+        <v>0.25253450399519944</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.25371742171993794</v>
+        <v>0.2503558471302133</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>8.5539453414731556E-2</v>
+        <v>8.4843897556334466E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.10999050225218872</v>
+        <v>0.109075055836096</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -886,14 +886,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>72397</v>
+        <v>73517</v>
       </c>
       <c r="C8" s="2">
-        <v>6385</v>
+        <v>6477</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>78782</v>
+        <v>79994</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -903,19 +903,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.27326038942905739</v>
+        <v>0.26912018401380106</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.24840808320786772</v>
+        <v>0.2446236924792905</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>7.6767273349689052E-2</v>
+        <v>7.614304763184794E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>8.4558166652561106E-2</v>
+        <v>8.3854392517263732E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -924,14 +924,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>64928</v>
+        <v>66006</v>
       </c>
       <c r="C9" s="2">
-        <v>12779</v>
+        <v>12991</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>77707</v>
+        <v>78997</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -941,19 +941,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.25449444708970875</v>
+        <v>0.25033862045394129</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.21777969443075407</v>
+        <v>0.21422294942883979</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>7.0519769498488052E-2</v>
+        <v>6.9946344758799003E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>6.6484234679004342E-2</v>
+        <v>6.5930889134458909E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -962,14 +962,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>66048</v>
+        <v>67273</v>
       </c>
       <c r="C10" s="2">
-        <v>952</v>
+        <v>989</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>67000</v>
+        <v>68262</v>
       </c>
       <c r="E10" s="2">
         <v>19396</v>
@@ -979,19 +979,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.28949253731343283</v>
+        <v>0.28414051741818286</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.28822977228682173</v>
+        <v>0.28298128521100591</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.9164717293318884E-2</v>
+        <v>6.8602311030626278E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>8.9509220338345505E-2</v>
+        <v>8.8764238787319261E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1000,14 +1000,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>40681</v>
+        <v>41784</v>
       </c>
       <c r="C11" s="2">
-        <v>14915</v>
+        <v>15136</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>55596</v>
+        <v>56920</v>
       </c>
       <c r="E11" s="2">
         <v>15272</v>
@@ -1017,19 +1017,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.27469602129649617</v>
+        <v>0.26830639494026703</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.28617782257073326</v>
+        <v>0.27862339651541262</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>5.4458834940377704E-2</v>
+        <v>5.4016008149088711E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>5.473900000940371E-2</v>
+        <v>5.4283409568838099E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1038,14 +1038,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>47987</v>
+        <v>49389</v>
       </c>
       <c r="C12" s="2">
-        <v>1972</v>
+        <v>2050</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>49959</v>
+        <v>51439</v>
       </c>
       <c r="E12" s="2">
         <v>12710</v>
@@ -1055,19 +1055,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.25440861506435275</v>
+        <v>0.24708878477419857</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.24198220351345157</v>
+        <v>0.23511308186033328</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>4.5322930336052947E-2</v>
+        <v>4.4954391276513718E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>5.459794434884005E-2</v>
+        <v>5.4143527908722552E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1076,37 +1076,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>23952</v>
+        <v>25252</v>
       </c>
       <c r="C13" s="2">
-        <v>12930</v>
+        <v>13087</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>36882</v>
+        <v>38339</v>
       </c>
       <c r="E13" s="2">
         <v>15031</v>
       </c>
       <c r="F13" s="2">
         <f>D2</f>
-        <v>280432</v>
+        <v>282731</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.4075429748929017</v>
+        <v>0.39205508750880302</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>11.70808283233133</v>
+        <v>11.196380484714082</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>5.3599446568151993E-2</v>
+        <v>5.3163607810958122E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>1.318550700106262</v>
+        <v>1.3182960548709126</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1115,14 +1115,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>29616</v>
+        <v>31306</v>
       </c>
       <c r="C14" s="2">
-        <v>4334</v>
+        <v>4423</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>33950</v>
+        <v>35729</v>
       </c>
       <c r="E14" s="2">
         <v>17633</v>
@@ -1132,19 +1132,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.51938144329896907</v>
+        <v>0.4935206694841725</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.61753781739600211</v>
+        <v>0.58420111160799848</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>6.2877988246705083E-2</v>
+        <v>6.2366701918077611E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>8.5992232534958288E-2</v>
+        <v>8.5276522728438414E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1153,37 +1153,37 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>27084</v>
+        <v>29157</v>
       </c>
       <c r="C15" s="2">
-        <v>6053</v>
+        <v>6197</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>33137</v>
+        <v>35354</v>
       </c>
       <c r="E15" s="2">
         <v>10753</v>
       </c>
       <c r="F15" s="2">
         <f>D2</f>
-        <v>280432</v>
+        <v>282731</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.32450131273199145</v>
+        <v>0.30415228828421115</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>10.35415743612465</v>
+        <v>9.696848098226841</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>3.8344411479431732E-2</v>
+        <v>3.8032617576424232E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>1.318550700106262</v>
+        <v>1.3182960548709126</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1192,14 +1192,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>28691</v>
+        <v>32013</v>
       </c>
       <c r="C16" s="2">
-        <v>3659</v>
+        <v>3471</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>32350</v>
+        <v>35484</v>
       </c>
       <c r="E16" s="2">
         <v>13047</v>
@@ -1209,19 +1209,19 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>0.40330757341576506</v>
+        <v>0.36768684477510993</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.83789341605381473</v>
+        <v>0.75094492862274698</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>4.6524647686426654E-2</v>
+        <v>4.6146336977551099E-2</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>0.11303260266501161</v>
+        <v>0.11209183697258786</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1230,14 +1230,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>9200</v>
+        <v>24889</v>
       </c>
       <c r="C17" s="2">
-        <v>971</v>
+        <v>915</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>10171</v>
+        <v>25804</v>
       </c>
       <c r="E17" s="2">
         <v>9676</v>
@@ -1247,19 +1247,19 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v>0.95133221905417364</v>
+        <v>0.37498062315920011</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0.99228260869565221</v>
+        <v>0.3667885411225843</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>3.4503908255833854E-2</v>
+        <v>3.4223343036313671E-2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>4.2923237509521255E-2</v>
+        <v>4.2565989173159506E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1267,29 +1267,37 @@
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" t="str">
+      <c r="B18" s="2">
+        <v>8085</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1093</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1" t="str">
+        <v>9178</v>
+      </c>
+      <c r="E18" s="2">
+        <v>7106</v>
+      </c>
+      <c r="F18" s="2">
+        <v>7793</v>
+      </c>
+      <c r="G18" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I18" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J18" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.77424275441272605</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.96388373531230676</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="2"/>
+        <v>2.5133430716829778E-2</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="3"/>
+        <v>3.6336592576014022E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -6165,24 +6173,47 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6199,47 +6230,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 Day 18 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A72992B-FEE6-405B-936E-12AA102A4987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4E852B-62B2-4018-B27E-4C9061766900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="756" windowWidth="11418" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4032" yWindow="558" windowWidth="16890" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -655,14 +655,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>214467</v>
+        <v>216683</v>
       </c>
       <c r="C2" s="2">
-        <v>68264</v>
+        <v>69033</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>282731</v>
+        <v>285716</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -672,19 +672,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>9.0166978506071138E-2</v>
+        <v>8.9224964650212096E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>9.5856238955177253E-2</v>
+        <v>9.4875924737981288E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>9.0166978506071138E-2</v>
+        <v>8.9224964650212096E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>9.5856238955177253E-2</v>
+        <v>9.4875924737981288E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -693,14 +693,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>181154</v>
+        <v>183246</v>
       </c>
       <c r="C3" s="2">
-        <v>8390</v>
+        <v>8513</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>189544</v>
+        <v>191759</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -710,19 +710,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.15540982568691175</v>
+        <v>0.15361469344333251</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.16343000982589398</v>
+        <v>0.16156423605426584</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.10418737244943073</v>
+        <v>0.10309888140671156</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.13804454764602481</v>
+        <v>0.13663277691374034</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -731,14 +731,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>119803</v>
+        <v>121230</v>
       </c>
       <c r="C4" s="2">
-        <v>17983</v>
+        <v>18235</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>137786</v>
+        <v>139465</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -748,19 +748,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.4736185098631211</v>
+        <v>0.46791668160470368</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.47584785022077913</v>
+        <v>0.47024663862080346</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.2308130342976186</v>
+        <v>0.22840162959022245</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.26581245599556108</v>
+        <v>0.26309401291287271</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -772,14 +772,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>119182</v>
+        <v>120677</v>
       </c>
       <c r="C5" s="2">
-        <v>16002</v>
+        <v>16233</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>135184</v>
+        <v>136910</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -789,19 +789,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.25238933601609659</v>
+        <v>0.24920750858228033</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.2205618298065144</v>
+        <v>0.21782941239838577</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.12067654413559178</v>
+        <v>0.11941578350529897</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.12256897331524197</v>
+        <v>0.12131547006456436</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -810,14 +810,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>72911</v>
+        <v>73869</v>
       </c>
       <c r="C6" s="2">
-        <v>28205</v>
+        <v>28633</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>101116</v>
+        <v>102502</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -827,19 +827,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.21978717512559831</v>
+        <v>0.21681528165304093</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.20710180905487513</v>
+        <v>0.20441592548971829</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>7.8604751512922177E-2</v>
+        <v>7.7783533298800209E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>7.0407102258156273E-2</v>
+        <v>6.9687054360517434E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -848,14 +848,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>93439</v>
+        <v>94739</v>
       </c>
       <c r="C7" s="2">
-        <v>1550</v>
+        <v>1598</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>94989</v>
+        <v>96337</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -865,19 +865,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.25253450399519944</v>
+        <v>0.24900090307981357</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.2503558471302133</v>
+        <v>0.24692048681113374</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>8.4843897556334466E-2</v>
+        <v>8.3957496255022468E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.109075055836096</v>
+        <v>0.10795955381825062</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -886,14 +886,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>73517</v>
+        <v>74619</v>
       </c>
       <c r="C8" s="2">
-        <v>6477</v>
+        <v>6602</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>79994</v>
+        <v>81221</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -903,19 +903,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.26912018401380106</v>
+        <v>0.26505460410484971</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.2446236924792905</v>
+        <v>0.24101100255966978</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>7.614304763184794E-2</v>
+        <v>7.5347547914712515E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>8.3854392517263732E-2</v>
+        <v>8.2996820239705005E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -924,14 +924,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>66006</v>
+        <v>67172</v>
       </c>
       <c r="C9" s="2">
-        <v>12991</v>
+        <v>13171</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>78997</v>
+        <v>80343</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -941,19 +941,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.25033862045394129</v>
+        <v>0.24614465479257683</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.21422294942883979</v>
+        <v>0.21050437682367654</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>6.9946344758799003E-2</v>
+        <v>6.9215584706491765E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>6.5930889134458909E-2</v>
+        <v>6.5256619116405068E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -962,14 +962,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>67273</v>
+        <v>68619</v>
       </c>
       <c r="C10" s="2">
-        <v>989</v>
+        <v>1027</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>68262</v>
+        <v>69646</v>
       </c>
       <c r="E10" s="2">
         <v>19396</v>
@@ -979,19 +979,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.28414051741818286</v>
+        <v>0.2784940987278523</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.28298128521100591</v>
+        <v>0.27743044929247002</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.8602311030626278E-2</v>
+        <v>6.7885592686443882E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>8.8764238787319261E-2</v>
+        <v>8.7856453898090756E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1000,14 +1000,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>41784</v>
+        <v>42776</v>
       </c>
       <c r="C11" s="2">
-        <v>15136</v>
+        <v>15347</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>56920</v>
+        <v>58123</v>
       </c>
       <c r="E11" s="2">
         <v>15272</v>
@@ -1017,19 +1017,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.26830639494026703</v>
+        <v>0.26275312698931574</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.27862339651541262</v>
+        <v>0.27216195997755749</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>5.4016008149088711E-2</v>
+        <v>5.345167928992426E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>5.4283409568838099E-2</v>
+        <v>5.3728257408287683E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1038,14 +1038,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>49389</v>
+        <v>50683</v>
       </c>
       <c r="C12" s="2">
-        <v>2050</v>
+        <v>2068</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>51439</v>
+        <v>52751</v>
       </c>
       <c r="E12" s="2">
         <v>12710</v>
@@ -1055,19 +1055,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.24708878477419857</v>
+        <v>0.24094329965308714</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.23511308186033328</v>
+        <v>0.22911035258370657</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>4.4954391276513718E-2</v>
+        <v>4.4484733091601447E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>5.4143527908722552E-2</v>
+        <v>5.3589806306909168E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1076,37 +1076,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>25252</v>
+        <v>26250</v>
       </c>
       <c r="C13" s="2">
-        <v>13087</v>
+        <v>13262</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>38339</v>
+        <v>39512</v>
       </c>
       <c r="E13" s="2">
         <v>15031</v>
       </c>
       <c r="F13" s="2">
         <f>D2</f>
-        <v>282731</v>
+        <v>285716</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.39205508750880302</v>
+        <v>0.38041607612877099</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>11.196380484714082</v>
+        <v>10.884419047619048</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>5.3163607810958122E-2</v>
+        <v>5.2608184350893893E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>1.3182960548709126</v>
+        <v>1.3185898293820928</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1115,14 +1115,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>31306</v>
+        <v>32659</v>
       </c>
       <c r="C14" s="2">
-        <v>4423</v>
+        <v>4568</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>35729</v>
+        <v>37227</v>
       </c>
       <c r="E14" s="2">
         <v>17633</v>
@@ -1132,19 +1132,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.4935206694841725</v>
+        <v>0.47366158970639588</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.58420111160799848</v>
+        <v>0.55999877522275632</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>6.2366701918077611E-2</v>
+        <v>6.1715129709221744E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>8.5276522728438414E-2</v>
+        <v>8.44044064370532E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1153,37 +1153,37 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>29157</v>
+        <v>30670</v>
       </c>
       <c r="C15" s="2">
-        <v>6197</v>
+        <v>6480</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>35354</v>
+        <v>37150</v>
       </c>
       <c r="E15" s="2">
         <v>10753</v>
       </c>
       <c r="F15" s="2">
         <f>D2</f>
-        <v>282731</v>
+        <v>285716</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.30415228828421115</v>
+        <v>0.28944818304172276</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>9.696848098226841</v>
+        <v>9.3158134985327674</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>3.8032617576424232E-2</v>
+        <v>3.763527418835487E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>1.3182960548709126</v>
+        <v>1.3185898293820928</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1192,14 +1192,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>32013</v>
+        <v>34024</v>
       </c>
       <c r="C16" s="2">
-        <v>3471</v>
+        <v>3587</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>35484</v>
+        <v>37611</v>
       </c>
       <c r="E16" s="2">
         <v>13047</v>
@@ -1209,19 +1209,19 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>0.36768684477510993</v>
+        <v>0.34689319613942732</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.75094492862274698</v>
+        <v>0.70656007524100639</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>4.6146336977551099E-2</v>
+        <v>4.5664226014643913E-2</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>0.11209183697258786</v>
+        <v>0.11094548257131386</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1230,14 +1230,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>24889</v>
+        <v>28286</v>
       </c>
       <c r="C17" s="2">
-        <v>915</v>
+        <v>876</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>25804</v>
+        <v>29162</v>
       </c>
       <c r="E17" s="2">
         <v>9676</v>
@@ -1247,19 +1247,19 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v>0.37498062315920011</v>
+        <v>0.33180165969412251</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0.3667885411225843</v>
+        <v>0.32273916425086613</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>3.4223343036313671E-2</v>
+        <v>3.3865796805219166E-2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>4.2565989173159506E-2</v>
+        <v>4.2130670149481041E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1268,14 +1268,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>8085</v>
+        <v>16546</v>
       </c>
       <c r="C18" s="2">
-        <v>1093</v>
+        <v>1097</v>
       </c>
       <c r="D18">
         <f t="shared" si="7"/>
-        <v>9178</v>
+        <v>17643</v>
       </c>
       <c r="E18" s="2">
         <v>7106</v>
@@ -1285,19 +1285,19 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="6"/>
-        <v>0.77424275441272605</v>
+        <v>0.40276596950631977</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>0.96388373531230676</v>
+        <v>0.47098996736371329</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="2"/>
-        <v>2.5133430716829778E-2</v>
+        <v>2.4870850774895349E-2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>3.6336592576014022E-2</v>
+        <v>3.596498110142466E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1305,29 +1305,37 @@
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" t="str">
+      <c r="B19" s="2">
+        <v>13234</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5408</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="1" t="str">
+        <v>18642</v>
+      </c>
+      <c r="E19" s="2">
+        <v>12762</v>
+      </c>
+      <c r="F19" s="2">
+        <v>10338</v>
+      </c>
+      <c r="G19" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I19" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J19" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.68458319922755073</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78116971437207194</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="2"/>
+        <v>4.4666731999608002E-2</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="3"/>
+        <v>4.7710249535035054E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2676,8 +2684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX20"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="BN12" sqref="BN12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AY24" sqref="AY24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6004,28 +6012,28 @@
         <v>14</v>
       </c>
       <c r="BN12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BO12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BP12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BQ12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="BR12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BS12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BT12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BU12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BV12" t="s">
         <v>20</v>
@@ -6173,47 +6181,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6230,24 +6215,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 Day 19 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4E852B-62B2-4018-B27E-4C9061766900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC08BF5-7D0E-4ABC-84A8-559229ABB0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4032" yWindow="558" windowWidth="16890" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3666" yWindow="480" windowWidth="16890" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -655,14 +655,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>216683</v>
+        <v>218012</v>
       </c>
       <c r="C2" s="2">
-        <v>69033</v>
+        <v>69648</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>285716</v>
+        <v>287660</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -672,19 +672,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>8.9224964650212096E-2</v>
+        <v>8.862198428700549E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>9.4875924737981288E-2</v>
+        <v>9.4297561602113639E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>8.9224964650212096E-2</v>
+        <v>8.862198428700549E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>9.4875924737981288E-2</v>
+        <v>9.4297561602113639E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -693,14 +693,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>183246</v>
+        <v>184421</v>
       </c>
       <c r="C3" s="2">
-        <v>8513</v>
+        <v>8581</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>191759</v>
+        <v>193002</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -710,19 +710,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.15361469344333251</v>
+        <v>0.15262536139521871</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.16156423605426584</v>
+        <v>0.16053486316634222</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.10309888140671156</v>
+        <v>0.10240214141695057</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.13663277691374034</v>
+        <v>0.13579986422765719</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -731,14 +731,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>121230</v>
+        <v>122034</v>
       </c>
       <c r="C4" s="2">
-        <v>18235</v>
+        <v>18399</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>139465</v>
+        <v>140433</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -748,19 +748,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.46791668160470368</v>
+        <v>0.46469134747530849</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.47024663862080346</v>
+        <v>0.46714849959847254</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.22840162959022245</v>
+        <v>0.22685809636376278</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.26309401291287271</v>
+        <v>0.26149019320037431</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -772,14 +772,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>120677</v>
+        <v>121528</v>
       </c>
       <c r="C5" s="2">
-        <v>16233</v>
+        <v>16361</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>136910</v>
+        <v>137889</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -789,19 +789,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.24920750858228033</v>
+        <v>0.24743815677827818</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.21782941239838577</v>
+        <v>0.2163040616154302</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.11941578350529897</v>
+        <v>0.11860877424737537</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.12131547006456436</v>
+        <v>0.1205759316000954</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -810,14 +810,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>73869</v>
+        <v>74406</v>
       </c>
       <c r="C6" s="2">
-        <v>28633</v>
+        <v>28865</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>102502</v>
+        <v>103271</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -827,19 +827,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.21681528165304093</v>
+        <v>0.21520078240745225</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.20441592548971829</v>
+        <v>0.20294062306803215</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>7.7783533298800209E-2</v>
+        <v>7.7257873878884789E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>6.9687054360517434E-2</v>
+        <v>6.9262242445369979E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -848,14 +848,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>94739</v>
+        <v>95486</v>
       </c>
       <c r="C7" s="2">
-        <v>1598</v>
+        <v>1614</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>96337</v>
+        <v>97100</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -865,19 +865,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.24900090307981357</v>
+        <v>0.24704428424304839</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.24692048681113374</v>
+        <v>0.24498879416877867</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>8.3957496255022468E-2</v>
+        <v>8.3390113328234719E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.10795955381825062</v>
+        <v>0.10730143294864503</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -886,14 +886,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>74619</v>
+        <v>75214</v>
       </c>
       <c r="C8" s="2">
-        <v>6602</v>
+        <v>6659</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>81221</v>
+        <v>81873</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -903,19 +903,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.26505460410484971</v>
+        <v>0.26294382763548424</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.24101100255966978</v>
+        <v>0.23910442204908661</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>7.5347547914712515E-2</v>
+        <v>7.4838350830841963E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>8.2996820239705005E-2</v>
+        <v>8.2490872062088327E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -924,14 +924,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>67172</v>
+        <v>67745</v>
       </c>
       <c r="C9" s="2">
-        <v>13171</v>
+        <v>13317</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>80343</v>
+        <v>81062</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -941,19 +941,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.24614465479257683</v>
+        <v>0.24396141225235005</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.21050437682367654</v>
+        <v>0.20872389106207101</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>6.9215584706491765E-2</v>
+        <v>6.8747827296113465E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>6.5256619116405068E-2</v>
+        <v>6.48588151110948E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -962,14 +962,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>68619</v>
+        <v>69345</v>
       </c>
       <c r="C10" s="2">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>69646</v>
+        <v>70368</v>
       </c>
       <c r="E10" s="2">
         <v>19396</v>
@@ -979,19 +979,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.2784940987278523</v>
+        <v>0.27563665302410184</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.27743044929247002</v>
+        <v>0.27452592111904245</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.7885592686443882E-2</v>
+        <v>6.7426823333101585E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>8.7856453898090756E-2</v>
+        <v>8.7320881419371416E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1000,14 +1000,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>42776</v>
+        <v>43327</v>
       </c>
       <c r="C11" s="2">
-        <v>15347</v>
+        <v>15479</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>58123</v>
+        <v>58806</v>
       </c>
       <c r="E11" s="2">
         <v>15272</v>
@@ -1017,19 +1017,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.26275312698931574</v>
+        <v>0.25970139101452233</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.27216195997755749</v>
+        <v>0.26870081011840191</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>5.345167928992426E-2</v>
+        <v>5.3090454008204127E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>5.3728257408287683E-2</v>
+        <v>5.3400730235032931E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1038,14 +1038,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>50683</v>
+        <v>51332</v>
       </c>
       <c r="C12" s="2">
-        <v>2068</v>
+        <v>2117</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>52751</v>
+        <v>53449</v>
       </c>
       <c r="E12" s="2">
         <v>12710</v>
@@ -1055,19 +1055,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.24094329965308714</v>
+        <v>0.23779677823719808</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.22911035258370657</v>
+        <v>0.2262136678874776</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>4.4484733091601447E-2</v>
+        <v>4.4184106236529234E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>5.3589806306909168E-2</v>
+        <v>5.3263123130836837E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1076,37 +1076,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>26250</v>
+        <v>26682</v>
       </c>
       <c r="C13" s="2">
-        <v>13262</v>
+        <v>13358</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>39512</v>
+        <v>40040</v>
       </c>
       <c r="E13" s="2">
         <v>15031</v>
       </c>
       <c r="F13" s="2">
         <f>D2</f>
-        <v>285716</v>
+        <v>287660</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.38041607612877099</v>
+        <v>0.37539960039960041</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>10.884419047619048</v>
+        <v>10.781050895734952</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>5.2608184350893893E-2</v>
+        <v>5.2252659389557116E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>1.3185898293820928</v>
+        <v>1.3194686531016642</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1115,14 +1115,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>32659</v>
+        <v>33262</v>
       </c>
       <c r="C14" s="2">
-        <v>4568</v>
+        <v>4647</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>37227</v>
+        <v>37909</v>
       </c>
       <c r="E14" s="2">
         <v>17633</v>
@@ -1132,19 +1132,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.47366158970639588</v>
+        <v>0.46514020417315149</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.55999877522275632</v>
+        <v>0.54984667187781855</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>6.1715129709221744E-2</v>
+        <v>6.1298060209970105E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>8.44044064370532E-2</v>
+        <v>8.3889877621415337E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1153,37 +1153,37 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>30670</v>
+        <v>31346</v>
       </c>
       <c r="C15" s="2">
-        <v>6480</v>
+        <v>6561</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>37150</v>
+        <v>37907</v>
       </c>
       <c r="E15" s="2">
         <v>10753</v>
       </c>
       <c r="F15" s="2">
         <f>D2</f>
-        <v>285716</v>
+        <v>287660</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.28944818304172276</v>
+        <v>0.28366792413010788</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>9.3158134985327674</v>
+        <v>9.1769284757225797</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>3.763527418835487E-2</v>
+        <v>3.7380935827018007E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>1.3185898293820928</v>
+        <v>1.3194686531016642</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1192,14 +1192,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>34024</v>
+        <v>34924</v>
       </c>
       <c r="C16" s="2">
-        <v>3587</v>
+        <v>3629</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>37611</v>
+        <v>38553</v>
       </c>
       <c r="E16" s="2">
         <v>13047</v>
@@ -1209,19 +1209,19 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>0.34689319613942732</v>
+        <v>0.33841724379425725</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.70656007524100639</v>
+        <v>0.68835184973084407</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>4.5664226014643913E-2</v>
+        <v>4.5355628172147673E-2</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>0.11094548257131386</v>
+        <v>0.11026915949580757</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1230,14 +1230,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>28286</v>
+        <v>29307</v>
       </c>
       <c r="C17" s="2">
-        <v>876</v>
+        <v>867</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>29162</v>
+        <v>30174</v>
       </c>
       <c r="E17" s="2">
         <v>9676</v>
@@ -1247,19 +1247,19 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v>0.33180165969412251</v>
+        <v>0.32067342745409955</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0.32273916425086613</v>
+        <v>0.31149554713890881</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>3.3865796805219166E-2</v>
+        <v>3.3636932489744836E-2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>4.2130670149481041E-2</v>
+        <v>4.1873841806873015E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1268,14 +1268,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>16546</v>
+        <v>17908</v>
       </c>
       <c r="C18" s="2">
-        <v>1097</v>
+        <v>1067</v>
       </c>
       <c r="D18">
         <f t="shared" si="7"/>
-        <v>17643</v>
+        <v>18975</v>
       </c>
       <c r="E18" s="2">
         <v>7106</v>
@@ -1285,19 +1285,19 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="6"/>
-        <v>0.40276596950631977</v>
+        <v>0.3744927536231884</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>0.47098996736371329</v>
+        <v>0.43516863971409425</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="2"/>
-        <v>2.4870850774895349E-2</v>
+        <v>2.4702774108322324E-2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>3.596498110142466E-2</v>
+        <v>3.5745738766673398E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1306,14 +1306,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>13234</v>
+        <v>17459</v>
       </c>
       <c r="C19" s="2">
-        <v>5408</v>
+        <v>4788</v>
       </c>
       <c r="D19">
         <f t="shared" si="7"/>
-        <v>18642</v>
+        <v>22247</v>
       </c>
       <c r="E19" s="2">
         <v>12762</v>
@@ -1323,19 +1323,19 @@
       </c>
       <c r="G19" s="1">
         <f t="shared" si="6"/>
-        <v>0.68458319922755073</v>
+        <v>0.57365037982649347</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>0.78116971437207194</v>
+        <v>0.59213013345552434</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="2"/>
-        <v>4.4666731999608002E-2</v>
+        <v>4.4364875199888756E-2</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>4.7710249535035054E-2</v>
+        <v>4.7419408105975815E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1343,29 +1343,37 @@
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" t="str">
+      <c r="B20" s="2">
+        <v>10623</v>
+      </c>
+      <c r="C20" s="2">
+        <v>7063</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="1" t="str">
+        <v>17686</v>
+      </c>
+      <c r="E20" s="2">
+        <v>12655</v>
+      </c>
+      <c r="F20" s="2">
+        <v>8796</v>
+      </c>
+      <c r="G20" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I20" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J20" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.71553771344566319</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.82801468511719856</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="2"/>
+        <v>4.3992908294514355E-2</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="3"/>
+        <v>4.0346402950296317E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2684,8 +2692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AY24" sqref="AY24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BZ12" sqref="BZ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6036,16 +6044,16 @@
         <v>14</v>
       </c>
       <c r="BV12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BW12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BX12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="BY12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="BZ12" t="s">
         <v>20</v>
@@ -6181,24 +6189,47 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6215,47 +6246,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 Day 20 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC08BF5-7D0E-4ABC-84A8-559229ABB0CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520DAB1C-3DFC-491E-8CDB-8D171480C532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3666" yWindow="480" windowWidth="16890" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="324" windowWidth="16890" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -655,14 +655,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>218012</v>
+        <v>219499</v>
       </c>
       <c r="C2" s="2">
-        <v>69648</v>
+        <v>70141</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>287660</v>
+        <v>289640</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -672,19 +672,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>8.862198428700549E-2</v>
+        <v>8.8016157989228003E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>9.4297561602113639E-2</v>
+        <v>9.3658741042100424E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>8.862198428700549E-2</v>
+        <v>8.8016157989228003E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>9.4297561602113639E-2</v>
+        <v>9.3658741042100424E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -693,14 +693,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>184421</v>
+        <v>185753</v>
       </c>
       <c r="C3" s="2">
-        <v>8581</v>
+        <v>8664</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>193002</v>
+        <v>194417</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -710,19 +710,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.15262536139521871</v>
+        <v>0.15151452805053056</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.16053486316634222</v>
+        <v>0.15938369770609356</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.10240214141695057</v>
+        <v>0.10170211296782213</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.13579986422765719</v>
+        <v>0.13487988555756519</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -731,14 +731,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>122034</v>
+        <v>122981</v>
       </c>
       <c r="C4" s="2">
-        <v>18399</v>
+        <v>18530</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>140433</v>
+        <v>141511</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -748,19 +748,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.46469134747530849</v>
+        <v>0.46115142992417552</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.46714849959847254</v>
+        <v>0.4635512802790675</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.22685809636376278</v>
+        <v>0.2253072780002762</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.26149019320037431</v>
+        <v>0.25971872309213256</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -772,14 +772,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>121528</v>
+        <v>122501</v>
       </c>
       <c r="C5" s="2">
-        <v>16361</v>
+        <v>16529</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>137889</v>
+        <v>139030</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -789,19 +789,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.24743815677827818</v>
+        <v>0.24540746601452923</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.2163040616154302</v>
+        <v>0.21458600337956424</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.11860877424737537</v>
+        <v>0.1177979560834139</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.1205759316000954</v>
+        <v>0.11975908774071864</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -810,14 +810,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>74406</v>
+        <v>75067</v>
       </c>
       <c r="C6" s="2">
-        <v>28865</v>
+        <v>29113</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>103271</v>
+        <v>104180</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -827,19 +827,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.21520078240745225</v>
+        <v>0.21332309464388557</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.20294062306803215</v>
+        <v>0.20115363608509731</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>7.7257873878884789E-2</v>
+        <v>7.6729733462228972E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>6.9262242445369979E-2</v>
+        <v>6.8793024114005077E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -848,14 +848,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>95486</v>
+        <v>96400</v>
       </c>
       <c r="C7" s="2">
-        <v>1614</v>
+        <v>1669</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>97100</v>
+        <v>98069</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -865,19 +865,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.24704428424304839</v>
+        <v>0.24460328952064364</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.24498879416877867</v>
+        <v>0.24266597510373444</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>8.3390113328234719E-2</v>
+        <v>8.2820052478939379E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.10730143294864503</v>
+        <v>0.10657451742376958</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -886,14 +886,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>75214</v>
+        <v>75956</v>
       </c>
       <c r="C8" s="2">
-        <v>6659</v>
+        <v>6725</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>81873</v>
+        <v>82681</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -903,19 +903,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.26294382763548424</v>
+        <v>0.26037420931048244</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.23910442204908661</v>
+        <v>0.23676865553741641</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>7.4838350830841963E-2</v>
+        <v>7.4326750448833037E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>8.2490872062088327E-2</v>
+        <v>8.1932036136838887E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -924,14 +924,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>67745</v>
+        <v>68395</v>
       </c>
       <c r="C9" s="2">
-        <v>13317</v>
+        <v>13479</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>81062</v>
+        <v>81874</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -941,19 +941,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.24396141225235005</v>
+        <v>0.24154188142755942</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.20872389106207101</v>
+        <v>0.20674025879084729</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>6.8747827296113465E-2</v>
+        <v>6.8277862173732912E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>6.48588151110948E-2</v>
+        <v>6.4419427878942503E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -962,14 +962,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>69345</v>
+        <v>70145</v>
       </c>
       <c r="C10" s="2">
-        <v>1023</v>
+        <v>1055</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>70368</v>
+        <v>71200</v>
       </c>
       <c r="E10" s="2">
         <v>19396</v>
@@ -979,19 +979,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.27563665302410184</v>
+        <v>0.27241573033707867</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.27452592111904245</v>
+        <v>0.27139496756718229</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.7426823333101585E-2</v>
+        <v>6.6965888689407546E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>8.7320881419371416E-2</v>
+        <v>8.6729324507173147E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1000,14 +1000,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>43327</v>
+        <v>43890</v>
       </c>
       <c r="C11" s="2">
-        <v>15479</v>
+        <v>15635</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>58806</v>
+        <v>59525</v>
       </c>
       <c r="E11" s="2">
         <v>15272</v>
@@ -1017,19 +1017,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.25970139101452233</v>
+        <v>0.25656446871062577</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.26870081011840191</v>
+        <v>0.26525404420141263</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>5.3090454008204127E-2</v>
+        <v>5.2727523822676425E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>5.3400730235032931E-2</v>
+        <v>5.3038966008956759E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1038,14 +1038,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>51332</v>
+        <v>52032</v>
       </c>
       <c r="C12" s="2">
-        <v>2117</v>
+        <v>2133</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>53449</v>
+        <v>54165</v>
       </c>
       <c r="E12" s="2">
         <v>12710</v>
@@ -1055,19 +1055,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.23779677823719808</v>
+        <v>0.23465337394996769</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.2262136678874776</v>
+        <v>0.22317035670356702</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>4.4184106236529234E-2</v>
+        <v>4.3882060488882754E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>5.3263123130836837E-2</v>
+        <v>5.2902291126611052E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1076,37 +1076,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>26682</v>
+        <v>27163</v>
       </c>
       <c r="C13" s="2">
-        <v>13358</v>
+        <v>13545</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>40040</v>
+        <v>40708</v>
       </c>
       <c r="E13" s="2">
         <v>15031</v>
       </c>
       <c r="F13" s="2">
         <f>D2</f>
-        <v>287660</v>
+        <v>289640</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.37539960039960041</v>
+        <v>0.36923946153090303</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>10.781050895734952</v>
+        <v>10.663034274564666</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>5.2252659389557116E-2</v>
+        <v>5.1895456428670071E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>1.3194686531016642</v>
+        <v>1.319550430753671</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1115,14 +1115,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>33262</v>
+        <v>33882</v>
       </c>
       <c r="C14" s="2">
-        <v>4647</v>
+        <v>4738</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>37909</v>
+        <v>38620</v>
       </c>
       <c r="E14" s="2">
         <v>17633</v>
@@ -1132,19 +1132,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.46514020417315149</v>
+        <v>0.45657690315898497</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.54984667187781855</v>
+        <v>0.53978513665072902</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>6.1298060209970105E-2</v>
+        <v>6.0879022234497995E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>8.3889877621415337E-2</v>
+        <v>8.3321564107353557E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1153,37 +1153,37 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>31346</v>
+        <v>32010</v>
       </c>
       <c r="C15" s="2">
-        <v>6561</v>
+        <v>6701</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>37907</v>
+        <v>38711</v>
       </c>
       <c r="E15" s="2">
         <v>10753</v>
       </c>
       <c r="F15" s="2">
         <f>D2</f>
-        <v>287660</v>
+        <v>289640</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.28366792413010788</v>
+        <v>0.27777634264162643</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>9.1769284757225797</v>
+        <v>9.0484223680099962</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>3.7380935827018007E-2</v>
+        <v>3.71253970446071E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>1.3194686531016642</v>
+        <v>1.319550430753671</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1192,14 +1192,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>34924</v>
+        <v>35737</v>
       </c>
       <c r="C16" s="2">
-        <v>3629</v>
+        <v>3719</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>38553</v>
+        <v>39456</v>
       </c>
       <c r="E16" s="2">
         <v>13047</v>
@@ -1209,19 +1209,19 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>0.33841724379425725</v>
+        <v>0.33067214111922139</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.68835184973084407</v>
+        <v>0.67269216778129115</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>4.5355628172147673E-2</v>
+        <v>4.5045573815771303E-2</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>0.11026915949580757</v>
+        <v>0.1095221390530253</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1230,14 +1230,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>29307</v>
+        <v>30215</v>
       </c>
       <c r="C17" s="2">
-        <v>867</v>
+        <v>915</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>30174</v>
+        <v>31130</v>
       </c>
       <c r="E17" s="2">
         <v>9676</v>
@@ -1247,19 +1247,19 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v>0.32067342745409955</v>
+        <v>0.31082557018952778</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0.31149554713890881</v>
+        <v>0.30213470130729769</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>3.3636932489744836E-2</v>
+        <v>3.3406987985084936E-2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>4.1873841806873015E-2</v>
+        <v>4.1590166697798164E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1268,14 +1268,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>17908</v>
+        <v>19003</v>
       </c>
       <c r="C18" s="2">
-        <v>1067</v>
+        <v>1046</v>
       </c>
       <c r="D18">
         <f t="shared" si="7"/>
-        <v>18975</v>
+        <v>20049</v>
       </c>
       <c r="E18" s="2">
         <v>7106</v>
@@ -1285,19 +1285,19 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="6"/>
-        <v>0.3744927536231884</v>
+        <v>0.35443164247593395</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>0.43516863971409425</v>
+        <v>0.41009314318791767</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="2"/>
-        <v>2.4702774108322324E-2</v>
+        <v>2.4533904156884407E-2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>3.5745738766673398E-2</v>
+        <v>3.5503578604002752E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1306,14 +1306,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>17459</v>
+        <v>19213</v>
       </c>
       <c r="C19" s="2">
-        <v>4788</v>
+        <v>4641</v>
       </c>
       <c r="D19">
         <f t="shared" si="7"/>
-        <v>22247</v>
+        <v>23854</v>
       </c>
       <c r="E19" s="2">
         <v>12762</v>
@@ -1323,19 +1323,19 @@
       </c>
       <c r="G19" s="1">
         <f t="shared" si="6"/>
-        <v>0.57365037982649347</v>
+        <v>0.53500461138593103</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>0.59213013345552434</v>
+        <v>0.53807317961796697</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="2"/>
-        <v>4.4364875199888756E-2</v>
+        <v>4.4061593702527276E-2</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>4.7419408105975815E-2</v>
+        <v>4.7098164456330097E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1344,14 +1344,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>10623</v>
+        <v>16216</v>
       </c>
       <c r="C20" s="2">
-        <v>7063</v>
+        <v>6636</v>
       </c>
       <c r="D20">
         <f t="shared" si="7"/>
-        <v>17686</v>
+        <v>22852</v>
       </c>
       <c r="E20" s="2">
         <v>12655</v>
@@ -1361,19 +1361,19 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" si="6"/>
-        <v>0.71553771344566319</v>
+        <v>0.55378085069140559</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
-        <v>0.82801468511719856</v>
+        <v>0.5424272323630982</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
-        <v>4.3992908294514355E-2</v>
+        <v>4.3692169589835655E-2</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="3"/>
-        <v>4.0346402950296317E-2</v>
+        <v>4.0073075503760838E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1381,29 +1381,37 @@
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" t="str">
+      <c r="B21" s="2">
+        <v>8907</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4077</v>
+      </c>
+      <c r="D21">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="1" t="str">
+        <v>12984</v>
+      </c>
+      <c r="E21" s="2">
+        <v>9863</v>
+      </c>
+      <c r="F21" s="2">
+        <v>7499</v>
+      </c>
+      <c r="G21" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I21" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J21" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.75962723351817618</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.84192208375435051</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4052617041845049E-2</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="3"/>
+        <v>3.4164164757014837E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2692,8 +2700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BZ12" sqref="BZ12"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="CW12" sqref="CW12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6056,16 +6064,16 @@
         <v>16</v>
       </c>
       <c r="BZ12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="CA12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="CB12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="CC12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="CD12" t="s">
         <v>20</v>
@@ -6189,47 +6197,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6246,24 +6231,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 Day 21 Part 1 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520DAB1C-3DFC-491E-8CDB-8D171480C532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F998CA42-325A-474A-B9AB-EBB8530740AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="324" windowWidth="16890" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2701,7 +2701,7 @@
   <dimension ref="A1:CX20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="CW12" sqref="CW12"/>
+      <selection activeCell="CH12" sqref="CH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6076,13 +6076,13 @@
         <v>14</v>
       </c>
       <c r="CD12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="CE12" t="s">
         <v>20</v>
       </c>
       <c r="CF12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="CG12" t="s">
         <v>20</v>
@@ -6197,24 +6197,47 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6231,47 +6254,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 Day24 part 1 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F998CA42-325A-474A-B9AB-EBB8530740AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF939A7-CD8B-409D-A126-F0EFA956968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="324" windowWidth="16890" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3174" yWindow="510" windowWidth="16890" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="33">
   <si>
     <t>Day</t>
   </si>
@@ -126,7 +126,13 @@
     <t>Hillwalking</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>S</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -604,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -655,14 +661,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>219499</v>
+        <v>223339</v>
       </c>
       <c r="C2" s="2">
-        <v>70141</v>
+        <v>71526</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>289640</v>
+        <v>294865</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -672,19 +678,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>8.8016157989228003E-2</v>
+        <v>8.645651399793125E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>9.3658741042100424E-2</v>
+        <v>9.204841071196701E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>8.8016157989228003E-2</v>
+        <v>8.645651399793125E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>9.3658741042100424E-2</v>
+        <v>9.204841071196701E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -693,14 +699,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>185753</v>
+        <v>189342</v>
       </c>
       <c r="C3" s="2">
-        <v>8664</v>
+        <v>8887</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>194417</v>
+        <v>198229</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -710,19 +716,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.15151452805053056</v>
+        <v>0.14860086062079716</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.15938369770609356</v>
+        <v>0.15636256086869263</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.10170211296782213</v>
+        <v>9.9899954216336295E-2</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.13487988555756519</v>
+        <v>0.13256081562109617</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -731,14 +737,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>122981</v>
+        <v>125482</v>
       </c>
       <c r="C4" s="2">
-        <v>18530</v>
+        <v>18994</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>141511</v>
+        <v>144476</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -748,19 +754,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.46115142992417552</v>
+        <v>0.45168747750491434</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.4635512802790675</v>
+        <v>0.45431217226375098</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.2253072780002762</v>
+        <v>0.22131483899411594</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.25971872309213256</v>
+        <v>0.2552532249181737</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -772,14 +778,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>122501</v>
+        <v>125190</v>
       </c>
       <c r="C5" s="2">
-        <v>16529</v>
+        <v>16993</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>139030</v>
+        <v>142183</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -789,19 +795,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.24540746601452923</v>
+        <v>0.23996539670706063</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.21458600337956424</v>
+        <v>0.20997683521048008</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.1177979560834139</v>
+        <v>0.11571057941769962</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.11975908774071864</v>
+        <v>0.1176999986567505</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -810,14 +816,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>75067</v>
+        <v>76801</v>
       </c>
       <c r="C6" s="2">
-        <v>29113</v>
+        <v>29821</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>104180</v>
+        <v>106622</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -827,19 +833,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.21332309464388557</v>
+        <v>0.20843728311230328</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.20115363608509731</v>
+        <v>0.19661202328094687</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>7.6729733462228972E-2</v>
+        <v>7.5370084614993296E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>6.8793024114005077E-2</v>
+        <v>6.7610224815191258E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -848,14 +854,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>96400</v>
+        <v>98842</v>
       </c>
       <c r="C7" s="2">
-        <v>1669</v>
+        <v>1747</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>98069</v>
+        <v>100589</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -865,19 +871,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.24460328952064364</v>
+        <v>0.23847538001173091</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.24266597510373444</v>
+        <v>0.23667064608162522</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>8.2820052478939379E-2</v>
+        <v>8.1352483339833484E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.10657451742376958</v>
+        <v>0.10474211848356087</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -886,14 +892,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>75956</v>
+        <v>77991</v>
       </c>
       <c r="C8" s="2">
-        <v>6725</v>
+        <v>6985</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>82681</v>
+        <v>84976</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -903,19 +909,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.26037420931048244</v>
+        <v>0.25334212012803614</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.23676865553741641</v>
+        <v>0.23059070918439306</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>7.4326750448833037E-2</v>
+        <v>7.3009682397029152E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>8.1932036136838887E-2</v>
+        <v>8.0523330005059568E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -924,14 +930,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>68395</v>
+        <v>70266</v>
       </c>
       <c r="C9" s="2">
-        <v>13479</v>
+        <v>13982</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>81874</v>
+        <v>84248</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -941,19 +947,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.24154188142755942</v>
+        <v>0.23473554268350583</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.20674025879084729</v>
+        <v>0.20123530583781629</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>6.8277862173732912E-2</v>
+        <v>6.7067980262153867E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>6.4419427878942503E-2</v>
+        <v>6.3311826416344655E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -962,14 +968,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>70145</v>
+        <v>72311</v>
       </c>
       <c r="C10" s="2">
-        <v>1055</v>
+        <v>1116</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>71200</v>
+        <v>73427</v>
       </c>
       <c r="E10" s="2">
         <v>19396</v>
@@ -979,19 +985,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.27241573033707867</v>
+        <v>0.26415351301292439</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.27139496756718229</v>
+        <v>0.26326561657285891</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.6965888689407546E-2</v>
+        <v>6.5779254913265389E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>8.6729324507173147E-2</v>
+        <v>8.5238135748794436E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1000,14 +1006,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>43890</v>
+        <v>54343</v>
       </c>
       <c r="C11" s="2">
-        <v>15635</v>
+        <v>16222</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>59525</v>
+        <v>70565</v>
       </c>
       <c r="E11" s="2">
         <v>15272</v>
@@ -1017,19 +1023,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.25656446871062577</v>
+        <v>0.21642457308864169</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.26525404420141263</v>
+        <v>0.21423182378595218</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>5.2727523822676425E-2</v>
+        <v>5.179319349532837E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>5.3038966008956759E-2</v>
+        <v>5.2127035582679247E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1038,14 +1044,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>52032</v>
+        <v>53838</v>
       </c>
       <c r="C12" s="2">
-        <v>2133</v>
+        <v>2239</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>54165</v>
+        <v>56077</v>
       </c>
       <c r="E12" s="2">
         <v>12710</v>
@@ -1055,19 +1061,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.23465337394996769</v>
+        <v>0.22665263833657293</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.22317035670356702</v>
+        <v>0.21568408930495189</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>4.3882060488882754E-2</v>
+        <v>4.3104471537822396E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>5.2902291126611052E-2</v>
+        <v>5.1992710632715287E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1076,37 +1082,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>27163</v>
+        <v>28383</v>
       </c>
       <c r="C13" s="2">
-        <v>13545</v>
+        <v>13965</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>40708</v>
+        <v>42348</v>
       </c>
       <c r="E13" s="2">
         <v>15031</v>
       </c>
       <c r="F13" s="2">
         <f>D2</f>
-        <v>289640</v>
+        <v>294865</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.36923946153090303</v>
+        <v>0.35494002078020215</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>10.663034274564666</v>
+        <v>10.388789063876263</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>5.1895456428670071E-2</v>
+        <v>5.097587031353331E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>1.319550430753671</v>
+        <v>1.3202575457040642</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1115,14 +1121,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>33882</v>
+        <v>35467</v>
       </c>
       <c r="C14" s="2">
-        <v>4738</v>
+        <v>4931</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>38620</v>
+        <v>40398</v>
       </c>
       <c r="E14" s="2">
         <v>17633</v>
@@ -1132,19 +1138,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.45657690315898497</v>
+        <v>0.43648200405960691</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.53978513665072902</v>
+        <v>0.51566244678151518</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>6.0879022234497995E-2</v>
+        <v>5.9800247570922289E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>8.3321564107353557E-2</v>
+        <v>8.1888966996359794E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1153,37 +1159,37 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>32010</v>
+        <v>33707</v>
       </c>
       <c r="C15" s="2">
-        <v>6701</v>
+        <v>7040</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>38711</v>
+        <v>40747</v>
       </c>
       <c r="E15" s="2">
         <v>10753</v>
       </c>
       <c r="F15" s="2">
         <f>D2</f>
-        <v>289640</v>
+        <v>294865</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.27777634264162643</v>
+        <v>0.26389672859351609</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>9.0484223680099962</v>
+        <v>8.747886195745691</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>3.71253970446071E-2</v>
+        <v>3.6467535991046747E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>1.319550430753671</v>
+        <v>1.3202575457040642</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1192,14 +1198,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>35737</v>
+        <v>37714</v>
       </c>
       <c r="C16" s="2">
-        <v>3719</v>
+        <v>3930</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>39456</v>
+        <v>41644</v>
       </c>
       <c r="E16" s="2">
         <v>13047</v>
@@ -1209,19 +1215,19 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>0.33067214111922139</v>
+        <v>0.31329843434828547</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.67269216778129115</v>
+        <v>0.63742907143235938</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>4.5045573815771303E-2</v>
+        <v>4.4247367439336646E-2</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>0.1095221390530253</v>
+        <v>0.10763905990445019</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1230,14 +1236,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>30215</v>
+        <v>32235</v>
       </c>
       <c r="C17" s="2">
-        <v>915</v>
+        <v>956</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>31130</v>
+        <v>33191</v>
       </c>
       <c r="E17" s="2">
         <v>9676</v>
@@ -1247,19 +1253,19 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v>0.31082557018952778</v>
+        <v>0.29152481094272542</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0.30213470130729769</v>
+        <v>0.28320148906468123</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>3.3406987985084936E-2</v>
+        <v>3.281501704169705E-2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>4.1590166697798164E-2</v>
+        <v>4.0875082274031853E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1268,14 +1274,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>19003</v>
+        <v>20970</v>
       </c>
       <c r="C18" s="2">
-        <v>1046</v>
+        <v>1058</v>
       </c>
       <c r="D18">
         <f t="shared" si="7"/>
-        <v>20049</v>
+        <v>22028</v>
       </c>
       <c r="E18" s="2">
         <v>7106</v>
@@ -1285,19 +1291,19 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="6"/>
-        <v>0.35443164247593395</v>
+        <v>0.32258943163246778</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>0.41009314318791767</v>
+        <v>0.37162613257033855</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="2"/>
-        <v>2.4533904156884407E-2</v>
+        <v>2.409916402421447E-2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>3.5503578604002752E-2</v>
+        <v>3.4893144502303672E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1306,14 +1312,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>19213</v>
+        <v>21622</v>
       </c>
       <c r="C19" s="2">
-        <v>4641</v>
+        <v>4862</v>
       </c>
       <c r="D19">
         <f t="shared" si="7"/>
-        <v>23854</v>
+        <v>26484</v>
       </c>
       <c r="E19" s="2">
         <v>12762</v>
@@ -1323,19 +1329,19 @@
       </c>
       <c r="G19" s="1">
         <f t="shared" si="6"/>
-        <v>0.53500461138593103</v>
+        <v>0.48187584956955143</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>0.53807317961796697</v>
+        <v>0.47812413282767552</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="2"/>
-        <v>4.4061593702527276E-2</v>
+        <v>4.3280823427670291E-2</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>4.7098164456330097E-2</v>
+        <v>4.6288377757579283E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1344,14 +1350,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>16216</v>
+        <v>19308</v>
       </c>
       <c r="C20" s="2">
-        <v>6636</v>
+        <v>6850</v>
       </c>
       <c r="D20">
         <f t="shared" si="7"/>
-        <v>22852</v>
+        <v>26158</v>
       </c>
       <c r="E20" s="2">
         <v>12655</v>
@@ -1361,19 +1367,19 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" si="6"/>
-        <v>0.55378085069140559</v>
+        <v>0.48379080969493082</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
-        <v>0.5424272323630982</v>
+        <v>0.45556246115599752</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
-        <v>4.3692169589835655E-2</v>
+        <v>4.2917945500483272E-2</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="3"/>
-        <v>4.0073075503760838E-2</v>
+        <v>3.9384075329431938E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1382,14 +1388,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>8907</v>
+        <v>15001</v>
       </c>
       <c r="C21" s="2">
-        <v>4077</v>
+        <v>4157</v>
       </c>
       <c r="D21">
         <f t="shared" si="7"/>
-        <v>12984</v>
+        <v>19158</v>
       </c>
       <c r="E21" s="2">
         <v>9863</v>
@@ -1399,19 +1405,19 @@
       </c>
       <c r="G21" s="1">
         <f t="shared" si="6"/>
-        <v>0.75962723351817618</v>
+        <v>0.51482409437310783</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>0.84192208375435051</v>
+        <v>0.49990000666622225</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="2"/>
-        <v>3.4052617041845049E-2</v>
+        <v>3.344920556865006E-2</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="3"/>
-        <v>3.4164164757014837E-2</v>
+        <v>3.3576759992656906E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1419,29 +1425,38 @@
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" t="str">
+      <c r="B22" s="2">
+        <v>10919</v>
+      </c>
+      <c r="C22" s="2">
+        <v>9871</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="1" t="str">
+        <v>20790</v>
+      </c>
+      <c r="E22" s="2">
+        <v>7152</v>
+      </c>
+      <c r="F22" s="2">
+        <f>D2</f>
+        <v>294865</v>
+      </c>
+      <c r="G22" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I22" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J22" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.34401154401154399</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>27.004762340873707</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="2"/>
+        <v>2.4255167619079917E-2</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3202575457040642</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1449,29 +1464,39 @@
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" t="str">
+      <c r="B23" s="2">
+        <v>12035</v>
+      </c>
+      <c r="C23" s="2">
+        <v>996</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="1" t="str">
+        <v>13031</v>
+      </c>
+      <c r="E23" s="2">
+        <f>D2</f>
+        <v>294865</v>
+      </c>
+      <c r="F23" s="2">
+        <f>D2</f>
+        <v>294865</v>
+      </c>
+      <c r="G23" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J23" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>22.627964085641931</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
+        <v>24.500623182384711</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3202575457040642</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1479,29 +1504,38 @@
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" t="str">
+      <c r="B24" s="2">
+        <v>9625</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3113</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="1" t="str">
+        <v>12738</v>
+      </c>
+      <c r="E24" s="2">
+        <v>4120</v>
+      </c>
+      <c r="F24" s="2">
+        <f>D2</f>
+        <v>294865</v>
+      </c>
+      <c r="G24" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I24" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J24" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.32344167059192969</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>30.635324675324675</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3972495887948723E-2</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3202575457040642</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1509,29 +1543,38 @@
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" t="str">
+      <c r="B25" s="2">
+        <v>3041</v>
+      </c>
+      <c r="C25" s="2">
+        <v>4209</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="1" t="str">
+        <v>7250</v>
+      </c>
+      <c r="E25" s="2">
+        <v>6788</v>
+      </c>
+      <c r="F25" s="2">
+        <f>D2</f>
+        <v>294865</v>
+      </c>
+      <c r="G25" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I25" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J25" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.93627586206896551</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>96.963170009865181</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="2"/>
+        <v>2.3020704390144642E-2</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3202575457040642</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -2700,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="CH12" sqref="CH12"/>
+    <sheetView topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="CT12" sqref="CT12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5971,13 +6014,13 @@
         <v>14</v>
       </c>
       <c r="AU12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="AV12" t="s">
         <v>14</v>
       </c>
       <c r="AW12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AX12" t="s">
         <v>14</v>
@@ -5995,13 +6038,13 @@
         <v>14</v>
       </c>
       <c r="BC12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="BD12" t="s">
         <v>14</v>
       </c>
       <c r="BE12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="BF12" t="s">
         <v>14</v>
@@ -6079,61 +6122,61 @@
         <v>14</v>
       </c>
       <c r="CE12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="CF12" t="s">
         <v>14</v>
       </c>
       <c r="CG12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="CH12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="CI12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="CJ12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="CK12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="CL12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="CM12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="CN12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="CO12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="CP12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="CQ12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="CR12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="CS12" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="CT12" t="s">
         <v>20</v>
       </c>
       <c r="CU12" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="CV12" t="s">
         <v>20</v>
       </c>
       <c r="CW12" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="CX12">
         <v>2023</v>
@@ -6197,47 +6240,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6254,24 +6274,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
2023 Day 25 done (sort of)
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF939A7-CD8B-409D-A126-F0EFA956968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E04E87D-5D45-4D1B-A5A9-BAC5AD764E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3174" yWindow="510" windowWidth="16890" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="660" windowWidth="16890" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="35">
   <si>
     <t>Day</t>
   </si>
@@ -134,6 +134,12 @@
   <si>
     <t>N</t>
   </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>done, but horrible</t>
+  </si>
 </sst>
 </file>
 
@@ -154,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +203,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -210,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -231,30 +243,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="28">
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -320,6 +320,166 @@
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF24B850"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF24B850"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B0F0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF24B850"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF24B850"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFC000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -610,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -661,14 +821,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>223339</v>
+        <v>224386</v>
       </c>
       <c r="C2" s="2">
-        <v>71526</v>
+        <v>71869</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>294865</v>
+        <v>296255</v>
       </c>
       <c r="E2" s="2">
         <v>25493</v>
@@ -678,19 +838,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>8.645651399793125E-2</v>
+        <v>8.605086833977485E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>9.204841071196701E-2</v>
+        <v>9.1618906705409425E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>8.645651399793125E-2</v>
+        <v>8.605086833977485E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>9.204841071196701E-2</v>
+        <v>9.1618906705409425E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -699,14 +859,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>189342</v>
+        <v>190379</v>
       </c>
       <c r="C3" s="2">
-        <v>8887</v>
+        <v>8953</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>198229</v>
+        <v>199332</v>
       </c>
       <c r="E3" s="2">
         <v>29457</v>
@@ -716,19 +876,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.14860086062079716</v>
+        <v>0.14777858045873216</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.15636256086869263</v>
+        <v>0.15551084941091192</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>9.9899954216336295E-2</v>
+        <v>9.9431233228131174E-2</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.13256081562109617</v>
+        <v>0.13194227803873682</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -737,14 +897,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>125482</v>
+        <v>126198</v>
       </c>
       <c r="C4" s="2">
-        <v>18994</v>
+        <v>19107</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>144476</v>
+        <v>145305</v>
       </c>
       <c r="E4" s="2">
         <v>65258</v>
@@ -754,19 +914,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.45168747750491434</v>
+        <v>0.44911049172430406</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.45431217226375098</v>
+        <v>0.45173457582529042</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.22131483899411594</v>
+        <v>0.22027645103036236</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.2552532249181737</v>
+        <v>0.25406219639371441</v>
       </c>
       <c r="K4" t="s">
         <v>29</v>
@@ -778,14 +938,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>125190</v>
+        <v>125952</v>
       </c>
       <c r="C5" s="2">
-        <v>16993</v>
+        <v>17070</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>142183</v>
+        <v>143022</v>
       </c>
       <c r="E5" s="2">
         <v>34119</v>
@@ -795,19 +955,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.23996539670706063</v>
+        <v>0.23855770440911189</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.20997683521048008</v>
+        <v>0.20870649136178862</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.11571057941769962</v>
+        <v>0.11516767649491148</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>0.1176999986567505</v>
+        <v>0.11715080263474548</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -816,14 +976,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>76801</v>
+        <v>77300</v>
       </c>
       <c r="C6" s="2">
-        <v>29821</v>
+        <v>30001</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>106622</v>
+        <v>107301</v>
       </c>
       <c r="E6" s="2">
         <v>22224</v>
@@ -833,19 +993,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.20843728311230328</v>
+        <v>0.20711829339894317</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.19661202328094687</v>
+        <v>0.19534282018111254</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>7.5370084614993296E-2</v>
+        <v>7.5016455418473946E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>6.7610224815191258E-2</v>
+        <v>6.7294751009421269E-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -854,14 +1014,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>98842</v>
+        <v>99515</v>
       </c>
       <c r="C7" s="2">
-        <v>1747</v>
+        <v>1766</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>100589</v>
+        <v>101281</v>
       </c>
       <c r="E7" s="2">
         <v>23988</v>
@@ -871,19 +1031,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.23847538001173091</v>
+        <v>0.23684600270534453</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.23667064608162522</v>
+        <v>0.23507008993619052</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>8.1352483339833484E-2</v>
+        <v>8.0970785303201634E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0.10474211848356087</v>
+        <v>0.1042533847922776</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -892,14 +1052,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>77991</v>
+        <v>78607</v>
       </c>
       <c r="C8" s="2">
-        <v>6985</v>
+        <v>7031</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>84976</v>
+        <v>85638</v>
       </c>
       <c r="E8" s="2">
         <v>21528</v>
@@ -909,19 +1069,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.25334212012803614</v>
+        <v>0.25138373152105375</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.23059070918439306</v>
+        <v>0.22878369610848906</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>7.3009682397029152E-2</v>
+        <v>7.2667127980962351E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>8.0523330005059568E-2</v>
+        <v>8.0147602791618019E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -930,14 +1090,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>70266</v>
+        <v>70834</v>
       </c>
       <c r="C9" s="2">
-        <v>13982</v>
+        <v>14102</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>84248</v>
+        <v>84936</v>
       </c>
       <c r="E9" s="2">
         <v>19776</v>
@@ -947,19 +1107,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.23473554268350583</v>
+        <v>0.23283413393614016</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.20123530583781629</v>
+        <v>0.19962165061975887</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>6.7067980262153867E-2</v>
+        <v>6.6753303741709E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>6.3311826416344655E-2</v>
+        <v>6.3016409223391828E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -968,14 +1128,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>72311</v>
+        <v>72923</v>
       </c>
       <c r="C10" s="2">
-        <v>1116</v>
+        <v>1129</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>73427</v>
+        <v>74052</v>
       </c>
       <c r="E10" s="2">
         <v>19396</v>
@@ -985,19 +1145,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.26415351301292439</v>
+        <v>0.26192405336790364</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.26326561657285891</v>
+        <v>0.26105618254871577</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.5779254913265389E-2</v>
+        <v>6.5470624968354971E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>8.5238135748794436E-2</v>
+        <v>8.4840408938169048E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1006,14 +1166,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>54343</v>
+        <v>45803</v>
       </c>
       <c r="C11" s="2">
-        <v>16222</v>
+        <v>16356</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>70565</v>
+        <v>62159</v>
       </c>
       <c r="E11" s="2">
         <v>15272</v>
@@ -1023,19 +1183,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.21642457308864169</v>
+        <v>0.24569249827056419</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.21423182378595218</v>
+        <v>0.25417549068838285</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>5.179319349532837E-2</v>
+        <v>5.1550184807007474E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>5.2127035582679247E-2</v>
+        <v>5.1883807367661086E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1044,14 +1204,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>53838</v>
+        <v>54398</v>
       </c>
       <c r="C12" s="2">
-        <v>2239</v>
+        <v>2276</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>56077</v>
+        <v>56674</v>
       </c>
       <c r="E12" s="2">
         <v>12710</v>
@@ -1061,19 +1221,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.22665263833657293</v>
+        <v>0.22426509510533932</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.21568408930495189</v>
+        <v>0.21346373028420162</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>4.3104471537822396E-2</v>
+        <v>4.2902229498236313E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>5.1992710632715287E-2</v>
+        <v>5.1750109186847665E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1082,37 +1242,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>28383</v>
+        <v>28767</v>
       </c>
       <c r="C13" s="2">
-        <v>13965</v>
+        <v>14075</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>42348</v>
+        <v>42842</v>
       </c>
       <c r="E13" s="2">
         <v>15031</v>
       </c>
       <c r="F13" s="2">
         <f>D2</f>
-        <v>294865</v>
+        <v>296255</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.35494002078020215</v>
+        <v>0.35084729937911396</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>10.388789063876263</v>
+        <v>10.29843223137623</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>5.097587031353331E-2</v>
+        <v>5.073669642706452E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>1.3202575457040642</v>
+        <v>1.3202918185626553</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1121,14 +1281,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>35467</v>
+        <v>35929</v>
       </c>
       <c r="C14" s="2">
-        <v>4931</v>
+        <v>4968</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>40398</v>
+        <v>40897</v>
       </c>
       <c r="E14" s="2">
         <v>17633</v>
@@ -1138,19 +1298,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.43648200405960691</v>
+        <v>0.43115631953444017</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.51566244678151518</v>
+        <v>0.50903170141111642</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>5.9800247570922289E-2</v>
+        <v>5.9519670554083477E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>8.1888966996359794E-2</v>
+        <v>8.1506867629887778E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1159,37 +1319,37 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>33707</v>
+        <v>34167</v>
       </c>
       <c r="C15" s="2">
-        <v>7040</v>
+        <v>7124</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>40747</v>
+        <v>41291</v>
       </c>
       <c r="E15" s="2">
         <v>10753</v>
       </c>
       <c r="F15" s="2">
         <f>D2</f>
-        <v>294865</v>
+        <v>296255</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.26389672859351609</v>
+        <v>0.2604199462352571</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>8.747886195745691</v>
+        <v>8.6707934556736035</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>3.6467535991046747E-2</v>
+        <v>3.6296433815463033E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>1.3202575457040642</v>
+        <v>1.3202918185626553</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -1198,14 +1358,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>37714</v>
+        <v>38266</v>
       </c>
       <c r="C16" s="2">
-        <v>3930</v>
+        <v>3983</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>41644</v>
+        <v>42249</v>
       </c>
       <c r="E16" s="2">
         <v>13047</v>
@@ -1215,19 +1375,19 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>0.31329843434828547</v>
+        <v>0.3088120428885891</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.63742907143235938</v>
+        <v>0.62823394135786337</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>4.4247367439336646E-2</v>
+        <v>4.4039763041973976E-2</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>0.10763905990445019</v>
+        <v>0.10713680889182034</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1236,14 +1396,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>32235</v>
+        <v>32762</v>
       </c>
       <c r="C17" s="2">
-        <v>956</v>
+        <v>981</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>33191</v>
+        <v>33743</v>
       </c>
       <c r="E17" s="2">
         <v>9676</v>
@@ -1253,19 +1413,19 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v>0.29152481094272542</v>
+        <v>0.2867557715674362</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0.28320148906468123</v>
+        <v>0.27864599230816189</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>3.281501704169705E-2</v>
+        <v>3.2661052134141194E-2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>4.0875082274031853E-2</v>
+        <v>4.0684356421523626E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1274,14 +1434,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>20970</v>
+        <v>21461</v>
       </c>
       <c r="C18" s="2">
-        <v>1058</v>
+        <v>1066</v>
       </c>
       <c r="D18">
         <f t="shared" si="7"/>
-        <v>22028</v>
+        <v>22527</v>
       </c>
       <c r="E18" s="2">
         <v>7106</v>
@@ -1291,19 +1451,19 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="6"/>
-        <v>0.32258943163246778</v>
+        <v>0.31544368979446885</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>0.37162613257033855</v>
+        <v>0.36312380597362659</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="2"/>
-        <v>2.409916402421447E-2</v>
+        <v>2.3986093061720476E-2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>3.4893144502303672E-2</v>
+        <v>3.4730330769299329E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1312,14 +1472,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>21622</v>
+        <v>22142</v>
       </c>
       <c r="C19" s="2">
-        <v>4862</v>
+        <v>4912</v>
       </c>
       <c r="D19">
         <f t="shared" si="7"/>
-        <v>26484</v>
+        <v>27054</v>
       </c>
       <c r="E19" s="2">
         <v>12762</v>
@@ -1329,19 +1489,19 @@
       </c>
       <c r="G19" s="1">
         <f t="shared" si="6"/>
-        <v>0.48187584956955143</v>
+        <v>0.47172322022621421</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>0.47812413282767552</v>
+        <v>0.4668954927287508</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="2"/>
-        <v>4.3280823427670291E-2</v>
+        <v>4.3077753961958447E-2</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>4.6288377757579283E-2</v>
+        <v>4.6072393108304438E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1350,14 +1510,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>19308</v>
+        <v>19869</v>
       </c>
       <c r="C20" s="2">
-        <v>6850</v>
+        <v>6926</v>
       </c>
       <c r="D20">
         <f t="shared" si="7"/>
-        <v>26158</v>
+        <v>26795</v>
       </c>
       <c r="E20" s="2">
         <v>12655</v>
@@ -1367,19 +1527,19 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" si="6"/>
-        <v>0.48379080969493082</v>
+        <v>0.47228960626982647</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
-        <v>0.45556246115599752</v>
+        <v>0.4426996829231466</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
-        <v>4.2917945500483272E-2</v>
+        <v>4.2716578623145603E-2</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="3"/>
-        <v>3.9384075329431938E-2</v>
+        <v>3.9200306614494668E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1388,14 +1548,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>15001</v>
+        <v>15615</v>
       </c>
       <c r="C21" s="2">
-        <v>4157</v>
+        <v>4201</v>
       </c>
       <c r="D21">
         <f t="shared" si="7"/>
-        <v>19158</v>
+        <v>19816</v>
       </c>
       <c r="E21" s="2">
         <v>9863</v>
@@ -1405,19 +1565,19 @@
       </c>
       <c r="G21" s="1">
         <f t="shared" si="6"/>
-        <v>0.51482409437310783</v>
+        <v>0.4977291077916835</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>0.49990000666622225</v>
+        <v>0.48024335574767851</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="2"/>
-        <v>3.344920556865006E-2</v>
+        <v>3.3292265109449631E-2</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="3"/>
-        <v>3.3576759992656906E-2</v>
+        <v>3.342008859732782E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1426,37 +1586,37 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>10919</v>
+        <v>11642</v>
       </c>
       <c r="C22" s="2">
-        <v>9871</v>
+        <v>9896</v>
       </c>
       <c r="D22">
         <f t="shared" si="7"/>
-        <v>20790</v>
+        <v>21538</v>
       </c>
       <c r="E22" s="2">
         <v>7152</v>
       </c>
       <c r="F22" s="2">
         <f>D2</f>
-        <v>294865</v>
+        <v>296255</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="6"/>
-        <v>0.34401154401154399</v>
+        <v>0.33206425851982541</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="1"/>
-        <v>27.004762340873707</v>
+        <v>25.447088129187424</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="2"/>
-        <v>2.4255167619079917E-2</v>
+        <v>2.4141364702705441E-2</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="3"/>
-        <v>1.3202575457040642</v>
+        <v>1.3202918185626553</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1465,30 +1625,30 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>12035</v>
+        <v>12927</v>
       </c>
       <c r="C23" s="2">
-        <v>996</v>
+        <v>984</v>
       </c>
       <c r="D23">
         <f t="shared" si="7"/>
-        <v>13031</v>
+        <v>13911</v>
       </c>
       <c r="E23" s="2">
         <f>D2</f>
-        <v>294865</v>
+        <v>296255</v>
       </c>
       <c r="F23" s="2">
         <f>D2</f>
-        <v>294865</v>
+        <v>296255</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="6"/>
-        <v>22.627964085641931</v>
+        <v>21.296456041981166</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="1"/>
-        <v>24.500623182384711</v>
+        <v>22.917536938191382</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="2"/>
@@ -1496,7 +1656,7 @@
       </c>
       <c r="J23" s="1">
         <f t="shared" si="3"/>
-        <v>1.3202575457040642</v>
+        <v>1.3202918185626553</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1505,37 +1665,37 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>9625</v>
+        <v>11079</v>
       </c>
       <c r="C24" s="2">
-        <v>3113</v>
+        <v>3064</v>
       </c>
       <c r="D24">
         <f t="shared" si="7"/>
-        <v>12738</v>
+        <v>14143</v>
       </c>
       <c r="E24" s="2">
         <v>4120</v>
       </c>
       <c r="F24" s="2">
         <f>D2</f>
-        <v>294865</v>
+        <v>296255</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="6"/>
-        <v>0.32344167059192969</v>
+        <v>0.29131018878597187</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="1"/>
-        <v>30.635324675324675</v>
+        <v>26.740229262568825</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="2"/>
-        <v>1.3972495887948723E-2</v>
+        <v>1.3906938279522708E-2</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="3"/>
-        <v>1.3202575457040642</v>
+        <v>1.3202918185626553</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1544,37 +1704,37 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>3041</v>
+        <v>7686</v>
       </c>
       <c r="C25" s="2">
-        <v>4209</v>
+        <v>4894</v>
       </c>
       <c r="D25">
         <f t="shared" si="7"/>
-        <v>7250</v>
+        <v>12580</v>
       </c>
       <c r="E25" s="2">
         <v>6788</v>
       </c>
       <c r="F25" s="2">
         <f>D2</f>
-        <v>294865</v>
+        <v>296255</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="6"/>
-        <v>0.93627586206896551</v>
+        <v>0.53958664546899837</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="1"/>
-        <v>96.963170009865181</v>
+        <v>38.544756700494403</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="2"/>
-        <v>2.3020704390144642E-2</v>
+        <v>2.2912693456650521E-2</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="3"/>
-        <v>1.3202575457040642</v>
+        <v>1.3202918185626553</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -1582,33 +1742,42 @@
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" t="str">
+      <c r="B26" s="2">
+        <v>6193</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2216</v>
+      </c>
+      <c r="D26">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="1" t="str">
+        <v>8409</v>
+      </c>
+      <c r="E26" s="2">
+        <v>8332</v>
+      </c>
+      <c r="F26" s="2">
+        <f>D2</f>
+        <v>296255</v>
+      </c>
+      <c r="G26" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I26" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J26" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.99084314425020814</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
+        <v>47.837074115937348</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="2"/>
+        <v>2.8124419841015342E-2</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3202918185626553</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection sheet="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="E2:F26">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -1622,7 +1791,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -2741,10 +2910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
-  <dimension ref="A1:CX20"/>
+  <dimension ref="A1:CX21"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="CT12" sqref="CT12"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6167,13 +6336,13 @@
         <v>31</v>
       </c>
       <c r="CT12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="CU12" t="s">
         <v>32</v>
       </c>
       <c r="CV12" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="CW12" t="s">
         <v>32</v>
@@ -6232,32 +6401,63 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" t="s">
         <v>20</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6274,72 +6474,53 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
       <formula>"s"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
       <formula>"f"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"t"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"h"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7229,7 +7410,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -8194,7 +8375,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -9249,7 +9430,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -10259,7 +10440,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
2023 Day 22 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E04E87D-5D45-4D1B-A5A9-BAC5AD764E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553EE87E-402C-4192-9B50-A474B40E289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="660" windowWidth="16890" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="660" windowWidth="16890" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="37">
   <si>
     <t>Day</t>
   </si>
@@ -120,9 +120,6 @@
     <t>not done yet</t>
   </si>
   <si>
-    <t>Excuse</t>
-  </si>
-  <si>
     <t>Hillwalking</t>
   </si>
   <si>
@@ -139,6 +136,15 @@
   </si>
   <si>
     <t>done, but horrible</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Xmas do</t>
   </si>
 </sst>
 </file>
@@ -240,21 +246,34 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="13">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -330,156 +349,6 @@
           <bgColor rgb="FF7030A0"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF24B850"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF24B850"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF24B850"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF24B850"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFC000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -770,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -813,7 +682,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -852,6 +721,7 @@
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
         <v>9.1618906705409425E-2</v>
       </c>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
@@ -890,6 +760,7 @@
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
         <v>0.13194227803873682</v>
       </c>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
@@ -928,8 +799,8 @@
         <f t="shared" si="3"/>
         <v>0.25406219639371441</v>
       </c>
-      <c r="K4" t="s">
-        <v>29</v>
+      <c r="K4" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -969,6 +840,7 @@
         <f t="shared" si="3"/>
         <v>0.11715080263474548</v>
       </c>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -1007,6 +879,7 @@
         <f t="shared" si="3"/>
         <v>6.7294751009421269E-2</v>
       </c>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -1045,6 +918,7 @@
         <f t="shared" si="3"/>
         <v>0.1042533847922776</v>
       </c>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -1083,6 +957,7 @@
         <f t="shared" si="3"/>
         <v>8.0147602791618019E-2</v>
       </c>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -1121,6 +996,7 @@
         <f t="shared" si="3"/>
         <v>6.3016409223391828E-2</v>
       </c>
+      <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -1159,6 +1035,7 @@
         <f t="shared" si="3"/>
         <v>8.4840408938169048E-2</v>
       </c>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -1197,6 +1074,7 @@
         <f t="shared" si="3"/>
         <v>5.1883807367661086E-2</v>
       </c>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -1235,6 +1113,7 @@
         <f t="shared" si="3"/>
         <v>5.1750109186847665E-2</v>
       </c>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -1274,6 +1153,7 @@
         <f t="shared" si="3"/>
         <v>1.3202918185626553</v>
       </c>
+      <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -1312,6 +1192,7 @@
         <f t="shared" si="3"/>
         <v>8.1506867629887778E-2</v>
       </c>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -1351,6 +1232,9 @@
         <f t="shared" si="3"/>
         <v>1.3202918185626553</v>
       </c>
+      <c r="K15" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -1389,8 +1273,9 @@
         <f t="shared" si="3"/>
         <v>0.10713680889182034</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -1427,8 +1312,9 @@
         <f t="shared" si="3"/>
         <v>4.0684356421523626E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -1465,8 +1351,9 @@
         <f t="shared" si="3"/>
         <v>3.4730330769299329E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -1503,8 +1390,9 @@
         <f t="shared" si="3"/>
         <v>4.6072393108304438E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <f t="shared" si="4"/>
         <v>19</v>
@@ -1541,8 +1429,9 @@
         <f t="shared" si="3"/>
         <v>3.9200306614494668E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -1579,8 +1468,9 @@
         <f t="shared" si="3"/>
         <v>3.342008859732782E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <f t="shared" si="4"/>
         <v>21</v>
@@ -1618,8 +1508,11 @@
         <f t="shared" si="3"/>
         <v>1.3202918185626553</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <f t="shared" si="4"/>
         <v>22</v>
@@ -1635,31 +1528,30 @@
         <v>13911</v>
       </c>
       <c r="E23" s="2">
-        <f>D2</f>
-        <v>296255</v>
+        <v>14576</v>
       </c>
       <c r="F23" s="2">
-        <f>D2</f>
-        <v>296255</v>
+        <v>13641</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="6"/>
-        <v>21.296456041981166</v>
+        <v>1.047803896197254</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="1"/>
-        <v>22.917536938191382</v>
+        <v>1.0552332327686238</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>4.9200857369495872E-2</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="3"/>
-        <v>1.3202918185626553</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+        <v>6.0792562815861949E-2</v>
+      </c>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <f t="shared" si="4"/>
         <v>23</v>
@@ -1697,8 +1589,9 @@
         <f t="shared" si="3"/>
         <v>1.3202918185626553</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <f t="shared" si="4"/>
         <v>24</v>
@@ -1736,8 +1629,9 @@
         <f t="shared" si="3"/>
         <v>1.3202918185626553</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <f t="shared" si="4"/>
         <v>25</v>
@@ -1775,6 +1669,7 @@
         <f t="shared" si="3"/>
         <v>1.3202918185626553</v>
       </c>
+      <c r="K26" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" selectLockedCells="1"/>
@@ -1791,7 +1686,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -1830,6 +1725,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2912,8 +2808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="BV13" sqref="BV13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2924,358 +2820,358 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:102" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="11">
+      <c r="B1" s="12">
         <v>1</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12">
         <v>2</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12">
         <v>3</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12">
         <v>4</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11">
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12">
         <v>5</v>
       </c>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11">
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12">
         <v>6</v>
       </c>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11">
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12">
         <v>7</v>
       </c>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11">
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12">
         <v>8</v>
       </c>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11">
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12">
         <v>9</v>
       </c>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11">
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12">
         <v>10</v>
       </c>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="11"/>
-      <c r="AO1" s="11"/>
-      <c r="AP1" s="11">
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12">
         <v>11</v>
       </c>
-      <c r="AQ1" s="11"/>
-      <c r="AR1" s="11"/>
-      <c r="AS1" s="11"/>
-      <c r="AT1" s="11">
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12">
         <v>12</v>
       </c>
-      <c r="AU1" s="11"/>
-      <c r="AV1" s="11"/>
-      <c r="AW1" s="11"/>
-      <c r="AX1" s="11">
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12">
         <v>13</v>
       </c>
-      <c r="AY1" s="11"/>
-      <c r="AZ1" s="11"/>
-      <c r="BA1" s="11"/>
-      <c r="BB1" s="11">
-        <v>14</v>
-      </c>
-      <c r="BC1" s="11"/>
-      <c r="BD1" s="11"/>
-      <c r="BE1" s="11"/>
-      <c r="BF1" s="11">
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12">
+        <v>14</v>
+      </c>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12">
         <v>15</v>
       </c>
-      <c r="BG1" s="11"/>
-      <c r="BH1" s="11"/>
-      <c r="BI1" s="11"/>
-      <c r="BJ1" s="11">
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12">
         <v>16</v>
       </c>
-      <c r="BK1" s="11"/>
-      <c r="BL1" s="11"/>
-      <c r="BM1" s="11"/>
-      <c r="BN1" s="11">
+      <c r="BK1" s="12"/>
+      <c r="BL1" s="12"/>
+      <c r="BM1" s="12"/>
+      <c r="BN1" s="12">
         <v>17</v>
       </c>
-      <c r="BO1" s="11"/>
-      <c r="BP1" s="11"/>
-      <c r="BQ1" s="11"/>
-      <c r="BR1" s="11">
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
+      <c r="BR1" s="12">
         <v>18</v>
       </c>
-      <c r="BS1" s="11"/>
-      <c r="BT1" s="11"/>
-      <c r="BU1" s="11"/>
-      <c r="BV1" s="11">
+      <c r="BS1" s="12"/>
+      <c r="BT1" s="12"/>
+      <c r="BU1" s="12"/>
+      <c r="BV1" s="12">
         <v>19</v>
       </c>
-      <c r="BW1" s="11"/>
-      <c r="BX1" s="11"/>
-      <c r="BY1" s="11"/>
-      <c r="BZ1" s="11">
+      <c r="BW1" s="12"/>
+      <c r="BX1" s="12"/>
+      <c r="BY1" s="12"/>
+      <c r="BZ1" s="12">
         <v>20</v>
       </c>
-      <c r="CA1" s="11"/>
-      <c r="CB1" s="11"/>
-      <c r="CC1" s="11"/>
-      <c r="CD1" s="11">
+      <c r="CA1" s="12"/>
+      <c r="CB1" s="12"/>
+      <c r="CC1" s="12"/>
+      <c r="CD1" s="12">
         <v>21</v>
       </c>
-      <c r="CE1" s="11"/>
-      <c r="CF1" s="11"/>
-      <c r="CG1" s="11"/>
-      <c r="CH1" s="11">
+      <c r="CE1" s="12"/>
+      <c r="CF1" s="12"/>
+      <c r="CG1" s="12"/>
+      <c r="CH1" s="12">
         <v>22</v>
       </c>
-      <c r="CI1" s="11"/>
-      <c r="CJ1" s="11"/>
-      <c r="CK1" s="11"/>
-      <c r="CL1" s="11">
+      <c r="CI1" s="12"/>
+      <c r="CJ1" s="12"/>
+      <c r="CK1" s="12"/>
+      <c r="CL1" s="12">
         <v>23</v>
       </c>
-      <c r="CM1" s="11"/>
-      <c r="CN1" s="11"/>
-      <c r="CO1" s="11"/>
-      <c r="CP1" s="11">
+      <c r="CM1" s="12"/>
+      <c r="CN1" s="12"/>
+      <c r="CO1" s="12"/>
+      <c r="CP1" s="12">
         <v>24</v>
       </c>
-      <c r="CQ1" s="11"/>
-      <c r="CR1" s="11"/>
-      <c r="CS1" s="11"/>
-      <c r="CT1" s="11">
+      <c r="CQ1" s="12"/>
+      <c r="CR1" s="12"/>
+      <c r="CS1" s="12"/>
+      <c r="CT1" s="12">
         <v>25</v>
       </c>
-      <c r="CU1" s="11"/>
-      <c r="CV1" s="11"/>
-      <c r="CW1" s="11"/>
+      <c r="CU1" s="12"/>
+      <c r="CV1" s="12"/>
+      <c r="CW1" s="12"/>
     </row>
     <row r="2" spans="1:102" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11" t="s">
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11" t="s">
+      <c r="S2" s="12"/>
+      <c r="T2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11" t="s">
+      <c r="U2" s="12"/>
+      <c r="V2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11" t="s">
+      <c r="W2" s="12"/>
+      <c r="X2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11" t="s">
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11" t="s">
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11" t="s">
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11" t="s">
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11" t="s">
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11" t="s">
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11" t="s">
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="11" t="s">
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="11" t="s">
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AQ2" s="11"/>
-      <c r="AR2" s="11" t="s">
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AS2" s="11"/>
-      <c r="AT2" s="11" t="s">
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AU2" s="11"/>
-      <c r="AV2" s="11" t="s">
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AW2" s="11"/>
-      <c r="AX2" s="11" t="s">
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AY2" s="11"/>
-      <c r="AZ2" s="11" t="s">
+      <c r="AY2" s="12"/>
+      <c r="AZ2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BA2" s="11"/>
-      <c r="BB2" s="11" t="s">
+      <c r="BA2" s="12"/>
+      <c r="BB2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BC2" s="11"/>
-      <c r="BD2" s="11" t="s">
+      <c r="BC2" s="12"/>
+      <c r="BD2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BE2" s="11"/>
-      <c r="BF2" s="11" t="s">
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BG2" s="11"/>
-      <c r="BH2" s="11" t="s">
+      <c r="BG2" s="12"/>
+      <c r="BH2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BI2" s="11"/>
-      <c r="BJ2" s="11" t="s">
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BK2" s="11"/>
-      <c r="BL2" s="11" t="s">
+      <c r="BK2" s="12"/>
+      <c r="BL2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BM2" s="11"/>
-      <c r="BN2" s="11" t="s">
+      <c r="BM2" s="12"/>
+      <c r="BN2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BO2" s="11"/>
-      <c r="BP2" s="11" t="s">
+      <c r="BO2" s="12"/>
+      <c r="BP2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BQ2" s="11"/>
-      <c r="BR2" s="11" t="s">
+      <c r="BQ2" s="12"/>
+      <c r="BR2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BS2" s="11"/>
-      <c r="BT2" s="11" t="s">
+      <c r="BS2" s="12"/>
+      <c r="BT2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BU2" s="11"/>
-      <c r="BV2" s="11" t="s">
+      <c r="BU2" s="12"/>
+      <c r="BV2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BW2" s="11"/>
-      <c r="BX2" s="11" t="s">
+      <c r="BW2" s="12"/>
+      <c r="BX2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BY2" s="11"/>
-      <c r="BZ2" s="11" t="s">
+      <c r="BY2" s="12"/>
+      <c r="BZ2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CA2" s="11"/>
-      <c r="CB2" s="11" t="s">
+      <c r="CA2" s="12"/>
+      <c r="CB2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CC2" s="11"/>
-      <c r="CD2" s="11" t="s">
+      <c r="CC2" s="12"/>
+      <c r="CD2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CE2" s="11"/>
-      <c r="CF2" s="11" t="s">
+      <c r="CE2" s="12"/>
+      <c r="CF2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CG2" s="11"/>
-      <c r="CH2" s="11" t="s">
+      <c r="CG2" s="12"/>
+      <c r="CH2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CI2" s="11"/>
-      <c r="CJ2" s="11" t="s">
+      <c r="CI2" s="12"/>
+      <c r="CJ2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CK2" s="11"/>
-      <c r="CL2" s="11" t="s">
+      <c r="CK2" s="12"/>
+      <c r="CL2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CM2" s="11"/>
-      <c r="CN2" s="11" t="s">
+      <c r="CM2" s="12"/>
+      <c r="CN2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CO2" s="11"/>
-      <c r="CP2" s="11" t="s">
+      <c r="CO2" s="12"/>
+      <c r="CP2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CQ2" s="11"/>
-      <c r="CR2" s="11" t="s">
+      <c r="CQ2" s="12"/>
+      <c r="CR2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CS2" s="11"/>
-      <c r="CT2" s="11" t="s">
+      <c r="CS2" s="12"/>
+      <c r="CT2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CU2" s="11"/>
-      <c r="CV2" s="11" t="s">
+      <c r="CU2" s="12"/>
+      <c r="CV2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CW2" s="11"/>
+      <c r="CW2" s="12"/>
     </row>
     <row r="3" spans="1:102" x14ac:dyDescent="0.55000000000000004">
       <c r="B3">
@@ -6183,13 +6079,13 @@
         <v>14</v>
       </c>
       <c r="AU12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AV12" t="s">
         <v>14</v>
       </c>
       <c r="AW12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AX12" t="s">
         <v>14</v>
@@ -6207,13 +6103,13 @@
         <v>14</v>
       </c>
       <c r="BC12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BD12" t="s">
         <v>14</v>
       </c>
       <c r="BE12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="BF12" t="s">
         <v>14</v>
@@ -6291,61 +6187,61 @@
         <v>14</v>
       </c>
       <c r="CE12" t="s">
+        <v>30</v>
+      </c>
+      <c r="CF12" t="s">
+        <v>14</v>
+      </c>
+      <c r="CG12" t="s">
+        <v>30</v>
+      </c>
+      <c r="CH12" t="s">
+        <v>29</v>
+      </c>
+      <c r="CI12" t="s">
+        <v>14</v>
+      </c>
+      <c r="CJ12" t="s">
+        <v>29</v>
+      </c>
+      <c r="CK12" t="s">
+        <v>14</v>
+      </c>
+      <c r="CL12" t="s">
+        <v>29</v>
+      </c>
+      <c r="CM12" t="s">
+        <v>30</v>
+      </c>
+      <c r="CN12" t="s">
+        <v>29</v>
+      </c>
+      <c r="CO12" t="s">
+        <v>30</v>
+      </c>
+      <c r="CP12" t="s">
+        <v>29</v>
+      </c>
+      <c r="CQ12" t="s">
+        <v>30</v>
+      </c>
+      <c r="CR12" t="s">
+        <v>29</v>
+      </c>
+      <c r="CS12" t="s">
+        <v>30</v>
+      </c>
+      <c r="CT12" t="s">
+        <v>14</v>
+      </c>
+      <c r="CU12" t="s">
         <v>31</v>
       </c>
-      <c r="CF12" t="s">
-        <v>14</v>
-      </c>
-      <c r="CG12" t="s">
+      <c r="CV12" t="s">
+        <v>32</v>
+      </c>
+      <c r="CW12" t="s">
         <v>31</v>
-      </c>
-      <c r="CH12" t="s">
-        <v>30</v>
-      </c>
-      <c r="CI12" t="s">
-        <v>31</v>
-      </c>
-      <c r="CJ12" t="s">
-        <v>30</v>
-      </c>
-      <c r="CK12" t="s">
-        <v>31</v>
-      </c>
-      <c r="CL12" t="s">
-        <v>30</v>
-      </c>
-      <c r="CM12" t="s">
-        <v>31</v>
-      </c>
-      <c r="CN12" t="s">
-        <v>30</v>
-      </c>
-      <c r="CO12" t="s">
-        <v>31</v>
-      </c>
-      <c r="CP12" t="s">
-        <v>30</v>
-      </c>
-      <c r="CQ12" t="s">
-        <v>31</v>
-      </c>
-      <c r="CR12" t="s">
-        <v>30</v>
-      </c>
-      <c r="CS12" t="s">
-        <v>31</v>
-      </c>
-      <c r="CT12" t="s">
-        <v>14</v>
-      </c>
-      <c r="CU12" t="s">
-        <v>32</v>
-      </c>
-      <c r="CV12" t="s">
-        <v>33</v>
-      </c>
-      <c r="CW12" t="s">
-        <v>32</v>
       </c>
       <c r="CX12">
         <v>2023</v>
@@ -6401,10 +6297,10 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.55000000000000004">
@@ -6417,47 +6313,24 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6474,49 +6347,72 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"h"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="equal">
       <formula>"s"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="equal">
       <formula>"f"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" stopIfTrue="1" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"t"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
-      <formula>"h"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7410,7 +7306,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -8375,7 +8271,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="25" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -9430,7 +9326,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -10440,7 +10336,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
2023 Day 23 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553EE87E-402C-4192-9B50-A474B40E289C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8657D31-60E1-4620-9423-4B8459F1635F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2190" yWindow="660" windowWidth="16890" windowHeight="11958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2190" yWindow="660" windowWidth="16890" windowHeight="11958" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="38">
   <si>
     <t>Day</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Xmas do</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -639,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221F9016-2A40-4C0A-A371-63EB68CE326F}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1570,8 +1573,7 @@
         <v>4120</v>
       </c>
       <c r="F24" s="2">
-        <f>D2</f>
-        <v>296255</v>
+        <v>13297</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="6"/>
@@ -1579,7 +1581,7 @@
       </c>
       <c r="H24" s="1">
         <f t="shared" si="1"/>
-        <v>26.740229262568825</v>
+        <v>1.2001985738785088</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="2"/>
@@ -1587,7 +1589,7 @@
       </c>
       <c r="J24" s="1">
         <f t="shared" si="3"/>
-        <v>1.3202918185626553</v>
+        <v>5.9259490342534742E-2</v>
       </c>
       <c r="K24" s="2"/>
     </row>
@@ -2808,8 +2810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CX21"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="BV13" sqref="BV13"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="CV12" sqref="CV12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6103,13 +6105,13 @@
         <v>14</v>
       </c>
       <c r="BC12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="BD12" t="s">
         <v>14</v>
       </c>
       <c r="BE12" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="BF12" t="s">
         <v>14</v>
@@ -6211,13 +6213,13 @@
         <v>29</v>
       </c>
       <c r="CM12" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="CN12" t="s">
         <v>29</v>
       </c>
       <c r="CO12" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="CP12" t="s">
         <v>29</v>
@@ -6313,24 +6315,47 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -6347,47 +6372,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW12">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">

</xml_diff>

<commit_message>
2024 Day 06 Done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC09861-B61E-4802-B32C-389C2C851651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1768D3-E402-4ECE-8AA9-F37F686A1AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2538" yWindow="1014" windowWidth="8460" windowHeight="11502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="12" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="39">
   <si>
     <t>Day</t>
   </si>
@@ -259,11 +259,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -271,13 +271,28 @@
   <dxfs count="14">
     <dxf>
       <font>
-        <color rgb="FF7030A0"/>
+        <color theme="0"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -346,28 +361,13 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
+        <color rgb="FF7030A0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AA6AC8-5A6F-44C5-8B15-8AB7181E67FD}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -709,14 +709,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>165920</v>
+        <v>179708</v>
       </c>
       <c r="C2" s="2">
-        <v>11763</v>
+        <v>12686</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>177683</v>
+        <v>192394</v>
       </c>
       <c r="E2" s="2">
         <v>14511</v>
@@ -726,19 +726,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>8.1667914206761477E-2</v>
+        <v>7.5423350000519765E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>8.4637174541947927E-2</v>
+        <v>7.8143432679680366E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>8.1667914206761477E-2</v>
+        <v>7.5423350000519765E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>8.4637174541947927E-2</v>
+        <v>7.8143432679680366E-2</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -748,14 +748,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>111601</v>
+        <v>123482</v>
       </c>
       <c r="C3" s="2">
-        <v>28689</v>
+        <v>30858</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>140290</v>
+        <v>154340</v>
       </c>
       <c r="E3" s="2">
         <v>24905</v>
@@ -765,19 +765,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.17752512652362962</v>
+        <v>0.16136451989114942</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.34545389378231378</v>
+        <v>0.31221554558559145</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.14016535065256666</v>
+        <v>0.12944790378078319</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.2323589681774349</v>
+        <v>0.21453135085805863</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
@@ -789,14 +789,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>92271</v>
+        <v>107754</v>
       </c>
       <c r="C4" s="2">
-        <v>10992</v>
+        <v>11741</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>103263</v>
+        <v>119495</v>
       </c>
       <c r="E4" s="2">
         <v>30159</v>
@@ -806,19 +806,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.29206007960256819</v>
+        <v>0.25238712916858447</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.27149375209979298</v>
+        <v>0.23248324888171204</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.16973486489984974</v>
+        <v>0.15675644770626943</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.1509824011571842</v>
+        <v>0.1393983573352327</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -828,14 +828,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>15523</v>
+        <v>77556</v>
       </c>
       <c r="C5" s="2">
-        <v>3679</v>
+        <v>7559</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>19202</v>
+        <v>85115</v>
       </c>
       <c r="E5" s="2">
         <v>17872</v>
@@ -845,19 +845,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.93073638162691386</v>
+        <v>0.20997474005756916</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.9821555111769632</v>
+        <v>0.19658053535509826</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>0.1005836236443554</v>
+        <v>9.2892709751863367E-2</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>9.1887656702025075E-2</v>
+        <v>8.4837625481336387E-2</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -866,29 +866,37 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" t="str">
+      <c r="B6" s="2">
+        <v>30697</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8767</v>
+      </c>
+      <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v/>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="1" t="str">
+        <v>39464</v>
+      </c>
+      <c r="E6" s="2">
+        <v>25203</v>
+      </c>
+      <c r="F6" s="2">
+        <v>27047</v>
+      </c>
+      <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I6" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J6" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.63863267788364075</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.88109587256083655</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="2"/>
+        <v>0.13099680863228583</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="3"/>
+        <v>0.15050526409508758</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -3701,7 +3709,7 @@
   <dimension ref="A1:CZ22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3712,358 +3720,358 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:104" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="10">
+      <c r="B1" s="12">
         <v>1</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12">
         <v>2</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12">
         <v>3</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12">
         <v>4</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10">
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12">
         <v>5</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10">
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12">
         <v>6</v>
       </c>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10">
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12">
         <v>7</v>
       </c>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10">
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12">
         <v>8</v>
       </c>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10">
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12">
         <v>9</v>
       </c>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10">
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12">
         <v>10</v>
       </c>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10">
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12">
         <v>11</v>
       </c>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10">
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12">
         <v>12</v>
       </c>
-      <c r="AU1" s="10"/>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10">
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12">
         <v>13</v>
       </c>
-      <c r="AY1" s="10"/>
-      <c r="AZ1" s="10"/>
-      <c r="BA1" s="10"/>
-      <c r="BB1" s="10">
-        <v>14</v>
-      </c>
-      <c r="BC1" s="10"/>
-      <c r="BD1" s="10"/>
-      <c r="BE1" s="10"/>
-      <c r="BF1" s="10">
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12">
+        <v>14</v>
+      </c>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12">
         <v>15</v>
       </c>
-      <c r="BG1" s="10"/>
-      <c r="BH1" s="10"/>
-      <c r="BI1" s="10"/>
-      <c r="BJ1" s="10">
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12">
         <v>16</v>
       </c>
-      <c r="BK1" s="10"/>
-      <c r="BL1" s="10"/>
-      <c r="BM1" s="10"/>
-      <c r="BN1" s="10">
+      <c r="BK1" s="12"/>
+      <c r="BL1" s="12"/>
+      <c r="BM1" s="12"/>
+      <c r="BN1" s="12">
         <v>17</v>
       </c>
-      <c r="BO1" s="10"/>
-      <c r="BP1" s="10"/>
-      <c r="BQ1" s="10"/>
-      <c r="BR1" s="10">
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
+      <c r="BR1" s="12">
         <v>18</v>
       </c>
-      <c r="BS1" s="10"/>
-      <c r="BT1" s="10"/>
-      <c r="BU1" s="10"/>
-      <c r="BV1" s="10">
+      <c r="BS1" s="12"/>
+      <c r="BT1" s="12"/>
+      <c r="BU1" s="12"/>
+      <c r="BV1" s="12">
         <v>19</v>
       </c>
-      <c r="BW1" s="10"/>
-      <c r="BX1" s="10"/>
-      <c r="BY1" s="10"/>
-      <c r="BZ1" s="10">
+      <c r="BW1" s="12"/>
+      <c r="BX1" s="12"/>
+      <c r="BY1" s="12"/>
+      <c r="BZ1" s="12">
         <v>20</v>
       </c>
-      <c r="CA1" s="10"/>
-      <c r="CB1" s="10"/>
-      <c r="CC1" s="10"/>
-      <c r="CD1" s="10">
+      <c r="CA1" s="12"/>
+      <c r="CB1" s="12"/>
+      <c r="CC1" s="12"/>
+      <c r="CD1" s="12">
         <v>21</v>
       </c>
-      <c r="CE1" s="10"/>
-      <c r="CF1" s="10"/>
-      <c r="CG1" s="10"/>
-      <c r="CH1" s="10">
+      <c r="CE1" s="12"/>
+      <c r="CF1" s="12"/>
+      <c r="CG1" s="12"/>
+      <c r="CH1" s="12">
         <v>22</v>
       </c>
-      <c r="CI1" s="10"/>
-      <c r="CJ1" s="10"/>
-      <c r="CK1" s="10"/>
-      <c r="CL1" s="10">
+      <c r="CI1" s="12"/>
+      <c r="CJ1" s="12"/>
+      <c r="CK1" s="12"/>
+      <c r="CL1" s="12">
         <v>23</v>
       </c>
-      <c r="CM1" s="10"/>
-      <c r="CN1" s="10"/>
-      <c r="CO1" s="10"/>
-      <c r="CP1" s="10">
+      <c r="CM1" s="12"/>
+      <c r="CN1" s="12"/>
+      <c r="CO1" s="12"/>
+      <c r="CP1" s="12">
         <v>24</v>
       </c>
-      <c r="CQ1" s="10"/>
-      <c r="CR1" s="10"/>
-      <c r="CS1" s="10"/>
-      <c r="CT1" s="10">
+      <c r="CQ1" s="12"/>
+      <c r="CR1" s="12"/>
+      <c r="CS1" s="12"/>
+      <c r="CT1" s="12">
         <v>25</v>
       </c>
-      <c r="CU1" s="10"/>
-      <c r="CV1" s="10"/>
-      <c r="CW1" s="10"/>
+      <c r="CU1" s="12"/>
+      <c r="CV1" s="12"/>
+      <c r="CW1" s="12"/>
     </row>
     <row r="2" spans="1:104" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10" t="s">
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10" t="s">
+      <c r="O2" s="12"/>
+      <c r="P2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10" t="s">
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10" t="s">
+      <c r="S2" s="12"/>
+      <c r="T2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10" t="s">
+      <c r="U2" s="12"/>
+      <c r="V2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10" t="s">
+      <c r="W2" s="12"/>
+      <c r="X2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10" t="s">
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10" t="s">
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10" t="s">
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10" t="s">
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10" t="s">
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10" t="s">
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10" t="s">
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10" t="s">
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10" t="s">
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AQ2" s="10"/>
-      <c r="AR2" s="10" t="s">
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="10" t="s">
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AU2" s="10"/>
-      <c r="AV2" s="10" t="s">
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="AW2" s="10"/>
-      <c r="AX2" s="10" t="s">
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="AY2" s="10"/>
-      <c r="AZ2" s="10" t="s">
+      <c r="AY2" s="12"/>
+      <c r="AZ2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BA2" s="10"/>
-      <c r="BB2" s="10" t="s">
+      <c r="BA2" s="12"/>
+      <c r="BB2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BC2" s="10"/>
-      <c r="BD2" s="10" t="s">
+      <c r="BC2" s="12"/>
+      <c r="BD2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BE2" s="10"/>
-      <c r="BF2" s="10" t="s">
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BG2" s="10"/>
-      <c r="BH2" s="10" t="s">
+      <c r="BG2" s="12"/>
+      <c r="BH2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BI2" s="10"/>
-      <c r="BJ2" s="10" t="s">
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BK2" s="10"/>
-      <c r="BL2" s="10" t="s">
+      <c r="BK2" s="12"/>
+      <c r="BL2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BM2" s="10"/>
-      <c r="BN2" s="10" t="s">
+      <c r="BM2" s="12"/>
+      <c r="BN2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BO2" s="10"/>
-      <c r="BP2" s="10" t="s">
+      <c r="BO2" s="12"/>
+      <c r="BP2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BQ2" s="10"/>
-      <c r="BR2" s="10" t="s">
+      <c r="BQ2" s="12"/>
+      <c r="BR2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BS2" s="10"/>
-      <c r="BT2" s="10" t="s">
+      <c r="BS2" s="12"/>
+      <c r="BT2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BU2" s="10"/>
-      <c r="BV2" s="10" t="s">
+      <c r="BU2" s="12"/>
+      <c r="BV2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="BW2" s="10"/>
-      <c r="BX2" s="10" t="s">
+      <c r="BW2" s="12"/>
+      <c r="BX2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BY2" s="10"/>
-      <c r="BZ2" s="10" t="s">
+      <c r="BY2" s="12"/>
+      <c r="BZ2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CA2" s="10"/>
-      <c r="CB2" s="10" t="s">
+      <c r="CA2" s="12"/>
+      <c r="CB2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CC2" s="10"/>
-      <c r="CD2" s="10" t="s">
+      <c r="CC2" s="12"/>
+      <c r="CD2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CE2" s="10"/>
-      <c r="CF2" s="10" t="s">
+      <c r="CE2" s="12"/>
+      <c r="CF2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CG2" s="10"/>
-      <c r="CH2" s="10" t="s">
+      <c r="CG2" s="12"/>
+      <c r="CH2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CI2" s="10"/>
-      <c r="CJ2" s="10" t="s">
+      <c r="CI2" s="12"/>
+      <c r="CJ2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CK2" s="10"/>
-      <c r="CL2" s="10" t="s">
+      <c r="CK2" s="12"/>
+      <c r="CL2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CM2" s="10"/>
-      <c r="CN2" s="10" t="s">
+      <c r="CM2" s="12"/>
+      <c r="CN2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CO2" s="10"/>
-      <c r="CP2" s="10" t="s">
+      <c r="CO2" s="12"/>
+      <c r="CP2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CQ2" s="10"/>
-      <c r="CR2" s="10" t="s">
+      <c r="CQ2" s="12"/>
+      <c r="CR2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CS2" s="10"/>
-      <c r="CT2" s="10" t="s">
+      <c r="CS2" s="12"/>
+      <c r="CT2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="CU2" s="10"/>
-      <c r="CV2" s="10" t="s">
+      <c r="CU2" s="12"/>
+      <c r="CV2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="CW2" s="10"/>
+      <c r="CW2" s="12"/>
     </row>
     <row r="3" spans="1:104" x14ac:dyDescent="0.55000000000000004">
       <c r="B3">
@@ -7173,8 +7181,12 @@
       <c r="I13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="J13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -7283,7 +7295,7 @@
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="1:104" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
@@ -7331,7 +7343,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D21" t="s">
@@ -7349,24 +7361,47 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -7383,71 +7418,48 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW13">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"u"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="equal">
       <formula>"s"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="equal">
       <formula>"f"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" stopIfTrue="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" stopIfTrue="1" operator="equal">
       <formula>"p"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
       <formula>"n"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"t"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8506,7 +8518,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -9435,7 +9447,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="11" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -10400,7 +10412,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H26">
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -11455,7 +11467,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -12465,7 +12477,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:H1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">

</xml_diff>

<commit_message>
2024 Day 07 Done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E432CA2-C97D-4FB2-B9D2-91090EC91DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755CB549-C7E9-4175-A904-30EC2D87A63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1326" yWindow="690" windowWidth="8460" windowHeight="11502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1326" yWindow="690" windowWidth="8460" windowHeight="11502" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="12" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="39">
   <si>
     <t>Day</t>
   </si>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AA6AC8-5A6F-44C5-8B15-8AB7181E67FD}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -709,14 +709,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>187181</v>
+        <v>193538</v>
       </c>
       <c r="C2" s="2">
-        <v>13385</v>
+        <v>13865</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>200566</v>
+        <v>207403</v>
       </c>
       <c r="E2" s="2">
         <v>14511</v>
@@ -726,19 +726,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>7.2350248795907582E-2</v>
+        <v>6.9965236761281177E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>7.5023640219894119E-2</v>
+        <v>7.2559394020812448E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>7.2350248795907582E-2</v>
+        <v>6.9965236761281177E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>7.5023640219894119E-2</v>
+        <v>7.2559394020812448E-2</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -748,14 +748,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>129620</v>
+        <v>134673</v>
       </c>
       <c r="C3" s="2">
-        <v>32208</v>
+        <v>33498</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>161828</v>
+        <v>168171</v>
       </c>
       <c r="E3" s="2">
         <v>24905</v>
@@ -765,19 +765,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.15389796574140446</v>
+        <v>0.14809330978587271</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.29743095201357816</v>
+        <v>0.28627119021630171</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.1241735887438549</v>
+        <v>0.12008023027632195</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.20596641753169392</v>
+        <v>0.19920119046388823</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
@@ -789,14 +789,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>114614</v>
+        <v>119945</v>
       </c>
       <c r="C4" s="2">
-        <v>12297</v>
+        <v>12791</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>126911</v>
+        <v>132736</v>
       </c>
       <c r="E4" s="2">
         <v>30159</v>
@@ -806,19 +806,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.23763897534492676</v>
+        <v>0.22721040260366443</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.21856841223585252</v>
+        <v>0.20885405810996707</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.15036945444392369</v>
+        <v>0.14541255430249322</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.13383302792484281</v>
+        <v>0.12943711312507106</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -828,14 +828,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>87148</v>
+        <v>93001</v>
       </c>
       <c r="C5" s="2">
-        <v>7740</v>
+        <v>7972</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>94888</v>
+        <v>100973</v>
       </c>
       <c r="E5" s="2">
         <v>17872</v>
@@ -845,19 +845,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.18834836860298457</v>
+        <v>0.17699781129608905</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.17494377381007023</v>
+        <v>0.1639337211427834</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>8.9107824855658491E-2</v>
+        <v>8.6170402549625602E-2</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>8.1450574577547938E-2</v>
+        <v>7.8775227603881406E-2</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -867,14 +867,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>64301</v>
+        <v>72604</v>
       </c>
       <c r="C6" s="2">
-        <v>9650</v>
+        <v>9909</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>73951</v>
+        <v>82513</v>
       </c>
       <c r="E6" s="2">
         <v>25203</v>
@@ -884,19 +884,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.34080675041581587</v>
+        <v>0.30544277871365721</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.42063109438422419</v>
+        <v>0.37252768442510054</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>0.12565938394344006</v>
+        <v>0.12151704652295289</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>0.14449650338442471</v>
+        <v>0.13975033326788538</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -906,14 +906,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>16560</v>
+        <v>45889</v>
       </c>
       <c r="C7" s="2">
-        <v>14765</v>
+        <v>20257</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>31325</v>
+        <v>66146</v>
       </c>
       <c r="E7" s="2">
         <v>21682</v>
@@ -923,19 +923,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.69216280925778129</v>
+        <v>0.32779004021407188</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.92868357487922704</v>
+        <v>0.33513478175597639</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>0.10810406549465014</v>
+        <v>0.10454043576997439</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>8.2161116780015059E-2</v>
+        <v>7.9462431150471746E-2</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -944,29 +944,37 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" t="str">
+      <c r="B8" s="2">
+        <v>20638</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2565</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="1" t="str">
+        <v>23203</v>
+      </c>
+      <c r="E8" s="2">
+        <v>13716</v>
+      </c>
+      <c r="F8" s="2">
+        <v>15720</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J8" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.5911304572684567</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76170171528248865</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="2"/>
+        <v>6.6132119593255642E-2</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="3"/>
+        <v>8.1224359040601851E-2</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -3716,8 +3724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CZ22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7195,24 +7203,60 @@
       <c r="K13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2"/>
-      <c r="Y13" s="2"/>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
+      <c r="L13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
@@ -7369,24 +7413,47 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -7403,47 +7470,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW13">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">

</xml_diff>

<commit_message>
2024 Day 09 Done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C40171-9AB4-4B1C-B458-13F497741B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4746215B-2CDA-4BB4-BD50-C7C6A7C181DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1326" yWindow="690" windowWidth="8460" windowHeight="11502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="40">
   <si>
     <t>Day</t>
   </si>
@@ -662,7 +662,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -712,14 +712,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>198728</v>
+        <v>202439</v>
       </c>
       <c r="C2" s="2">
-        <v>14060</v>
+        <v>14242</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>212788</v>
+        <v>216681</v>
       </c>
       <c r="E2" s="2">
         <v>14511</v>
@@ -729,19 +729,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>6.8194635035810289E-2</v>
+        <v>6.6969415869411714E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>7.0664425747755721E-2</v>
+        <v>6.9369044502294516E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>6.8194635035810289E-2</v>
+        <v>6.6969415869411714E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>7.0664425747755721E-2</v>
+        <v>6.9369044502294516E-2</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -751,14 +751,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>139328</v>
+        <v>142709</v>
       </c>
       <c r="C3" s="2">
-        <v>34329</v>
+        <v>34815</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>173657</v>
+        <v>177524</v>
       </c>
       <c r="E3" s="2">
         <v>24905</v>
@@ -768,19 +768,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.14341489257559442</v>
+        <v>0.14029089024582592</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.27670676389526871</v>
+        <v>0.27015114673916851</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.11704137451360039</v>
+        <v>0.11493855021898551</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.19399883257517814</v>
+        <v>0.19044255306536784</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
@@ -792,14 +792,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>124852</v>
+        <v>128195</v>
       </c>
       <c r="C4" s="2">
-        <v>13152</v>
+        <v>13479</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>138004</v>
+        <v>141674</v>
       </c>
       <c r="E4" s="2">
         <v>30159</v>
@@ -809,19 +809,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.21853714385090287</v>
+        <v>0.21287603935796265</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.20064556434818825</v>
+        <v>0.19541323764577401</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.1417326165009305</v>
+        <v>0.13918617691445029</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.1260567207439314</v>
+        <v>0.12374591852360464</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -831,14 +831,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>98004</v>
+        <v>101422</v>
       </c>
       <c r="C5" s="2">
-        <v>8303</v>
+        <v>8547</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>106307</v>
+        <v>109969</v>
       </c>
       <c r="E5" s="2">
         <v>17872</v>
@@ -848,19 +848,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.16811686906788828</v>
+        <v>0.16251852794878557</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.15556507897636832</v>
+        <v>0.15032241525507287</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>8.3989698667218074E-2</v>
+        <v>8.2480697430785344E-2</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>7.6717926009419915E-2</v>
+        <v>7.5311575338744011E-2</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -870,14 +870,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>78220</v>
+        <v>81853</v>
       </c>
       <c r="C6" s="2">
-        <v>10160</v>
+        <v>10427</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>88380</v>
+        <v>92280</v>
       </c>
       <c r="E6" s="2">
         <v>25203</v>
@@ -887,19 +887,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.28516632722335372</v>
+        <v>0.27311443433029908</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.3457811301457428</v>
+        <v>0.33043382649383651</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>0.11844182942647141</v>
+        <v>0.11631384385340662</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>0.13610059981482228</v>
+        <v>0.13360567874767215</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -909,14 +909,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>54313</v>
+        <v>58651</v>
       </c>
       <c r="C7" s="2">
-        <v>20372</v>
+        <v>20749</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>74685</v>
+        <v>79400</v>
       </c>
       <c r="E7" s="2">
         <v>21682</v>
@@ -926,19 +926,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.2903126464484167</v>
+        <v>0.27307304785894204</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.28315504575331873</v>
+        <v>0.26221206799543062</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>0.10189484369419329</v>
+        <v>0.10006414960241092</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>7.7387182480576466E-2</v>
+        <v>7.5968563369706435E-2</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -948,14 +948,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>50203</v>
+        <v>57438</v>
       </c>
       <c r="C8" s="2">
-        <v>2890</v>
+        <v>3044</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>53093</v>
+        <v>60482</v>
       </c>
       <c r="E8" s="2">
         <v>13716</v>
@@ -965,19 +965,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.25833914075301828</v>
+        <v>0.22677821500611753</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.31312869748819794</v>
+        <v>0.27368640969393082</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>6.445852209711074E-2</v>
+        <v>6.3300427817852056E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>7.9103095688579358E-2</v>
+        <v>7.7653021403978478E-2</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -987,14 +987,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>23450</v>
+        <v>46509</v>
       </c>
       <c r="C9" s="2">
-        <v>2816</v>
+        <v>2234</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>26266</v>
+        <v>48743</v>
       </c>
       <c r="E9" s="2">
         <v>22990</v>
@@ -1004,19 +1004,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.87527602223406686</v>
+        <v>0.47165746876474568</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.9128358208955224</v>
+        <v>0.46025500440774902</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>0.10804180686880839</v>
+        <v>0.10610067334007135</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>0.10771506783140776</v>
+        <v>0.10574049466752948</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>39</v>
@@ -1027,29 +1027,37 @@
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" t="str">
+      <c r="B10" s="2">
+        <v>11261</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8063</v>
+      </c>
+      <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v/>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="1" t="str">
+        <v>19324</v>
+      </c>
+      <c r="E10" s="2">
+        <v>15866</v>
+      </c>
+      <c r="F10" s="2">
+        <v>11126</v>
+      </c>
+      <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H10" s="1" t="str">
+        <v>0.82105154212378395</v>
+      </c>
+      <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v/>
-      </c>
-      <c r="I10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J10" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.98801172187194741</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>7.3222848334648635E-2</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="3"/>
+        <v>5.495976565780309E-2</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -3737,8 +3745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CZ22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH13" sqref="AH13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AL13" sqref="AL13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7282,10 +7290,18 @@
       <c r="AG13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AH13" s="2"/>
-      <c r="AI13" s="2"/>
-      <c r="AJ13" s="2"/>
-      <c r="AK13" s="2"/>
+      <c r="AH13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK13" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="AL13" s="2"/>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
@@ -7434,24 +7450,47 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -7468,47 +7507,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW13">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">

</xml_diff>

<commit_message>
2024 Day16 done (but slow)
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CC49AC-3198-4061-AC9B-DCDDC734689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA6F5B9-AD49-43AE-8C5F-0B94818A0D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="792" yWindow="684" windowWidth="8460" windowHeight="11502" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="10506" windowHeight="11502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="12" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="40">
   <si>
     <t>Day</t>
   </si>
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AA6AC8-5A6F-44C5-8B15-8AB7181E67FD}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -712,14 +712,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>218630</v>
+        <v>222421</v>
       </c>
       <c r="C2" s="2">
-        <v>15641</v>
+        <v>15923</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>234271</v>
+        <v>238344</v>
       </c>
       <c r="E2" s="2">
         <v>14511</v>
@@ -729,19 +729,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>6.1941085324261222E-2</v>
+        <v>6.0882589870103719E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>6.4231807162786439E-2</v>
+        <v>6.3137023932092737E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>6.1941085324261222E-2</v>
+        <v>6.0882589870103719E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>6.4231807162786439E-2</v>
+        <v>6.3137023932092737E-2</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -751,14 +751,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>154967</v>
+        <v>158012</v>
       </c>
       <c r="C3" s="2">
-        <v>37919</v>
+        <v>38616</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>192886</v>
+        <v>196628</v>
       </c>
       <c r="E3" s="2">
         <v>24905</v>
@@ -768,19 +768,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.12911771720083365</v>
+        <v>0.12666049596191795</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.24878199874812057</v>
+        <v>0.2439877983950586</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.10630850596104512</v>
+        <v>0.10449182693921391</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.17633902026254403</v>
+        <v>0.17333345322608926</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
@@ -792,14 +792,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>140194</v>
+        <v>143151</v>
       </c>
       <c r="C4" s="2">
-        <v>15108</v>
+        <v>15364</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>155302</v>
+        <v>158515</v>
       </c>
       <c r="E4" s="2">
         <v>30159</v>
@@ -809,19 +809,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.1941958249088872</v>
+        <v>0.19025959688357569</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.17868810362783</v>
+        <v>0.17499703110701287</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.12873552424329088</v>
+        <v>0.12653559560970698</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.11458171339706354</v>
+        <v>0.11262875357992276</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -831,14 +831,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>112327</v>
+        <v>115030</v>
       </c>
       <c r="C5" s="2">
-        <v>9480</v>
+        <v>9721</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>121807</v>
+        <v>124751</v>
       </c>
       <c r="E5" s="2">
         <v>17872</v>
@@ -848,19 +848,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.14672391570271001</v>
+        <v>0.14326137666231131</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.13572872061036081</v>
+        <v>0.13253933756411371</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>7.6287718070098307E-2</v>
+        <v>7.4984056657604131E-2</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>6.9734254219457531E-2</v>
+        <v>6.854568588397679E-2</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -870,14 +870,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>92053</v>
+        <v>94504</v>
       </c>
       <c r="C6" s="2">
-        <v>11754</v>
+        <v>12006</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>103807</v>
+        <v>106510</v>
       </c>
       <c r="E6" s="2">
         <v>25203</v>
@@ -887,19 +887,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.24278709528259174</v>
+        <v>0.23662566895127218</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.29381986464319471</v>
+        <v>0.28619952594599168</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>0.10758053707031601</v>
+        <v>0.10574212063236331</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>0.12371129305218863</v>
+        <v>0.12160272636126984</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -909,14 +909,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>68319</v>
+        <v>70277</v>
       </c>
       <c r="C7" s="2">
-        <v>23258</v>
+        <v>23971</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>91577</v>
+        <v>94248</v>
       </c>
       <c r="E7" s="2">
         <v>21682</v>
@@ -926,19 +926,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.23676250586937769</v>
+        <v>0.23005262711145064</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.2251057538898403</v>
+        <v>0.21883404243209015</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>9.2550934601380447E-2</v>
+        <v>9.0969355217668579E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>7.0342587933952344E-2</v>
+        <v>6.914365100417677E-2</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -948,14 +948,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>70969</v>
+        <v>73248</v>
       </c>
       <c r="C8" s="2">
-        <v>3612</v>
+        <v>3731</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>74581</v>
+        <v>76979</v>
       </c>
       <c r="E8" s="2">
         <v>13716</v>
@@ -965,19 +965,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.1839074295061745</v>
+        <v>0.17817846425648554</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.22150516422663416</v>
+        <v>0.21461336828309305</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>5.854757951261573E-2</v>
+        <v>5.7547074816232002E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>7.1902300690664597E-2</v>
+        <v>7.0676779620629349E-2</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -987,14 +987,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>60976</v>
+        <v>63093</v>
       </c>
       <c r="C9" s="2">
-        <v>2507</v>
+        <v>2632</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>63483</v>
+        <v>65725</v>
       </c>
       <c r="E9" s="2">
         <v>22990</v>
@@ -1004,19 +1004,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.36214419608399101</v>
+        <v>0.3497907949790795</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.35105615324061928</v>
+        <v>0.33927694038958361</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>9.8134212087710393E-2</v>
+        <v>9.6457221494982037E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>9.7909710469743408E-2</v>
+        <v>9.6240912503765388E-2</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>39</v>
@@ -1028,14 +1028,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>50625</v>
+        <v>52964</v>
       </c>
       <c r="C10" s="2">
-        <v>10143</v>
+        <v>10347</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>60768</v>
+        <v>63311</v>
       </c>
       <c r="E10" s="2">
         <v>15866</v>
@@ -1045,19 +1045,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.26109136387572407</v>
+        <v>0.25060416041446193</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.21977283950617285</v>
+        <v>0.21006721546710974</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.7724985166751323E-2</v>
+        <v>6.6567650119155511E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>5.0889630883227371E-2</v>
+        <v>5.0022255092819476E-2</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -1067,14 +1067,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>51200</v>
+        <v>53992</v>
       </c>
       <c r="C11" s="2">
-        <v>1084</v>
+        <v>1131</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>52284</v>
+        <v>55123</v>
       </c>
       <c r="E11" s="2">
         <v>15096</v>
@@ -1084,19 +1084,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.288730778058297</v>
+        <v>0.27386027610979086</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.27796874999999999</v>
+        <v>0.26359460660838641</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>6.443819337433998E-2</v>
+        <v>6.3337025475782904E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>6.5096281388647481E-2</v>
+        <v>6.3986763839745345E-2</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -1106,14 +1106,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>45949</v>
+        <v>49075</v>
       </c>
       <c r="C12" s="2">
-        <v>7993</v>
+        <v>8101</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>53942</v>
+        <v>57176</v>
       </c>
       <c r="E12" s="2">
         <v>18412</v>
@@ -1123,19 +1123,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.34132957621148641</v>
+        <v>0.32202322652861343</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.39045463448606066</v>
+        <v>0.36558329088130415</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>7.8592740885555623E-2</v>
+        <v>7.7249689524384921E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>8.2061016328957598E-2</v>
+        <v>8.0662347530134293E-2</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -1145,14 +1145,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>31900</v>
+        <v>35664</v>
       </c>
       <c r="C13" s="2">
-        <v>10075</v>
+        <v>10043</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>41975</v>
+        <v>45707</v>
       </c>
       <c r="E13" s="2">
         <v>14898</v>
@@ -1162,19 +1162,19 @@
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.35492555092316858</v>
+        <v>0.32594569759555431</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>0.29557993730407522</v>
+        <v>0.26438425302826379</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>6.3593018342005619E-2</v>
+        <v>6.2506293424629947E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>4.3127658601289851E-2</v>
+        <v>4.2392579837335506E-2</v>
       </c>
       <c r="K13" s="2"/>
     </row>
@@ -1184,14 +1184,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>30440</v>
+        <v>36369</v>
       </c>
       <c r="C14" s="2">
-        <v>4809</v>
+        <v>4687</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>35249</v>
+        <v>41056</v>
       </c>
       <c r="E14" s="2">
         <v>15681</v>
@@ -1201,19 +1201,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.44486368407614402</v>
+        <v>0.38194173811379578</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.47861366622864654</v>
+        <v>0.40058841320905164</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>6.6935301424418725E-2</v>
+        <v>6.5791461081462083E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>6.6637698394547862E-2</v>
+        <v>6.5501908542808462E-2</v>
       </c>
       <c r="K14" s="2"/>
     </row>
@@ -1223,14 +1223,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>13688</v>
+        <v>33355</v>
       </c>
       <c r="C15" s="2">
-        <v>4562</v>
+        <v>3968</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>18250</v>
+        <v>37323</v>
       </c>
       <c r="E15" s="2">
         <v>11770</v>
@@ -1240,19 +1240,19 @@
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.64493150684931511</v>
+        <v>0.31535514294134986</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>0.80537697253068385</v>
+        <v>0.33050517163843501</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>5.0240960255430678E-2</v>
+        <v>4.9382405262981238E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>5.0423089237524588E-2</v>
+        <v>4.9563665301387907E-2</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -1261,29 +1261,37 @@
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" t="str">
+      <c r="B16" s="2">
+        <v>22210</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8743</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1" t="str">
+        <v>30953</v>
+      </c>
+      <c r="E16" s="2">
+        <v>11623</v>
+      </c>
+      <c r="F16" s="2">
+        <v>18398</v>
+      </c>
+      <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J16" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.37550479759635574</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.82836560108059432</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="2"/>
+        <v>4.876564964924647E-2</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="3"/>
+        <v>8.27170096348816E-2</v>
       </c>
       <c r="K16" s="2"/>
     </row>
@@ -1292,29 +1300,37 @@
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" t="str">
+      <c r="B17" s="2">
+        <v>6718</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3760</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1" t="str">
+        <v>10478</v>
+      </c>
+      <c r="E17" s="2">
+        <v>8838</v>
+      </c>
+      <c r="F17" s="2">
+        <v>6371</v>
+      </c>
+      <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J17" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.84348158045428512</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.94834772253646915</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="2"/>
+        <v>3.7080857919645556E-2</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="3"/>
+        <v>2.8643878051083305E-2</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -3785,7 +3801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CZ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -7402,14 +7418,30 @@
       <c r="BE13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="BF13" s="2"/>
-      <c r="BG13" s="2"/>
-      <c r="BH13" s="2"/>
-      <c r="BI13" s="2"/>
-      <c r="BJ13" s="2"/>
-      <c r="BK13" s="2"/>
-      <c r="BL13" s="2"/>
-      <c r="BM13" s="2"/>
+      <c r="BF13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BG13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BH13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BI13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BJ13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BK13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BL13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BM13" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="BN13" s="2"/>
       <c r="BO13" s="2"/>
       <c r="BP13" s="2"/>
@@ -7530,24 +7562,47 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -7564,47 +7619,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW13">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">

</xml_diff>

<commit_message>
2024 Day17 done (sort of)
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA6F5B9-AD49-43AE-8C5F-0B94818A0D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D78532F-6786-40D2-887D-45144A438DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="10506" windowHeight="11502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="10506" windowHeight="11502" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="12" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="40">
   <si>
     <t>Day</t>
   </si>
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AA6AC8-5A6F-44C5-8B15-8AB7181E67FD}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -712,14 +712,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>222421</v>
+        <v>224932</v>
       </c>
       <c r="C2" s="2">
-        <v>15923</v>
+        <v>16217</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>238344</v>
+        <v>241149</v>
       </c>
       <c r="E2" s="2">
         <v>14511</v>
@@ -729,19 +729,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>6.0882589870103719E-2</v>
+        <v>6.0174414988243781E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>6.3137023932092737E-2</v>
+        <v>6.2432201732079029E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>6.0882589870103719E-2</v>
+        <v>6.0174414988243781E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>6.3137023932092737E-2</v>
+        <v>6.2432201732079029E-2</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -751,14 +751,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>158012</v>
+        <v>159874</v>
       </c>
       <c r="C3" s="2">
-        <v>38616</v>
+        <v>39056</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>196628</v>
+        <v>198930</v>
       </c>
       <c r="E3" s="2">
         <v>24905</v>
@@ -768,19 +768,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.12666049596191795</v>
+        <v>0.12519479213793797</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.2439877983950586</v>
+        <v>0.24114615259516869</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.10449182693921391</v>
+        <v>0.10327639757991947</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.17333345322608926</v>
+        <v>0.17139846709227677</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
@@ -792,14 +792,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>143151</v>
+        <v>144879</v>
       </c>
       <c r="C4" s="2">
-        <v>15364</v>
+        <v>15610</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>158515</v>
+        <v>160489</v>
       </c>
       <c r="E4" s="2">
         <v>30159</v>
@@ -809,19 +809,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.19025959688357569</v>
+        <v>0.18791942126874739</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.17499703110701287</v>
+        <v>0.17290980749452992</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.12653559560970698</v>
+        <v>0.12506375726210767</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.11262875357992276</v>
+        <v>0.1113714367008696</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -831,14 +831,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>115030</v>
+        <v>116545</v>
       </c>
       <c r="C5" s="2">
-        <v>9721</v>
+        <v>9897</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>124751</v>
+        <v>126442</v>
       </c>
       <c r="E5" s="2">
         <v>17872</v>
@@ -848,19 +848,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.14326137666231131</v>
+        <v>0.14134543901551699</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.13253933756411371</v>
+        <v>0.13081642284096273</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>7.4984056657604131E-2</v>
+        <v>7.4111856155323064E-2</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>6.854568588397679E-2</v>
+        <v>6.7780484768730109E-2</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -870,14 +870,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>94504</v>
+        <v>95837</v>
       </c>
       <c r="C6" s="2">
-        <v>12006</v>
+        <v>12238</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>106510</v>
+        <v>108075</v>
       </c>
       <c r="E6" s="2">
         <v>25203</v>
@@ -887,19 +887,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.23662566895127218</v>
+        <v>0.23319916724496878</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.28619952594599168</v>
+        <v>0.28221876728194745</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>0.10574212063236331</v>
+        <v>0.10451214809101426</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>0.12160272636126984</v>
+        <v>0.1202452296694112</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -909,14 +909,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>70277</v>
+        <v>71334</v>
       </c>
       <c r="C7" s="2">
-        <v>23971</v>
+        <v>22394</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>94248</v>
+        <v>93728</v>
       </c>
       <c r="E7" s="2">
         <v>21682</v>
@@ -926,19 +926,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.23005262711145064</v>
+        <v>0.23132895186070332</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.21883404243209015</v>
+        <v>0.2155914430706255</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>9.0969355217668579E-2</v>
+        <v>8.9911216716635767E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>6.914365100417677E-2</v>
+        <v>6.8371774580762185E-2</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -948,14 +948,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>73248</v>
+        <v>74562</v>
       </c>
       <c r="C8" s="2">
-        <v>3731</v>
+        <v>3864</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>76979</v>
+        <v>78426</v>
       </c>
       <c r="E8" s="2">
         <v>13716</v>
@@ -965,19 +965,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.17817846425648554</v>
+        <v>0.17489098003213219</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.21461336828309305</v>
+        <v>0.21083125452643436</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>5.7547074816232002E-2</v>
+        <v>5.6877698020725773E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>7.0676779620629349E-2</v>
+        <v>6.9887788309355714E-2</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -987,14 +987,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>63093</v>
+        <v>64260</v>
       </c>
       <c r="C9" s="2">
-        <v>2632</v>
+        <v>2673</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>65725</v>
+        <v>66933</v>
       </c>
       <c r="E9" s="2">
         <v>22990</v>
@@ -1004,19 +1004,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.3497907949790795</v>
+        <v>0.34347780616437334</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.33927694038958361</v>
+        <v>0.33311546840958606</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>9.6457221494982037E-2</v>
+        <v>9.5335249161306909E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>9.6240912503765388E-2</v>
+        <v>9.5166539220742266E-2</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>39</v>
@@ -1028,14 +1028,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>52964</v>
+        <v>54063</v>
       </c>
       <c r="C10" s="2">
-        <v>10347</v>
+        <v>10543</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>63311</v>
+        <v>64606</v>
       </c>
       <c r="E10" s="2">
         <v>15866</v>
@@ -1045,19 +1045,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.25060416041446193</v>
+        <v>0.24558090579822309</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.21006721546710974</v>
+        <v>0.20579694060632966</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.6567650119155511E-2</v>
+        <v>6.5793347681309067E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>5.0022255092819476E-2</v>
+        <v>4.9463837959916775E-2</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -1067,14 +1067,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>53992</v>
+        <v>55211</v>
       </c>
       <c r="C11" s="2">
-        <v>1131</v>
+        <v>1170</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>55123</v>
+        <v>56381</v>
       </c>
       <c r="E11" s="2">
         <v>15096</v>
@@ -1084,19 +1084,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.27386027610979086</v>
+        <v>0.26774977385998827</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.26359460660838641</v>
+        <v>0.25777471880603503</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>6.3337025475782904E-2</v>
+        <v>6.2600301058681557E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>6.3986763839745345E-2</v>
+        <v>6.3272455675493042E-2</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -1106,14 +1106,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>49075</v>
+        <v>50361</v>
       </c>
       <c r="C12" s="2">
-        <v>8101</v>
+        <v>8248</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>57176</v>
+        <v>58609</v>
       </c>
       <c r="E12" s="2">
         <v>18412</v>
@@ -1123,19 +1123,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.32202322652861343</v>
+        <v>0.31414970397038</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.36558329088130415</v>
+        <v>0.35624789023252118</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>7.7249689524384921E-2</v>
+        <v>7.6351135604957932E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>8.0662347530134293E-2</v>
+        <v>7.9761883591485422E-2</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -1145,14 +1145,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>35664</v>
+        <v>36896</v>
       </c>
       <c r="C13" s="2">
-        <v>10043</v>
+        <v>10261</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>45707</v>
+        <v>47157</v>
       </c>
       <c r="E13" s="2">
         <v>14898</v>
@@ -1162,19 +1162,19 @@
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.32594569759555431</v>
+        <v>0.3159234047967428</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>0.26438425302826379</v>
+        <v>0.2555561578490893</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>6.2506293424629947E-2</v>
+        <v>6.1779231927148778E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>4.2392579837335506E-2</v>
+        <v>4.1919335621432255E-2</v>
       </c>
       <c r="K13" s="2"/>
     </row>
@@ -1184,14 +1184,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>36369</v>
+        <v>38122</v>
       </c>
       <c r="C14" s="2">
-        <v>4687</v>
+        <v>4815</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>41056</v>
+        <v>42937</v>
       </c>
       <c r="E14" s="2">
         <v>15681</v>
@@ -1201,19 +1201,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.38194173811379578</v>
+        <v>0.36520949297808419</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.40058841320905164</v>
+        <v>0.38216777713656158</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>6.5791461081462083E-2</v>
+        <v>6.5026187129119339E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>6.5501908542808462E-2</v>
+        <v>6.4770686251844997E-2</v>
       </c>
       <c r="K14" s="2"/>
     </row>
@@ -1223,14 +1223,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>33355</v>
+        <v>35865</v>
       </c>
       <c r="C15" s="2">
-        <v>3968</v>
+        <v>4091</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>37323</v>
+        <v>39956</v>
       </c>
       <c r="E15" s="2">
         <v>11770</v>
@@ -1240,19 +1240,19 @@
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.31535514294134986</v>
+        <v>0.29457403143457805</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>0.33050517163843501</v>
+        <v>0.30737487801477764</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>4.9382405262981238E-2</v>
+        <v>4.8807998374448991E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>4.9563665301387907E-2</v>
+        <v>4.9010367577756835E-2</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -1262,14 +1262,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>22210</v>
+        <v>25802</v>
       </c>
       <c r="C16" s="2">
-        <v>8743</v>
+        <v>8769</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>30953</v>
+        <v>34571</v>
       </c>
       <c r="E16" s="2">
         <v>11623</v>
@@ -1279,19 +1279,19 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>0.37550479759635574</v>
+        <v>0.33620664718984122</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.82836560108059432</v>
+        <v>0.7130455003488102</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>4.876564964924647E-2</v>
+        <v>4.8198416746492834E-2</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>8.27170096348816E-2</v>
+        <v>8.1793608735084386E-2</v>
       </c>
       <c r="K16" s="2"/>
     </row>
@@ -1301,14 +1301,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>6718</v>
+        <v>19487</v>
       </c>
       <c r="C17" s="2">
-        <v>3760</v>
+        <v>5226</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>10478</v>
+        <v>24713</v>
       </c>
       <c r="E17" s="2">
         <v>8838</v>
@@ -1318,19 +1318,19 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v>0.84348158045428512</v>
+        <v>0.35762554121312667</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0.94834772253646915</v>
+        <v>0.32693590598860778</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>3.7080857919645556E-2</v>
+        <v>3.6649540325690753E-2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>2.8643878051083305E-2</v>
+        <v>2.8324115732754788E-2</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -1339,29 +1339,37 @@
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" t="str">
+      <c r="B18" s="2">
+        <v>7904</v>
+      </c>
+      <c r="C18" s="2">
+        <v>9921</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1" t="str">
+        <v>17825</v>
+      </c>
+      <c r="E18" s="2">
+        <v>12179</v>
+      </c>
+      <c r="F18" s="2">
+        <v>7184</v>
+      </c>
+      <c r="G18" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I18" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J18" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.68325385694249652</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.90890688259109309</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="2"/>
+        <v>5.0504045216857626E-2</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="3"/>
+        <v>3.1938541425853145E-2</v>
       </c>
       <c r="K18" s="2"/>
     </row>
@@ -3801,8 +3809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CZ22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7442,10 +7450,18 @@
       <c r="BM13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="BN13" s="2"/>
-      <c r="BO13" s="2"/>
-      <c r="BP13" s="2"/>
-      <c r="BQ13" s="2"/>
+      <c r="BN13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BO13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BP13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BQ13" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="BR13" s="2"/>
       <c r="BS13" s="2"/>
       <c r="BT13" s="2"/>
@@ -7562,47 +7578,24 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -7619,24 +7612,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW13">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">

</xml_diff>

<commit_message>
2024 Day 22 Done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4660FAC7-132C-4C97-AC4F-B7393437928B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F3F470-E6B1-4196-B575-A0961FD1C242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="10506" windowHeight="11502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="10506" windowHeight="11502" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="12" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="41">
   <si>
     <t>Day</t>
   </si>
@@ -664,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AA6AC8-5A6F-44C5-8B15-8AB7181E67FD}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -715,14 +715,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>229660</v>
+        <v>232441</v>
       </c>
       <c r="C2" s="2">
-        <v>16736</v>
+        <v>17025</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>246396</v>
+        <v>249466</v>
       </c>
       <c r="E2" s="2">
         <v>14511</v>
@@ -732,19 +732,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>5.8893001509764765E-2</v>
+        <v>5.8168247376395983E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>6.114691282765828E-2</v>
+        <v>6.041533120232661E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>5.8893001509764765E-2</v>
+        <v>5.8168247376395983E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>6.114691282765828E-2</v>
+        <v>6.041533120232661E-2</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -754,14 +754,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>163342</v>
+        <v>165422</v>
       </c>
       <c r="C3" s="2">
-        <v>40071</v>
+        <v>40678</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>203413</v>
+        <v>206100</v>
       </c>
       <c r="E3" s="2">
         <v>24905</v>
@@ -771,19 +771,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.12243563587381337</v>
+        <v>0.12083939835031537</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.23602625166827881</v>
+        <v>0.23305848073412241</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>0.10107712787545252</v>
+        <v>9.9833243808775549E-2</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.16786989462683968</v>
+        <v>0.16586144440954909</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
@@ -795,14 +795,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>148214</v>
+        <v>150210</v>
       </c>
       <c r="C4" s="2">
-        <v>16003</v>
+        <v>16299</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>164217</v>
+        <v>166509</v>
       </c>
       <c r="E4" s="2">
         <v>30159</v>
@@ -812,19 +812,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.1836533367434553</v>
+        <v>0.18112534457596888</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.16901912100071517</v>
+        <v>0.16677318420877438</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.12240052598256465</v>
+        <v>0.12089423007544114</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.10907863798658887</v>
+        <v>0.10777358555504407</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -834,14 +834,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>119462</v>
+        <v>121145</v>
       </c>
       <c r="C5" s="2">
-        <v>10228</v>
+        <v>10409</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>129690</v>
+        <v>131554</v>
       </c>
       <c r="E5" s="2">
         <v>17872</v>
@@ -851,19 +851,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.13780553627881872</v>
+        <v>0.13585295772078387</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.1276221727411227</v>
+        <v>0.12584918898840233</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>7.2533645026704979E-2</v>
+        <v>7.1641025229891048E-2</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>6.6385091004093011E-2</v>
+        <v>6.5590838105153565E-2</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -873,14 +873,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>98407</v>
+        <v>99755</v>
       </c>
       <c r="C6" s="2">
-        <v>12647</v>
+        <v>12940</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>111054</v>
+        <v>112695</v>
       </c>
       <c r="E6" s="2">
         <v>25203</v>
@@ -890,19 +890,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.22694364903560429</v>
+        <v>0.22363902568880606</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.27484833395998254</v>
+        <v>0.27113427898350961</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>0.10228656309355671</v>
+        <v>0.10102779537091226</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>0.11776974658190369</v>
+        <v>0.11636071089007533</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -912,14 +912,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>73253</v>
+        <v>74369</v>
       </c>
       <c r="C7" s="2">
-        <v>25211</v>
+        <v>25670</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>98464</v>
+        <v>100039</v>
       </c>
       <c r="E7" s="2">
         <v>21682</v>
@@ -929,19 +929,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.22020230744231395</v>
+        <v>0.21673547316546546</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.20994362005651646</v>
+        <v>0.20679315306108728</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>8.7996558385688081E-2</v>
+        <v>8.6913647551169301E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>6.6964207959592445E-2</v>
+        <v>6.6163026316355553E-2</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -951,14 +951,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>76845</v>
+        <v>78125</v>
       </c>
       <c r="C8" s="2">
-        <v>3991</v>
+        <v>4129</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>80836</v>
+        <v>82254</v>
       </c>
       <c r="E8" s="2">
         <v>13716</v>
@@ -968,19 +968,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.16967687663912118</v>
+        <v>0.16675176891093443</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.20456763615069296</v>
+        <v>0.20121600000000001</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>5.5666488092339164E-2</v>
+        <v>5.4981440356601699E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>6.8449011582339112E-2</v>
+        <v>6.7630065263873412E-2</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -990,14 +990,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>66364</v>
+        <v>67521</v>
       </c>
       <c r="C9" s="2">
-        <v>2735</v>
+        <v>2831</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>69099</v>
+        <v>70352</v>
       </c>
       <c r="E9" s="2">
         <v>22990</v>
@@ -1007,19 +1007,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.33271103778636452</v>
+        <v>0.32678530816465773</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.32255439696220845</v>
+        <v>0.31702729521186002</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>9.330508612152795E-2</v>
+        <v>9.215684702524593E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>9.3207349995645741E-2</v>
+        <v>9.2092186834508538E-2</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>39</v>
@@ -1031,14 +1031,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>56068</v>
+        <v>57210</v>
       </c>
       <c r="C10" s="2">
-        <v>10889</v>
+        <v>11054</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>66957</v>
+        <v>68264</v>
       </c>
       <c r="E10" s="2">
         <v>15866</v>
@@ -1048,19 +1048,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.23695804770225667</v>
+        <v>0.23242118832766906</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.19843761147178426</v>
+        <v>0.19447649012410417</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.4392279095439861E-2</v>
+        <v>6.3599849278057938E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>4.844552817208047E-2</v>
+        <v>4.7865910058896663E-2</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -1070,14 +1070,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>57404</v>
+        <v>58624</v>
       </c>
       <c r="C11" s="2">
-        <v>1249</v>
+        <v>1269</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>58653</v>
+        <v>59893</v>
       </c>
       <c r="E11" s="2">
         <v>15096</v>
@@ -1087,19 +1087,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.25737813922561503</v>
+        <v>0.25204948825405304</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.24792697373005365</v>
+        <v>0.2427674672489083</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>6.1267228364096822E-2</v>
+        <v>6.0513256315489886E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>6.1969868501262737E-2</v>
+        <v>6.1228440765613637E-2</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -1109,14 +1109,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>52552</v>
+        <v>53738</v>
       </c>
       <c r="C12" s="2">
-        <v>8489</v>
+        <v>8634</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>61041</v>
+        <v>62372</v>
       </c>
       <c r="E12" s="2">
         <v>18412</v>
@@ -1126,19 +1126,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.30163332841860391</v>
+        <v>0.29519656256012311</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.34139518952656417</v>
+        <v>0.33386058282779413</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>7.472523904608841E-2</v>
+        <v>7.3805648865977722E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>7.8119829312897321E-2</v>
+        <v>7.7185178174246374E-2</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -1148,14 +1148,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>38904</v>
+        <v>40028</v>
       </c>
       <c r="C13" s="2">
-        <v>10600</v>
+        <v>10826</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>49504</v>
+        <v>50854</v>
       </c>
       <c r="E13" s="2">
         <v>14898</v>
@@ -1165,19 +1165,19 @@
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.30094537815126049</v>
+        <v>0.29295630628859087</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>0.24236582356570019</v>
+        <v>0.23556010792445289</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>6.0463643890322896E-2</v>
+        <v>5.9719560982258106E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>4.1056344160933553E-2</v>
+        <v>4.0565132657319494E-2</v>
       </c>
       <c r="K13" s="2"/>
     </row>
@@ -1187,14 +1187,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>40579</v>
+        <v>41744</v>
       </c>
       <c r="C14" s="2">
-        <v>4890</v>
+        <v>5029</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>45469</v>
+        <v>46773</v>
       </c>
       <c r="E14" s="2">
         <v>15681</v>
@@ -1204,19 +1204,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.34487233059886957</v>
+        <v>0.33525752036431272</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.35902806870548803</v>
+        <v>0.34900824070525105</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>6.3641455218428872E-2</v>
+        <v>6.2858265254583795E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>6.3437255072716192E-2</v>
+        <v>6.2678271045125425E-2</v>
       </c>
       <c r="K14" s="2"/>
     </row>
@@ -1226,14 +1226,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>38483</v>
+        <v>39701</v>
       </c>
       <c r="C15" s="2">
-        <v>4361</v>
+        <v>4512</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>42844</v>
+        <v>44213</v>
       </c>
       <c r="E15" s="2">
         <v>11770</v>
@@ -1243,19 +1243,19 @@
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.27471758005788444</v>
+        <v>0.2662112953203809</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>0.28646415300262451</v>
+        <v>0.27767562529911083</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>4.7768632607672203E-2</v>
+        <v>4.7180778142111551E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>4.8001393364103459E-2</v>
+        <v>4.7427089024741763E-2</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -1265,14 +1265,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>28715</v>
+        <v>29882</v>
       </c>
       <c r="C16" s="2">
-        <v>8970</v>
+        <v>9245</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>37685</v>
+        <v>39127</v>
       </c>
       <c r="E16" s="2">
         <v>11623</v>
@@ -1282,19 +1282,19 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>0.30842510282605812</v>
+        <v>0.29705829733943312</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.6407104300888038</v>
+        <v>0.61568837427213707</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>4.7172032013506712E-2</v>
+        <v>4.6591519485621284E-2</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>8.0109727423147259E-2</v>
+        <v>7.9151268493940399E-2</v>
       </c>
       <c r="K16" s="2"/>
     </row>
@@ -1304,14 +1304,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>23892</v>
+        <v>25315</v>
       </c>
       <c r="C17" s="2">
-        <v>5434</v>
+        <v>5611</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>29326</v>
+        <v>30926</v>
       </c>
       <c r="E17" s="2">
         <v>8838</v>
@@ -1321,19 +1321,19 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v>0.30137079724476573</v>
+        <v>0.28577895621806892</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0.26665829566382054</v>
+        <v>0.25166897096583052</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>3.5869088783908827E-2</v>
+        <v>3.5427673510618679E-2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>2.7741008447269878E-2</v>
+        <v>2.7409105966675413E-2</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -1343,14 +1343,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>20508</v>
+        <v>22036</v>
       </c>
       <c r="C18" s="2">
-        <v>9261</v>
+        <v>9549</v>
       </c>
       <c r="D18">
         <f t="shared" si="7"/>
-        <v>29769</v>
+        <v>31585</v>
       </c>
       <c r="E18" s="2">
         <v>12179</v>
@@ -1360,19 +1360,19 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="6"/>
-        <v>0.40911686653901708</v>
+        <v>0.38559442773468416</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>0.35030232104544567</v>
+        <v>0.32601198039571611</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="2"/>
-        <v>4.9428562151982984E-2</v>
+        <v>4.8820280118332761E-2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>3.128102412261604E-2</v>
+        <v>3.0906767738910088E-2</v>
       </c>
       <c r="K18" s="2"/>
     </row>
@@ -1382,14 +1382,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>25201</v>
+        <v>27190</v>
       </c>
       <c r="C19" s="2">
-        <v>628</v>
+        <v>661</v>
       </c>
       <c r="D19">
         <f t="shared" si="7"/>
-        <v>25829</v>
+        <v>27851</v>
       </c>
       <c r="E19" s="2">
         <v>9308</v>
@@ -1399,19 +1399,19 @@
       </c>
       <c r="G19" s="1">
         <f t="shared" si="6"/>
-        <v>0.36037012660188161</v>
+        <v>0.33420703026821297</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>0.35950954327209239</v>
+        <v>0.33321073924236849</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="2"/>
-        <v>3.7776587282261076E-2</v>
+        <v>3.7311697786471906E-2</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>3.9449621179134371E-2</v>
+        <v>3.8977633033759104E-2</v>
       </c>
       <c r="K19" s="2"/>
     </row>
@@ -1421,14 +1421,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>21636</v>
+        <v>24440</v>
       </c>
       <c r="C20" s="2">
-        <v>2559</v>
+        <v>2639</v>
       </c>
       <c r="D20">
         <f t="shared" si="7"/>
-        <v>24195</v>
+        <v>27079</v>
       </c>
       <c r="E20" s="2">
         <v>16201</v>
@@ -1438,19 +1438,19 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" si="6"/>
-        <v>0.66960115726389746</v>
+        <v>0.59828649506998044</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
-        <v>0.71427250878166015</v>
+        <v>0.63232405891980359</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
-        <v>6.5751879088946252E-2</v>
+        <v>6.4942717644889486E-2</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="3"/>
-        <v>6.7290777671340243E-2</v>
+        <v>6.6485688841469451E-2</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>40</v>
@@ -1462,14 +1462,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>6849</v>
+        <v>18707</v>
       </c>
       <c r="C21" s="2">
-        <v>3868</v>
+        <v>3710</v>
       </c>
       <c r="D21">
         <f t="shared" si="7"/>
-        <v>10717</v>
+        <v>22417</v>
       </c>
       <c r="E21" s="2">
         <v>8179</v>
@@ -1479,19 +1479,19 @@
       </c>
       <c r="G21" s="1">
         <f t="shared" si="6"/>
-        <v>0.76317999440141826</v>
+        <v>0.3648570281482803</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>0.96101620674551025</v>
+        <v>0.35184690222911208</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="2"/>
-        <v>3.319453237877238E-2</v>
+        <v>3.2786030962135122E-2</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="3"/>
-        <v>2.8659757902987023E-2</v>
+        <v>2.8316863203995853E-2</v>
       </c>
       <c r="K21" s="2"/>
     </row>
@@ -1500,25 +1500,31 @@
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" t="str">
+      <c r="B22" s="2">
+        <v>9353</v>
+      </c>
+      <c r="C22" s="2">
+        <v>3829</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E22" s="2"/>
+        <v>13182</v>
+      </c>
+      <c r="E22" s="2">
+        <v>6458</v>
+      </c>
       <c r="F22" s="2"/>
-      <c r="G22" s="1" t="str">
+      <c r="G22" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I22" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <v>0.48991048399332421</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="2"/>
+        <v>2.5887295262681086E-2</v>
       </c>
       <c r="J22" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1531,29 +1537,37 @@
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" t="str">
+      <c r="B23" s="2">
+        <v>9657</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3570</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="1" t="str">
+        <v>13227</v>
+      </c>
+      <c r="E23" s="2">
+        <v>10291</v>
+      </c>
+      <c r="F23" s="2">
+        <v>8994</v>
+      </c>
+      <c r="G23" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="J23" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <v>0.77802978755575714</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="1"/>
+        <v>0.93134513824168996</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1252114516607472E-2</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="3"/>
+        <v>3.8693690011658871E-2</v>
       </c>
       <c r="K23" s="2"/>
     </row>
@@ -3838,8 +3852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CZ22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="CD13" sqref="CD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7527,14 +7541,30 @@
       <c r="CC13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="CD13" s="2"/>
-      <c r="CE13" s="2"/>
-      <c r="CF13" s="2"/>
-      <c r="CG13" s="2"/>
-      <c r="CH13" s="2"/>
-      <c r="CI13" s="2"/>
-      <c r="CJ13" s="2"/>
-      <c r="CK13" s="2"/>
+      <c r="CD13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CE13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="CF13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="CG13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="CH13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CI13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CJ13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CK13" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="CL13" s="2"/>
       <c r="CM13" s="2"/>
       <c r="CN13" s="2"/>
@@ -7631,47 +7661,24 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="75">
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -7688,24 +7695,47 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW13">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">

</xml_diff>

<commit_message>
2024 day 25 done
</commit_message>
<xml_diff>
--- a/Documents/AdventStats.xlsx
+++ b/Documents/AdventStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Userfiles\Hobbies\Computer\Sources\Advent\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F3F470-E6B1-4196-B575-A0961FD1C242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E7A559-0265-4453-95A3-85FFD526C580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="10506" windowHeight="11502" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="10506" windowHeight="11502" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="12" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="41">
   <si>
     <t>Day</t>
   </si>
@@ -664,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2AA6AC8-5A6F-44C5-8B15-8AB7181E67FD}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -715,14 +715,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>232441</v>
+        <v>235739</v>
       </c>
       <c r="C2" s="2">
-        <v>17025</v>
+        <v>17272</v>
       </c>
       <c r="D2">
         <f>IF(ISBLANK(B2),"",B2+C2)</f>
-        <v>249466</v>
+        <v>253011</v>
       </c>
       <c r="E2" s="2">
         <v>14511</v>
@@ -732,19 +732,19 @@
       </c>
       <c r="G2" s="1">
         <f t="shared" ref="G2:G11" si="0">IF(D2="","",E2/D2)</f>
-        <v>5.8168247376395983E-2</v>
+        <v>5.7353237606270084E-2</v>
       </c>
       <c r="H2" s="1">
         <f>IF(ISBLANK(C2),"",F2/B2)</f>
-        <v>6.041533120232661E-2</v>
+        <v>5.9570117799770082E-2</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISBLANK(E2),"",E2/$D$2)</f>
-        <v>5.8168247376395983E-2</v>
+        <v>5.7353237606270084E-2</v>
       </c>
       <c r="J2" s="1">
         <f>IF(ISBLANK(F2),"",F2/$B$2)</f>
-        <v>6.041533120232661E-2</v>
+        <v>5.9570117799770082E-2</v>
       </c>
       <c r="K2" s="2"/>
     </row>
@@ -754,14 +754,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>165422</v>
+        <v>167942</v>
       </c>
       <c r="C3" s="2">
-        <v>40678</v>
+        <v>41343</v>
       </c>
       <c r="D3">
         <f>IF(ISBLANK(B3),"",B3+C3)</f>
-        <v>206100</v>
+        <v>209285</v>
       </c>
       <c r="E3" s="2">
         <v>24905</v>
@@ -771,19 +771,19 @@
       </c>
       <c r="G3" s="1">
         <f t="shared" si="0"/>
-        <v>0.12083939835031537</v>
+        <v>0.11900040614473087</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H26" si="1">IF(ISBLANK(C3),"",F3/B3)</f>
-        <v>0.23305848073412241</v>
+        <v>0.22956139619630586</v>
       </c>
       <c r="I3" s="1">
         <f t="shared" ref="I3:I26" si="2">IF(ISBLANK(E3),"",E3/$D$2)</f>
-        <v>9.9833243808775549E-2</v>
+        <v>9.843445541893435E-2</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J26" si="3">IF(ISBLANK(F3),"",F3/$B$2)</f>
-        <v>0.16586144440954909</v>
+        <v>0.1635410347884737</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>35</v>
@@ -795,14 +795,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>150210</v>
+        <v>152684</v>
       </c>
       <c r="C4" s="2">
-        <v>16299</v>
+        <v>16568</v>
       </c>
       <c r="D4">
         <f>IF(ISBLANK(B4),"",B4+C4)</f>
-        <v>166509</v>
+        <v>169252</v>
       </c>
       <c r="E4" s="2">
         <v>30159</v>
@@ -812,19 +812,19 @@
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>0.18112534457596888</v>
+        <v>0.17818991799210646</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.16677318420877438</v>
+        <v>0.16407089151450055</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
-        <v>0.12089423007544114</v>
+        <v>0.1192003509728826</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="3"/>
-        <v>0.10777358555504407</v>
+        <v>0.10626582788592469</v>
       </c>
       <c r="K4" s="2"/>
     </row>
@@ -834,14 +834,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>121145</v>
+        <v>123284</v>
       </c>
       <c r="C5" s="2">
-        <v>10409</v>
+        <v>10628</v>
       </c>
       <c r="D5">
         <f>IF(ISBLANK(B5),"",B5+C5)</f>
-        <v>131554</v>
+        <v>133912</v>
       </c>
       <c r="E5" s="2">
         <v>17872</v>
@@ -851,19 +851,19 @@
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>0.13585295772078387</v>
+        <v>0.13346078021387181</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.12584918898840233</v>
+        <v>0.12366568248921191</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
-        <v>7.1641025229891048E-2</v>
+        <v>7.0637245020967465E-2</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="3"/>
-        <v>6.5590838105153565E-2</v>
+        <v>6.4673219110965935E-2</v>
       </c>
       <c r="K5" s="2"/>
     </row>
@@ -873,14 +873,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>99755</v>
+        <v>101647</v>
       </c>
       <c r="C6" s="2">
-        <v>12940</v>
+        <v>13214</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D11" si="5">IF(ISBLANK(B6),"",B6+C6)</f>
-        <v>112695</v>
+        <v>114861</v>
       </c>
       <c r="E6" s="2">
         <v>25203</v>
@@ -890,19 +890,19 @@
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>0.22363902568880606</v>
+        <v>0.21942173583722935</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.27113427898350961</v>
+        <v>0.26608753824510317</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>0.10102779537091226</v>
+        <v>9.9612269822260693E-2</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>0.11636071089007533</v>
+        <v>0.11473281892262205</v>
       </c>
       <c r="K6" s="2"/>
     </row>
@@ -912,14 +912,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>74369</v>
+        <v>75826</v>
       </c>
       <c r="C7" s="2">
-        <v>25670</v>
+        <v>26243</v>
       </c>
       <c r="D7">
         <f t="shared" si="5"/>
-        <v>100039</v>
+        <v>102069</v>
       </c>
       <c r="E7" s="2">
         <v>21682</v>
@@ -929,19 +929,19 @@
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.21673547316546546</v>
+        <v>0.21242492823482154</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.20679315306108728</v>
+        <v>0.20281961332524465</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
-        <v>8.6913647551169301E-2</v>
+        <v>8.5695878835307562E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>6.6163026316355553E-2</v>
+        <v>6.5237402381447276E-2</v>
       </c>
       <c r="K7" s="2"/>
     </row>
@@ -951,14 +951,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>78125</v>
+        <v>79797</v>
       </c>
       <c r="C8" s="2">
-        <v>4129</v>
+        <v>4226</v>
       </c>
       <c r="D8">
         <f t="shared" si="5"/>
-        <v>82254</v>
+        <v>84023</v>
       </c>
       <c r="E8" s="2">
         <v>13716</v>
@@ -968,19 +968,19 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.16675176891093443</v>
+        <v>0.1632410173404901</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.20121600000000001</v>
+        <v>0.19699988721380504</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>5.4981440356601699E-2</v>
+        <v>5.4211081731624318E-2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>6.7630065263873412E-2</v>
+        <v>6.6683917383207697E-2</v>
       </c>
       <c r="K8" s="2"/>
     </row>
@@ -990,14 +990,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>67521</v>
+        <v>69004</v>
       </c>
       <c r="C9" s="2">
-        <v>2831</v>
+        <v>2956</v>
       </c>
       <c r="D9">
         <f>IF(ISBLANK(B9),"",B9+C9)</f>
-        <v>70352</v>
+        <v>71960</v>
       </c>
       <c r="E9" s="2">
         <v>22990</v>
@@ -1007,19 +1007,19 @@
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.32678530816465773</v>
+        <v>0.31948304613674261</v>
       </c>
       <c r="H9" s="1">
         <f>IF(ISBLANK(C9),"",F9/B9)</f>
-        <v>0.31702729521186002</v>
+        <v>0.31021390064344095</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>9.215684702524593E-2</v>
+        <v>9.0865614538498327E-2</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>9.2092186834508538E-2</v>
+        <v>9.0803812691154201E-2</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>39</v>
@@ -1031,14 +1031,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>57210</v>
+        <v>58605</v>
       </c>
       <c r="C10" s="2">
-        <v>11054</v>
+        <v>11247</v>
       </c>
       <c r="D10">
         <f>IF(ISBLANK(B10),"",B10+C10)</f>
-        <v>68264</v>
+        <v>69852</v>
       </c>
       <c r="E10" s="2">
         <v>15866</v>
@@ -1048,19 +1048,19 @@
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.23242118832766906</v>
+        <v>0.22713737616675256</v>
       </c>
       <c r="H10" s="1">
         <f>IF(ISBLANK(C10),"",F10/B10)</f>
-        <v>0.19447649012410417</v>
+        <v>0.18984728265506357</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>6.3599849278057938E-2</v>
+        <v>6.2708735983810979E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>4.7865910058896663E-2</v>
+        <v>4.7196263664476393E-2</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -1070,14 +1070,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>58624</v>
+        <v>60162</v>
       </c>
       <c r="C11" s="2">
-        <v>1269</v>
+        <v>1359</v>
       </c>
       <c r="D11">
         <f t="shared" si="5"/>
-        <v>59893</v>
+        <v>61521</v>
       </c>
       <c r="E11" s="2">
         <v>15096</v>
@@ -1087,19 +1087,19 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>0.25204948825405304</v>
+        <v>0.24537962646901057</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>0.2427674672489083</v>
+        <v>0.23656128453176423</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>6.0513256315489886E-2</v>
+        <v>5.9665390042330173E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>6.1228440765613637E-2</v>
+        <v>6.0371851920980407E-2</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -1109,14 +1109,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>53738</v>
+        <v>55190</v>
       </c>
       <c r="C12" s="2">
-        <v>8634</v>
+        <v>8810</v>
       </c>
       <c r="D12">
         <f>IF(ISBLANK(B12),"",B12+C12)</f>
-        <v>62372</v>
+        <v>64000</v>
       </c>
       <c r="E12" s="2">
         <v>18412</v>
@@ -1126,19 +1126,19 @@
       </c>
       <c r="G12" s="1">
         <f>IF(D12="","",E12/D12)</f>
-        <v>0.29519656256012311</v>
+        <v>0.28768749999999998</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>0.33386058282779413</v>
+        <v>0.32507700670411305</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>7.3805648865977722E-2</v>
+        <v>7.2771539577330624E-2</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>7.7185178174246374E-2</v>
+        <v>7.6105353802298298E-2</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -1148,14 +1148,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>40028</v>
+        <v>41284</v>
       </c>
       <c r="C13" s="2">
-        <v>10826</v>
+        <v>11049</v>
       </c>
       <c r="D13">
         <f>IF(ISBLANK(B13),"",B13+C13)</f>
-        <v>50854</v>
+        <v>52333</v>
       </c>
       <c r="E13" s="2">
         <v>14898</v>
@@ -1165,19 +1165,19 @@
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G26" si="6">IF(D13="","",E13/D13)</f>
-        <v>0.29295630628859087</v>
+        <v>0.28467697246479279</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>0.23556010792445289</v>
+        <v>0.22839356651487258</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>5.9719560982258106E-2</v>
+        <v>5.8882815371663684E-2</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>4.0565132657319494E-2</v>
+        <v>3.999762449149271E-2</v>
       </c>
       <c r="K13" s="2"/>
     </row>
@@ -1187,14 +1187,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>41744</v>
+        <v>43180</v>
       </c>
       <c r="C14" s="2">
-        <v>5029</v>
+        <v>5179</v>
       </c>
       <c r="D14">
         <f>IF(ISBLANK(B14),"",B14+C14)</f>
-        <v>46773</v>
+        <v>48359</v>
       </c>
       <c r="E14" s="2">
         <v>15681</v>
@@ -1204,19 +1204,19 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="6"/>
-        <v>0.33525752036431272</v>
+        <v>0.3242622883020741</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>0.34900824070525105</v>
+        <v>0.33740157480314958</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>6.2858265254583795E-2</v>
+        <v>6.1977542478390268E-2</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>6.2678271045125425E-2</v>
+        <v>6.1801399004831614E-2</v>
       </c>
       <c r="K14" s="2"/>
     </row>
@@ -1226,14 +1226,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>39701</v>
+        <v>41101</v>
       </c>
       <c r="C15" s="2">
-        <v>4512</v>
+        <v>4727</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:D26" si="7">IF(ISBLANK(B15),"",B15+C15)</f>
-        <v>44213</v>
+        <v>45828</v>
       </c>
       <c r="E15" s="2">
         <v>11770</v>
@@ -1243,19 +1243,19 @@
       </c>
       <c r="G15" s="1">
         <f t="shared" si="6"/>
-        <v>0.2662112953203809</v>
+        <v>0.25682988565942216</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>0.27767562529911083</v>
+        <v>0.26821731831342305</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>4.7180778142111551E-2</v>
+        <v>4.6519716534063733E-2</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>4.7427089024741763E-2</v>
+        <v>4.6763581757791453E-2</v>
       </c>
       <c r="K15" s="2"/>
     </row>
@@ -1265,14 +1265,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>29882</v>
+        <v>31212</v>
       </c>
       <c r="C16" s="2">
-        <v>9245</v>
+        <v>9477</v>
       </c>
       <c r="D16">
         <f t="shared" si="7"/>
-        <v>39127</v>
+        <v>40689</v>
       </c>
       <c r="E16" s="2">
         <v>11623</v>
@@ -1282,19 +1282,19 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="6"/>
-        <v>0.29705829733943312</v>
+        <v>0.28565459952321265</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.61568837427213707</v>
+        <v>0.58945277457388179</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="2"/>
-        <v>4.6591519485621284E-2</v>
+        <v>4.5938714127053762E-2</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="3"/>
-        <v>7.9151268493940399E-2</v>
+        <v>7.8043938423425913E-2</v>
       </c>
       <c r="K16" s="2"/>
     </row>
@@ -1304,14 +1304,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>25315</v>
+        <v>26745</v>
       </c>
       <c r="C17" s="2">
-        <v>5611</v>
+        <v>5733</v>
       </c>
       <c r="D17">
         <f t="shared" si="7"/>
-        <v>30926</v>
+        <v>32478</v>
       </c>
       <c r="E17" s="2">
         <v>8838</v>
@@ -1321,19 +1321,19 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="6"/>
-        <v>0.28577895621806892</v>
+        <v>0.27212266765194904</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>0.25166897096583052</v>
+        <v>0.2382127500467377</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
-        <v>3.5427673510618679E-2</v>
+        <v>3.4931287572477085E-2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="3"/>
-        <v>2.7409105966675413E-2</v>
+        <v>2.7025651249899252E-2</v>
       </c>
       <c r="K17" s="2"/>
     </row>
@@ -1343,14 +1343,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>22036</v>
+        <v>23490</v>
       </c>
       <c r="C18" s="2">
-        <v>9549</v>
+        <v>9873</v>
       </c>
       <c r="D18">
         <f t="shared" si="7"/>
-        <v>31585</v>
+        <v>33363</v>
       </c>
       <c r="E18" s="2">
         <v>12179</v>
@@ -1360,19 +1360,19 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="6"/>
-        <v>0.38559442773468416</v>
+        <v>0.36504510985223149</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>0.32601198039571611</v>
+        <v>0.30583226905065986</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="2"/>
-        <v>4.8820280118332761E-2</v>
+        <v>4.8136247040642503E-2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="3"/>
-        <v>3.0906767738910088E-2</v>
+        <v>3.0474380564946828E-2</v>
       </c>
       <c r="K18" s="2"/>
     </row>
@@ -1382,14 +1382,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>27190</v>
+        <v>29006</v>
       </c>
       <c r="C19" s="2">
-        <v>661</v>
+        <v>686</v>
       </c>
       <c r="D19">
         <f t="shared" si="7"/>
-        <v>27851</v>
+        <v>29692</v>
       </c>
       <c r="E19" s="2">
         <v>9308</v>
@@ -1399,19 +1399,19 @@
       </c>
       <c r="G19" s="1">
         <f t="shared" si="6"/>
-        <v>0.33420703026821297</v>
+        <v>0.31348511383537653</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>0.33321073924236849</v>
+        <v>0.31234916913741984</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="2"/>
-        <v>3.7311697786471906E-2</v>
+        <v>3.6788914315978354E-2</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="3"/>
-        <v>3.8977633033759104E-2</v>
+        <v>3.8432334064367794E-2</v>
       </c>
       <c r="K19" s="2"/>
     </row>
@@ -1421,14 +1421,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>24440</v>
+        <v>26364</v>
       </c>
       <c r="C20" s="2">
-        <v>2639</v>
+        <v>2764</v>
       </c>
       <c r="D20">
         <f t="shared" si="7"/>
-        <v>27079</v>
+        <v>29128</v>
       </c>
       <c r="E20" s="2">
         <v>16201</v>
@@ -1438,19 +1438,19 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" si="6"/>
-        <v>0.59828649506998044</v>
+        <v>0.55620021971985723</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
-        <v>0.63232405891980359</v>
+        <v>0.5861781216810803</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="2"/>
-        <v>6.4942717644889486E-2</v>
+        <v>6.4032789088221465E-2</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="3"/>
-        <v>6.6485688841469451E-2</v>
+        <v>6.5555550842245028E-2</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>40</v>
@@ -1462,14 +1462,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>18707</v>
+        <v>21074</v>
       </c>
       <c r="C21" s="2">
-        <v>3710</v>
+        <v>3753</v>
       </c>
       <c r="D21">
         <f t="shared" si="7"/>
-        <v>22417</v>
+        <v>24827</v>
       </c>
       <c r="E21" s="2">
         <v>8179</v>
@@ -1479,19 +1479,19 @@
       </c>
       <c r="G21" s="1">
         <f t="shared" si="6"/>
-        <v>0.3648570281482803</v>
+        <v>0.32943972288234585</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>0.35184690222911208</v>
+        <v>0.3123279870931005</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="2"/>
-        <v>3.2786030962135122E-2</v>
+        <v>3.2326657734248705E-2</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="3"/>
-        <v>2.8316863203995853E-2</v>
+        <v>2.7920708919610248E-2</v>
       </c>
       <c r="K21" s="2"/>
     </row>
@@ -1501,14 +1501,14 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>9353</v>
+        <v>13580</v>
       </c>
       <c r="C22" s="2">
-        <v>3829</v>
+        <v>3662</v>
       </c>
       <c r="D22">
         <f t="shared" si="7"/>
-        <v>13182</v>
+        <v>17242</v>
       </c>
       <c r="E22" s="2">
         <v>6458</v>
@@ -1516,7 +1516,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="1">
         <f t="shared" si="6"/>
-        <v>0.48991048399332421</v>
+        <v>0.37455051618141749</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="1"/>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="I22" s="1">
         <f t="shared" si="2"/>
-        <v>2.5887295262681086E-2</v>
+        <v>2.5524581935172781E-2</v>
       </c>
       <c r="J22" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1538,14 +1538,14 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>9657</v>
+        <v>19343</v>
       </c>
       <c r="C23" s="2">
-        <v>3570</v>
+        <v>3351</v>
       </c>
       <c r="D23">
         <f t="shared" si="7"/>
-        <v>13227</v>
+        <v>22694</v>
       </c>
       <c r="E23" s="2">
         <v>10291</v>
@@ -1555,19 +1555,19 @@
       </c>
       <c r="G23" s="1">
         <f t="shared" si="6"/>
-        <v>0.77802978755575714</v>
+        <v>0.45346787697188684</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="1"/>
-        <v>0.93134513824168996</v>
+        <v>0.46497440934705059</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="2"/>
-        <v>4.1252114516607472E-2</v>
+        <v>4.0674120888024634E-2</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="3"/>
-        <v>3.8693690011658871E-2</v>
+        <v>3.8152363418865777E-2</v>
       </c>
       <c r="K23" s="2"/>
     </row>
@@ -1576,25 +1576,31 @@
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" t="str">
+      <c r="B24" s="2">
+        <v>18464</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2449</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E24" s="2"/>
+        <v>20913</v>
+      </c>
+      <c r="E24" s="2">
+        <v>8600</v>
+      </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="1" t="str">
+      <c r="G24" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I24" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <v>0.41122746616936834</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="2"/>
+        <v>3.3990617008746657E-2</v>
       </c>
       <c r="J24" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1607,25 +1613,31 @@
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" t="str">
+      <c r="B25" s="2">
+        <v>10385</v>
+      </c>
+      <c r="C25" s="2">
+        <v>8542</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E25" s="2"/>
+        <v>18927</v>
+      </c>
+      <c r="E25" s="2">
+        <v>7332</v>
+      </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="1" t="str">
+      <c r="G25" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I25" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <v>0.38738310350293231</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="2"/>
+        <v>2.8978977198619821E-2</v>
       </c>
       <c r="J25" s="1" t="str">
         <f t="shared" si="3"/>
@@ -1638,25 +1650,31 @@
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" t="str">
+      <c r="B26" s="2">
+        <v>6472</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3405</v>
+      </c>
+      <c r="D26">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="E26" s="2"/>
+        <v>9877</v>
+      </c>
+      <c r="E26" s="2">
+        <v>7849</v>
+      </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="1" t="str">
+      <c r="G26" s="1">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="H26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="I26" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
+        <v>0.7946744963045459</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="2"/>
+        <v>3.102236661647122E-2</v>
       </c>
       <c r="J26" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3852,8 +3870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76543402-6771-4C6D-98B2-2473D542FE19}">
   <dimension ref="A1:CZ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7565,18 +7583,42 @@
       <c r="CK13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="CL13" s="2"/>
-      <c r="CM13" s="2"/>
-      <c r="CN13" s="2"/>
-      <c r="CO13" s="2"/>
-      <c r="CP13" s="2"/>
-      <c r="CQ13" s="2"/>
-      <c r="CR13" s="2"/>
-      <c r="CS13" s="2"/>
-      <c r="CT13" s="2"/>
-      <c r="CU13" s="2"/>
-      <c r="CV13" s="2"/>
-      <c r="CW13" s="2"/>
+      <c r="CL13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CM13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="CN13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CO13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="CP13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CQ13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="CR13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CS13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="CT13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CU13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="CV13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="CW13" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="CX13">
         <v>2024</v>
       </c>
@@ -7601,6 +7643,18 @@
       <c r="D15" t="s">
         <v>21</v>
       </c>
+      <c r="AL15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN15" t="s">
+        <v>21</v>
+      </c>
+      <c r="BZ15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="CB15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:104" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="5" t="s">
@@ -7609,76 +7663,182 @@
       <c r="D16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AL16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN16" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="CB16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:80" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AL17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>22</v>
+      </c>
+      <c r="BZ17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="CB17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:80" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AL18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN18" t="s">
+        <v>23</v>
+      </c>
+      <c r="BZ18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="CB18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:80" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AL19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="AN19" t="s">
+        <v>24</v>
+      </c>
+      <c r="BZ19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="CB19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:80" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AL20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN20" t="s">
+        <v>25</v>
+      </c>
+      <c r="BZ20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="CB20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:80" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="AL21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN21" t="s">
+        <v>38</v>
+      </c>
+      <c r="BZ21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="CB21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:80" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
       </c>
+      <c r="AL22" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>26</v>
+      </c>
+      <c r="BZ22" t="s">
+        <v>20</v>
+      </c>
+      <c r="CB22" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="75">
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="BR1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="CN2:CO2"/>
+    <mergeCell ref="CP2:CQ2"/>
+    <mergeCell ref="CR2:CS2"/>
+    <mergeCell ref="CT2:CU2"/>
+    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BR2:BS2"/>
+    <mergeCell ref="BT2:BU2"/>
+    <mergeCell ref="BV2:BW2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CB2:CC2"/>
+    <mergeCell ref="CD2:CE2"/>
+    <mergeCell ref="CF2:CG2"/>
+    <mergeCell ref="CH2:CI2"/>
+    <mergeCell ref="CJ2:CK2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="AZ2:BA2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BH2:BI2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="AP2:AQ2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AF2:AG2"/>
+    <mergeCell ref="AH2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AM2"/>
+    <mergeCell ref="AN2:AO2"/>
     <mergeCell ref="CT1:CW1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
@@ -7695,47 +7855,24 @@
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="CL1:CO1"/>
     <mergeCell ref="CP1:CS1"/>
-    <mergeCell ref="AP2:AQ2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AF2:AG2"/>
-    <mergeCell ref="AH2:AI2"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AM2"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BH2:BI2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="CL2:CM2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BR2:BS2"/>
-    <mergeCell ref="BT2:BU2"/>
-    <mergeCell ref="BV2:BW2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CB2:CC2"/>
-    <mergeCell ref="CD2:CE2"/>
-    <mergeCell ref="CF2:CG2"/>
-    <mergeCell ref="CH2:CI2"/>
-    <mergeCell ref="CJ2:CK2"/>
-    <mergeCell ref="CN2:CO2"/>
-    <mergeCell ref="CP2:CQ2"/>
-    <mergeCell ref="CR2:CS2"/>
-    <mergeCell ref="CT2:CU2"/>
-    <mergeCell ref="CV2:CW2"/>
+    <mergeCell ref="BR1:BU1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AX1:BA1"/>
+    <mergeCell ref="BB1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="BJ1:BM1"/>
+    <mergeCell ref="BN1:BQ1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:CW13">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">

</xml_diff>